<commit_message>
Flintstones - about half of level 3 done, but found a trick that may save frames earlier in the level, will need to redo
</commit_message>
<xml_diff>
--- a/Flintstones/Compare/Flintstones.xlsx
+++ b/Flintstones/Compare/Flintstones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="228">
   <si>
     <t>Notes</t>
   </si>
@@ -725,6 +725,24 @@
   </si>
   <si>
     <t>X = 100</t>
+  </si>
+  <si>
+    <t>Camera = 190</t>
+  </si>
+  <si>
+    <t>X = 42</t>
+  </si>
+  <si>
+    <t>X = 0</t>
+  </si>
+  <si>
+    <t>X = 169</t>
+  </si>
+  <si>
+    <t>X = 1</t>
+  </si>
+  <si>
+    <t>X = 228</t>
   </si>
 </sst>
 </file>
@@ -2368,8 +2386,8 @@
   <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+      <pane ySplit="6" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -3238,111 +3256,171 @@
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="149"/>
-      <c r="B60" s="100"/>
-      <c r="C60" s="101"/>
-      <c r="D60" s="101"/>
+      <c r="B60" s="212" t="s">
+        <v>217</v>
+      </c>
+      <c r="C60" s="101">
+        <v>14457</v>
+      </c>
+      <c r="D60" s="101">
+        <v>14480</v>
+      </c>
       <c r="E60" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="149"/>
-      <c r="B61" s="100"/>
-      <c r="C61" s="101"/>
-      <c r="D61" s="101"/>
+      <c r="B61" s="212" t="s">
+        <v>222</v>
+      </c>
+      <c r="C61" s="101">
+        <v>14718</v>
+      </c>
+      <c r="D61" s="101">
+        <v>14741</v>
+      </c>
       <c r="E61" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="149"/>
-      <c r="B62" s="100"/>
-      <c r="C62" s="101"/>
-      <c r="D62" s="101"/>
+      <c r="B62" s="212" t="s">
+        <v>217</v>
+      </c>
+      <c r="C62" s="101">
+        <v>14834</v>
+      </c>
+      <c r="D62" s="101">
+        <v>14857</v>
+      </c>
       <c r="E62" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="149"/>
-      <c r="B63" s="100"/>
-      <c r="C63" s="101"/>
-      <c r="D63" s="101"/>
+      <c r="B63" s="212" t="s">
+        <v>217</v>
+      </c>
+      <c r="C63" s="101">
+        <v>14941</v>
+      </c>
+      <c r="D63" s="101">
+        <v>14964</v>
+      </c>
       <c r="E63" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="149"/>
-      <c r="B64" s="100"/>
-      <c r="C64" s="101"/>
-      <c r="D64" s="101"/>
+      <c r="B64" s="212" t="s">
+        <v>223</v>
+      </c>
+      <c r="C64" s="101">
+        <v>15104</v>
+      </c>
+      <c r="D64" s="101">
+        <v>15127</v>
+      </c>
       <c r="E64" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="149"/>
-      <c r="B65" s="100"/>
-      <c r="C65" s="101"/>
-      <c r="D65" s="101"/>
+      <c r="B65" s="212" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" s="101">
+        <v>15443</v>
+      </c>
+      <c r="D65" s="101">
+        <v>15466</v>
+      </c>
       <c r="E65" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="149"/>
-      <c r="B66" s="100"/>
-      <c r="C66" s="101"/>
-      <c r="D66" s="101"/>
+      <c r="B66" s="212" t="s">
+        <v>224</v>
+      </c>
+      <c r="C66" s="101">
+        <v>15678</v>
+      </c>
+      <c r="D66" s="101">
+        <v>15700</v>
+      </c>
       <c r="E66" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="149"/>
-      <c r="B67" s="100"/>
-      <c r="C67" s="101"/>
-      <c r="D67" s="101"/>
+      <c r="B67" s="212" t="s">
+        <v>225</v>
+      </c>
+      <c r="C67" s="101">
+        <v>16467</v>
+      </c>
+      <c r="D67" s="101">
+        <v>16490</v>
+      </c>
       <c r="E67" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="149"/>
-      <c r="B68" s="100"/>
-      <c r="C68" s="101"/>
-      <c r="D68" s="101"/>
+      <c r="B68" s="212" t="s">
+        <v>226</v>
+      </c>
+      <c r="C68" s="101">
+        <v>16526</v>
+      </c>
+      <c r="D68" s="101">
+        <v>16549</v>
+      </c>
       <c r="E68" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="149"/>
-      <c r="B69" s="100"/>
-      <c r="C69" s="101"/>
-      <c r="D69" s="101"/>
+      <c r="B69" s="212" t="s">
+        <v>227</v>
+      </c>
+      <c r="C69" s="101">
+        <v>16917</v>
+      </c>
+      <c r="D69" s="101">
+        <v>16943</v>
+      </c>
       <c r="E69" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F69" s="105"/>
     </row>

</xml_diff>

<commit_message>
Flinstones - redid beginning of level 3 with the ice/speed trick, now 58 frames ahead (saved 22 with this new means of motion on ice)
</commit_message>
<xml_diff>
--- a/Flintstones/Compare/Flintstones.xlsx
+++ b/Flintstones/Compare/Flintstones.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="227">
   <si>
     <t>Notes</t>
   </si>
@@ -741,9 +741,6 @@
   <si>
     <t>X = 1</t>
   </si>
-  <si>
-    <t>X = 228</t>
-  </si>
 </sst>
 </file>
 
@@ -753,10 +750,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1668,34 +1672,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1703,208 +1707,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="26" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="26" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="26" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1914,10 +1918,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1938,134 +1942,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2386,7 +2393,7 @@
   <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
@@ -2403,16 +2410,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="154" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="154" t="s">
+      <c r="B1" s="153"/>
+      <c r="C1" s="155" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="156"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65539)</f>
@@ -2490,10 +2497,10 @@
       <c r="B5" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="151" t="s">
+      <c r="C5" s="152" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="151"/>
+      <c r="D5" s="152"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2509,10 +2516,10 @@
       <c r="B6" s="147" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="152" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="152"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2530,7 +2537,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="156" t="s">
+      <c r="A8" s="157" t="s">
         <v>190</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2550,7 +2557,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="149"/>
+      <c r="A9" s="150"/>
       <c r="B9" s="98" t="s">
         <v>185</v>
       </c>
@@ -2560,7 +2567,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="149"/>
+      <c r="A10" s="150"/>
       <c r="B10" s="100"/>
       <c r="C10" s="101"/>
       <c r="D10" s="101"/>
@@ -2571,7 +2578,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="149"/>
+      <c r="A11" s="150"/>
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
       <c r="D11" s="101"/>
@@ -2582,7 +2589,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
+      <c r="A12" s="150"/>
       <c r="B12" s="100"/>
       <c r="C12" s="101"/>
       <c r="D12" s="101"/>
@@ -2593,7 +2600,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="149"/>
+      <c r="A13" s="150"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2604,7 +2611,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="149"/>
+      <c r="A14" s="150"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2615,7 +2622,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="149"/>
+      <c r="A15" s="150"/>
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
@@ -2626,7 +2633,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="149"/>
+      <c r="A16" s="150"/>
       <c r="B16" s="98" t="s">
         <v>188</v>
       </c>
@@ -2669,7 +2676,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="151" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2689,7 +2696,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="149"/>
+      <c r="A20" s="150"/>
       <c r="B20" s="98" t="s">
         <v>185</v>
       </c>
@@ -2702,7 +2709,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="149"/>
+      <c r="A21" s="150"/>
       <c r="B21" s="100"/>
       <c r="C21" s="101"/>
       <c r="D21" s="101"/>
@@ -2713,7 +2720,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="149"/>
+      <c r="A22" s="150"/>
       <c r="B22" s="100"/>
       <c r="C22" s="101"/>
       <c r="D22" s="101"/>
@@ -2724,7 +2731,7 @@
       <c r="F22" s="105"/>
     </row>
     <row r="23" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="149"/>
+      <c r="A23" s="150"/>
       <c r="B23" s="100"/>
       <c r="C23" s="101"/>
       <c r="D23" s="101"/>
@@ -2735,7 +2742,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="149"/>
+      <c r="A24" s="150"/>
       <c r="B24" s="100"/>
       <c r="C24" s="101"/>
       <c r="D24" s="101"/>
@@ -2746,7 +2753,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="149"/>
+      <c r="A25" s="150"/>
       <c r="B25" s="100"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -2757,7 +2764,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="149"/>
+      <c r="A26" s="150"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -2768,7 +2775,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="149"/>
+      <c r="A27" s="150"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -2779,7 +2786,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="149"/>
+      <c r="A28" s="150"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2790,7 +2797,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="149"/>
+      <c r="A29" s="150"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2801,7 +2808,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="149"/>
+      <c r="A30" s="150"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2812,7 +2819,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="149"/>
+      <c r="A31" s="150"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2823,7 +2830,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="149"/>
+      <c r="A32" s="150"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2834,7 +2841,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="149"/>
+      <c r="A33" s="150"/>
       <c r="B33" s="98" t="s">
         <v>188</v>
       </c>
@@ -2873,7 +2880,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="148" t="s">
+      <c r="A36" s="149" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2893,7 +2900,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="149"/>
+      <c r="A37" s="150"/>
       <c r="B37" s="98" t="s">
         <v>185</v>
       </c>
@@ -2910,8 +2917,8 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="149"/>
-      <c r="B38" s="212" t="s">
+      <c r="A38" s="150"/>
+      <c r="B38" s="148" t="s">
         <v>216</v>
       </c>
       <c r="C38" s="101">
@@ -2927,8 +2934,8 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="149"/>
-      <c r="B39" s="212" t="s">
+      <c r="A39" s="150"/>
+      <c r="B39" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C39" s="101">
@@ -2944,8 +2951,8 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="149"/>
-      <c r="B40" s="212" t="s">
+      <c r="A40" s="150"/>
+      <c r="B40" s="148" t="s">
         <v>218</v>
       </c>
       <c r="C40" s="101">
@@ -2961,8 +2968,8 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="149"/>
-      <c r="B41" s="212" t="s">
+      <c r="A41" s="150"/>
+      <c r="B41" s="148" t="s">
         <v>219</v>
       </c>
       <c r="C41" s="101">
@@ -2978,8 +2985,8 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="149"/>
-      <c r="B42" s="212" t="s">
+      <c r="A42" s="150"/>
+      <c r="B42" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C42" s="101">
@@ -2995,8 +3002,8 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="149"/>
-      <c r="B43" s="212" t="s">
+      <c r="A43" s="150"/>
+      <c r="B43" s="148" t="s">
         <v>220</v>
       </c>
       <c r="C43" s="101">
@@ -3012,8 +3019,8 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="149"/>
-      <c r="B44" s="212" t="s">
+      <c r="A44" s="150"/>
+      <c r="B44" s="148" t="s">
         <v>221</v>
       </c>
       <c r="C44" s="101">
@@ -3029,8 +3036,8 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="149"/>
-      <c r="B45" s="212" t="s">
+      <c r="A45" s="150"/>
+      <c r="B45" s="148" t="s">
         <v>169</v>
       </c>
       <c r="C45" s="101">
@@ -3046,8 +3053,8 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="149"/>
-      <c r="B46" s="212" t="s">
+      <c r="A46" s="150"/>
+      <c r="B46" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C46" s="101">
@@ -3063,8 +3070,8 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="149"/>
-      <c r="B47" s="212" t="s">
+      <c r="A47" s="150"/>
+      <c r="B47" s="148" t="s">
         <v>169</v>
       </c>
       <c r="C47" s="101">
@@ -3080,8 +3087,8 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="149"/>
-      <c r="B48" s="212" t="s">
+      <c r="A48" s="150"/>
+      <c r="B48" s="148" t="s">
         <v>216</v>
       </c>
       <c r="C48" s="101">
@@ -3097,8 +3104,8 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="149"/>
-      <c r="B49" s="212" t="s">
+      <c r="A49" s="150"/>
+      <c r="B49" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C49" s="101">
@@ -3114,8 +3121,8 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="149"/>
-      <c r="B50" s="212" t="s">
+      <c r="A50" s="150"/>
+      <c r="B50" s="148" t="s">
         <v>169</v>
       </c>
       <c r="C50" s="101">
@@ -3131,23 +3138,23 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="149"/>
-      <c r="B51" s="212"/>
+      <c r="A51" s="150"/>
+      <c r="B51" s="148"/>
       <c r="C51" s="101"/>
       <c r="D51" s="101"/>
       <c r="E51" s="123"/>
       <c r="F51" s="105"/>
     </row>
     <row r="52" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="149"/>
-      <c r="B52" s="212"/>
+      <c r="A52" s="150"/>
+      <c r="B52" s="148"/>
       <c r="C52" s="101"/>
       <c r="D52" s="101"/>
       <c r="E52" s="123"/>
       <c r="F52" s="105"/>
     </row>
     <row r="53" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="149"/>
+      <c r="A53" s="150"/>
       <c r="B53" s="100"/>
       <c r="C53" s="101"/>
       <c r="D53" s="101"/>
@@ -3158,7 +3165,7 @@
       <c r="F53" s="105"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="149"/>
+      <c r="A54" s="150"/>
       <c r="B54" s="98" t="s">
         <v>188</v>
       </c>
@@ -3201,7 +3208,7 @@
     </row>
     <row r="56" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="150" t="s">
+      <c r="A57" s="151" t="s">
         <v>171</v>
       </c>
       <c r="B57" s="109" t="s">
@@ -3221,7 +3228,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="149"/>
+      <c r="A58" s="150"/>
       <c r="B58" s="98" t="s">
         <v>185</v>
       </c>
@@ -3238,8 +3245,8 @@
       <c r="F58" s="104"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="149"/>
-      <c r="B59" s="212" t="s">
+      <c r="A59" s="150"/>
+      <c r="B59" s="148" t="s">
         <v>216</v>
       </c>
       <c r="C59" s="101">
@@ -3255,177 +3262,171 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="149"/>
-      <c r="B60" s="212" t="s">
+      <c r="A60" s="150"/>
+      <c r="B60" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C60" s="101">
-        <v>14457</v>
+        <v>14450</v>
       </c>
       <c r="D60" s="101">
         <v>14480</v>
       </c>
       <c r="E60" s="123">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="149"/>
-      <c r="B61" s="212" t="s">
+      <c r="A61" s="150"/>
+      <c r="B61" s="148" t="s">
         <v>222</v>
       </c>
-      <c r="C61" s="101">
-        <v>14718</v>
-      </c>
+      <c r="C61" s="101"/>
       <c r="D61" s="101">
         <v>14741</v>
       </c>
       <c r="E61" s="123">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="149"/>
-      <c r="B62" s="212" t="s">
+      <c r="A62" s="150"/>
+      <c r="B62" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C62" s="101">
-        <v>14834</v>
+        <v>14820</v>
       </c>
       <c r="D62" s="101">
         <v>14857</v>
       </c>
       <c r="E62" s="123">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="149"/>
-      <c r="B63" s="212" t="s">
+      <c r="A63" s="150"/>
+      <c r="B63" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C63" s="101">
-        <v>14941</v>
+        <v>14925</v>
       </c>
       <c r="D63" s="101">
         <v>14964</v>
       </c>
       <c r="E63" s="123">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="149"/>
-      <c r="B64" s="212" t="s">
+      <c r="A64" s="150"/>
+      <c r="B64" s="148" t="s">
         <v>223</v>
       </c>
-      <c r="C64" s="101">
-        <v>15104</v>
-      </c>
+      <c r="C64" s="101"/>
       <c r="D64" s="101">
         <v>15127</v>
       </c>
       <c r="E64" s="123">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="149"/>
-      <c r="B65" s="212" t="s">
+      <c r="A65" s="150"/>
+      <c r="B65" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C65" s="101">
-        <v>15443</v>
+        <v>15418</v>
       </c>
       <c r="D65" s="101">
         <v>15466</v>
       </c>
       <c r="E65" s="123">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="149"/>
-      <c r="B66" s="212" t="s">
+      <c r="A66" s="150"/>
+      <c r="B66" s="148" t="s">
         <v>224</v>
       </c>
       <c r="C66" s="101">
-        <v>15678</v>
+        <v>15652</v>
       </c>
       <c r="D66" s="101">
         <v>15700</v>
       </c>
       <c r="E66" s="123">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="149"/>
-      <c r="B67" s="212" t="s">
+      <c r="A67" s="150"/>
+      <c r="B67" s="148" t="s">
         <v>225</v>
       </c>
       <c r="C67" s="101">
-        <v>16467</v>
+        <v>16439</v>
       </c>
       <c r="D67" s="101">
         <v>16490</v>
       </c>
       <c r="E67" s="123">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="149"/>
-      <c r="B68" s="212" t="s">
+      <c r="A68" s="150"/>
+      <c r="B68" s="148" t="s">
         <v>226</v>
       </c>
-      <c r="C68" s="101">
-        <v>16526</v>
-      </c>
+      <c r="C68" s="101"/>
       <c r="D68" s="101">
         <v>16549</v>
       </c>
       <c r="E68" s="123">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="149"/>
-      <c r="B69" s="212" t="s">
-        <v>227</v>
+      <c r="A69" s="150"/>
+      <c r="B69" s="213" t="s">
+        <v>217</v>
       </c>
       <c r="C69" s="101">
-        <v>16917</v>
+        <v>16587</v>
       </c>
       <c r="D69" s="101">
-        <v>16943</v>
+        <v>16645</v>
       </c>
       <c r="E69" s="123">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="149"/>
+      <c r="A70" s="150"/>
       <c r="B70" s="100"/>
       <c r="C70" s="101"/>
       <c r="D70" s="101"/>
@@ -3436,7 +3437,7 @@
       <c r="F70" s="105"/>
     </row>
     <row r="71" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="149"/>
+      <c r="A71" s="150"/>
       <c r="B71" s="98" t="s">
         <v>188</v>
       </c>
@@ -3475,7 +3476,7 @@
     </row>
     <row r="73" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="148" t="s">
+      <c r="A74" s="149" t="s">
         <v>172</v>
       </c>
       <c r="B74" s="113" t="s">
@@ -3495,7 +3496,7 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="149"/>
+      <c r="A75" s="150"/>
       <c r="B75" s="98" t="s">
         <v>185</v>
       </c>
@@ -3508,7 +3509,7 @@
       <c r="F75" s="104"/>
     </row>
     <row r="76" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="149"/>
+      <c r="A76" s="150"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3519,7 +3520,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="149"/>
+      <c r="A77" s="150"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3530,7 +3531,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="149"/>
+      <c r="A78" s="150"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3541,7 +3542,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="149"/>
+      <c r="A79" s="150"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3552,7 +3553,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="149"/>
+      <c r="A80" s="150"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3563,7 +3564,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="149"/>
+      <c r="A81" s="150"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3574,7 +3575,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="149"/>
+      <c r="A82" s="150"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3585,7 +3586,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="149"/>
+      <c r="A83" s="150"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3596,7 +3597,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="149"/>
+      <c r="A84" s="150"/>
       <c r="B84" s="100"/>
       <c r="C84" s="101"/>
       <c r="D84" s="101"/>
@@ -3607,7 +3608,7 @@
       <c r="F84" s="105"/>
     </row>
     <row r="85" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="149"/>
+      <c r="A85" s="150"/>
       <c r="B85" s="100"/>
       <c r="C85" s="101"/>
       <c r="D85" s="101"/>
@@ -3618,7 +3619,7 @@
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="149"/>
+      <c r="A86" s="150"/>
       <c r="B86" s="100"/>
       <c r="C86" s="101"/>
       <c r="D86" s="101"/>
@@ -3629,7 +3630,7 @@
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="149"/>
+      <c r="A87" s="150"/>
       <c r="B87" s="100"/>
       <c r="C87" s="101"/>
       <c r="D87" s="101"/>
@@ -3640,7 +3641,7 @@
       <c r="F87" s="105"/>
     </row>
     <row r="88" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="149"/>
+      <c r="A88" s="150"/>
       <c r="B88" s="98" t="s">
         <v>188</v>
       </c>
@@ -3679,7 +3680,7 @@
     </row>
     <row r="90" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="150" t="s">
+      <c r="A91" s="151" t="s">
         <v>173</v>
       </c>
       <c r="B91" s="109" t="s">
@@ -3699,7 +3700,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="149"/>
+      <c r="A92" s="150"/>
       <c r="B92" s="98" t="s">
         <v>185</v>
       </c>
@@ -3712,7 +3713,7 @@
       <c r="F92" s="104"/>
     </row>
     <row r="93" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="149"/>
+      <c r="A93" s="150"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3723,7 +3724,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="149"/>
+      <c r="A94" s="150"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3734,7 +3735,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="149"/>
+      <c r="A95" s="150"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3745,7 +3746,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="149"/>
+      <c r="A96" s="150"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3756,7 +3757,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="149"/>
+      <c r="A97" s="150"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3767,7 +3768,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="149"/>
+      <c r="A98" s="150"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3778,7 +3779,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="149"/>
+      <c r="A99" s="150"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3789,7 +3790,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="149"/>
+      <c r="A100" s="150"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3800,7 +3801,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="149"/>
+      <c r="A101" s="150"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -3811,7 +3812,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="149"/>
+      <c r="A102" s="150"/>
       <c r="B102" s="100"/>
       <c r="C102" s="101"/>
       <c r="D102" s="101"/>
@@ -3822,7 +3823,7 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="149"/>
+      <c r="A103" s="150"/>
       <c r="B103" s="100"/>
       <c r="C103" s="101"/>
       <c r="D103" s="101"/>
@@ -3833,7 +3834,7 @@
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="149"/>
+      <c r="A104" s="150"/>
       <c r="B104" s="100"/>
       <c r="C104" s="101"/>
       <c r="D104" s="101"/>
@@ -3844,7 +3845,7 @@
       <c r="F104" s="105"/>
     </row>
     <row r="105" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="149"/>
+      <c r="A105" s="150"/>
       <c r="B105" s="98" t="s">
         <v>188</v>
       </c>
@@ -3882,7 +3883,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="148" t="s">
+      <c r="A108" s="149" t="s">
         <v>174</v>
       </c>
       <c r="B108" s="113" t="s">
@@ -3902,7 +3903,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="149"/>
+      <c r="A109" s="150"/>
       <c r="B109" s="98" t="s">
         <v>185</v>
       </c>
@@ -3915,7 +3916,7 @@
       <c r="F109" s="104"/>
     </row>
     <row r="110" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="149"/>
+      <c r="A110" s="150"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3926,7 +3927,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="149"/>
+      <c r="A111" s="150"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3937,7 +3938,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="149"/>
+      <c r="A112" s="150"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3948,7 +3949,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="149"/>
+      <c r="A113" s="150"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3959,7 +3960,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="149"/>
+      <c r="A114" s="150"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3970,7 +3971,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="149"/>
+      <c r="A115" s="150"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -3981,7 +3982,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="149"/>
+      <c r="A116" s="150"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -3992,7 +3993,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="149"/>
+      <c r="A117" s="150"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -4003,7 +4004,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="149"/>
+      <c r="A118" s="150"/>
       <c r="B118" s="100"/>
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
@@ -4014,7 +4015,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="149"/>
+      <c r="A119" s="150"/>
       <c r="B119" s="100"/>
       <c r="C119" s="101"/>
       <c r="D119" s="101"/>
@@ -4025,7 +4026,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="149"/>
+      <c r="A120" s="150"/>
       <c r="B120" s="100"/>
       <c r="C120" s="101"/>
       <c r="D120" s="101"/>
@@ -4036,7 +4037,7 @@
       <c r="F120" s="105"/>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="149"/>
+      <c r="A121" s="150"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -4047,7 +4048,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="149"/>
+      <c r="A122" s="150"/>
       <c r="B122" s="98" t="s">
         <v>188</v>
       </c>
@@ -4085,7 +4086,7 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="150" t="s">
+      <c r="A125" s="151" t="s">
         <v>175</v>
       </c>
       <c r="B125" s="109" t="s">
@@ -4105,7 +4106,7 @@
       </c>
     </row>
     <row r="126" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="149"/>
+      <c r="A126" s="150"/>
       <c r="B126" s="98" t="s">
         <v>185</v>
       </c>
@@ -4118,7 +4119,7 @@
       <c r="F126" s="104"/>
     </row>
     <row r="127" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="149"/>
+      <c r="A127" s="150"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4129,7 +4130,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="149"/>
+      <c r="A128" s="150"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4140,7 +4141,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="149"/>
+      <c r="A129" s="150"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4151,7 +4152,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="149"/>
+      <c r="A130" s="150"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4162,7 +4163,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="149"/>
+      <c r="A131" s="150"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4173,7 +4174,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="149"/>
+      <c r="A132" s="150"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4184,7 +4185,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="149"/>
+      <c r="A133" s="150"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4195,7 +4196,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="149"/>
+      <c r="A134" s="150"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4206,7 +4207,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="149"/>
+      <c r="A135" s="150"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4217,7 +4218,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="149"/>
+      <c r="A136" s="150"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
       <c r="D136" s="101"/>
@@ -4228,7 +4229,7 @@
       <c r="F136" s="105"/>
     </row>
     <row r="137" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="149"/>
+      <c r="A137" s="150"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4239,7 +4240,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="149"/>
+      <c r="A138" s="150"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4250,7 +4251,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="149"/>
+      <c r="A139" s="150"/>
       <c r="B139" s="98" t="s">
         <v>188</v>
       </c>
@@ -4288,7 +4289,7 @@
       </c>
     </row>
     <row r="142" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A142" s="148" t="s">
+      <c r="A142" s="149" t="s">
         <v>176</v>
       </c>
       <c r="B142" s="113" t="s">
@@ -4308,7 +4309,7 @@
       </c>
     </row>
     <row r="143" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="149"/>
+      <c r="A143" s="150"/>
       <c r="B143" s="98" t="s">
         <v>185</v>
       </c>
@@ -4321,7 +4322,7 @@
       <c r="F143" s="104"/>
     </row>
     <row r="144" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="149"/>
+      <c r="A144" s="150"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4332,7 +4333,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A145" s="149"/>
+      <c r="A145" s="150"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4343,7 +4344,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A146" s="149"/>
+      <c r="A146" s="150"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4354,7 +4355,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A147" s="149"/>
+      <c r="A147" s="150"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4365,7 +4366,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A148" s="149"/>
+      <c r="A148" s="150"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4376,7 +4377,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A149" s="149"/>
+      <c r="A149" s="150"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
@@ -4387,7 +4388,7 @@
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A150" s="149"/>
+      <c r="A150" s="150"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -4398,7 +4399,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A151" s="149"/>
+      <c r="A151" s="150"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -4409,7 +4410,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A152" s="149"/>
+      <c r="A152" s="150"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
@@ -4420,7 +4421,7 @@
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A153" s="149"/>
+      <c r="A153" s="150"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
@@ -4431,7 +4432,7 @@
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A154" s="149"/>
+      <c r="A154" s="150"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -4442,7 +4443,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A155" s="149"/>
+      <c r="A155" s="150"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
@@ -4453,7 +4454,7 @@
       <c r="F155" s="105"/>
     </row>
     <row r="156" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="149"/>
+      <c r="A156" s="150"/>
       <c r="B156" s="98" t="s">
         <v>188</v>
       </c>
@@ -4492,11 +4493,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A142:A156"/>
-    <mergeCell ref="A108:A122"/>
-    <mergeCell ref="A74:A88"/>
-    <mergeCell ref="A125:A139"/>
-    <mergeCell ref="A91:A105"/>
     <mergeCell ref="A36:A54"/>
     <mergeCell ref="A57:A71"/>
     <mergeCell ref="C5:D5"/>
@@ -4505,6 +4501,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A142:A156"/>
+    <mergeCell ref="A108:A122"/>
+    <mergeCell ref="A74:A88"/>
+    <mergeCell ref="A125:A139"/>
+    <mergeCell ref="A91:A105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4536,13 +4537,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4572,18 +4573,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="159"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4735,9 +4736,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="162"/>
-      <c r="D21" s="163"/>
-      <c r="E21" s="163"/>
+      <c r="C21" s="160"/>
+      <c r="D21" s="161"/>
+      <c r="E21" s="161"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4888,9 +4889,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="160"/>
-      <c r="D38" s="161"/>
-      <c r="E38" s="161"/>
+      <c r="C38" s="158"/>
+      <c r="D38" s="159"/>
+      <c r="E38" s="159"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -5041,9 +5042,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="160"/>
-      <c r="D55" s="161"/>
-      <c r="E55" s="161"/>
+      <c r="C55" s="158"/>
+      <c r="D55" s="159"/>
+      <c r="E55" s="159"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -5194,9 +5195,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="160"/>
-      <c r="D72" s="161"/>
-      <c r="E72" s="161"/>
+      <c r="C72" s="158"/>
+      <c r="D72" s="159"/>
+      <c r="E72" s="159"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5347,9 +5348,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="160"/>
-      <c r="D89" s="161"/>
-      <c r="E89" s="161"/>
+      <c r="C89" s="158"/>
+      <c r="D89" s="159"/>
+      <c r="E89" s="159"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5500,9 +5501,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="160"/>
-      <c r="D106" s="161"/>
-      <c r="E106" s="161"/>
+      <c r="C106" s="158"/>
+      <c r="D106" s="159"/>
+      <c r="E106" s="159"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5653,9 +5654,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="160"/>
-      <c r="D123" s="161"/>
-      <c r="E123" s="161"/>
+      <c r="C123" s="158"/>
+      <c r="D123" s="159"/>
+      <c r="E123" s="159"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5806,9 +5807,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="160"/>
-      <c r="D140" s="161"/>
-      <c r="E140" s="161"/>
+      <c r="C140" s="158"/>
+      <c r="D140" s="159"/>
+      <c r="E140" s="159"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -5959,9 +5960,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="160"/>
-      <c r="D157" s="161"/>
-      <c r="E157" s="161"/>
+      <c r="C157" s="158"/>
+      <c r="D157" s="159"/>
+      <c r="E157" s="159"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -6112,9 +6113,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="160"/>
-      <c r="D174" s="161"/>
-      <c r="E174" s="161"/>
+      <c r="C174" s="158"/>
+      <c r="D174" s="159"/>
+      <c r="E174" s="159"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6265,9 +6266,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="160"/>
-      <c r="D191" s="161"/>
-      <c r="E191" s="161"/>
+      <c r="C191" s="158"/>
+      <c r="D191" s="159"/>
+      <c r="E191" s="159"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6418,9 +6419,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="160"/>
-      <c r="D208" s="161"/>
-      <c r="E208" s="161"/>
+      <c r="C208" s="158"/>
+      <c r="D208" s="159"/>
+      <c r="E208" s="159"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6571,9 +6572,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="160"/>
-      <c r="D225" s="161"/>
-      <c r="E225" s="161"/>
+      <c r="C225" s="158"/>
+      <c r="D225" s="159"/>
+      <c r="E225" s="159"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6724,9 +6725,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="160"/>
-      <c r="D242" s="161"/>
-      <c r="E242" s="161"/>
+      <c r="C242" s="158"/>
+      <c r="D242" s="159"/>
+      <c r="E242" s="159"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6877,9 +6878,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="160"/>
-      <c r="D259" s="161"/>
-      <c r="E259" s="161"/>
+      <c r="C259" s="158"/>
+      <c r="D259" s="159"/>
+      <c r="E259" s="159"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -7030,18 +7031,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="164"/>
-      <c r="D276" s="165"/>
-      <c r="E276" s="165"/>
+      <c r="C276" s="174"/>
+      <c r="D276" s="175"/>
+      <c r="E276" s="175"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="160"/>
-      <c r="D277" s="161"/>
-      <c r="E277" s="161"/>
+      <c r="C277" s="158"/>
+      <c r="D277" s="159"/>
+      <c r="E277" s="159"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -7192,9 +7193,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="162"/>
-      <c r="D294" s="163"/>
-      <c r="E294" s="163"/>
+      <c r="C294" s="160"/>
+      <c r="D294" s="161"/>
+      <c r="E294" s="161"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7345,9 +7346,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="160"/>
-      <c r="D311" s="161"/>
-      <c r="E311" s="161"/>
+      <c r="C311" s="158"/>
+      <c r="D311" s="159"/>
+      <c r="E311" s="159"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7498,9 +7499,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="160"/>
-      <c r="D328" s="161"/>
-      <c r="E328" s="161"/>
+      <c r="C328" s="158"/>
+      <c r="D328" s="159"/>
+      <c r="E328" s="159"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7651,9 +7652,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="160"/>
-      <c r="D345" s="161"/>
-      <c r="E345" s="161"/>
+      <c r="C345" s="158"/>
+      <c r="D345" s="159"/>
+      <c r="E345" s="159"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7804,9 +7805,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="160"/>
-      <c r="D362" s="161"/>
-      <c r="E362" s="161"/>
+      <c r="C362" s="158"/>
+      <c r="D362" s="159"/>
+      <c r="E362" s="159"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7957,9 +7958,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="160"/>
-      <c r="D379" s="161"/>
-      <c r="E379" s="161"/>
+      <c r="C379" s="158"/>
+      <c r="D379" s="159"/>
+      <c r="E379" s="159"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -8110,9 +8111,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="160"/>
-      <c r="D396" s="161"/>
-      <c r="E396" s="161"/>
+      <c r="C396" s="158"/>
+      <c r="D396" s="159"/>
+      <c r="E396" s="159"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8263,9 +8264,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="160"/>
-      <c r="D413" s="161"/>
-      <c r="E413" s="161"/>
+      <c r="C413" s="158"/>
+      <c r="D413" s="159"/>
+      <c r="E413" s="159"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8416,9 +8417,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="160"/>
-      <c r="D430" s="161"/>
-      <c r="E430" s="161"/>
+      <c r="C430" s="158"/>
+      <c r="D430" s="159"/>
+      <c r="E430" s="159"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8569,9 +8570,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="160"/>
-      <c r="D447" s="161"/>
-      <c r="E447" s="161"/>
+      <c r="C447" s="158"/>
+      <c r="D447" s="159"/>
+      <c r="E447" s="159"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8722,9 +8723,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="160"/>
-      <c r="D464" s="161"/>
-      <c r="E464" s="161"/>
+      <c r="C464" s="158"/>
+      <c r="D464" s="159"/>
+      <c r="E464" s="159"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8875,9 +8876,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="160"/>
-      <c r="D481" s="161"/>
-      <c r="E481" s="161"/>
+      <c r="C481" s="158"/>
+      <c r="D481" s="159"/>
+      <c r="E481" s="159"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -9028,9 +9029,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="160"/>
-      <c r="D498" s="161"/>
-      <c r="E498" s="161"/>
+      <c r="C498" s="158"/>
+      <c r="D498" s="159"/>
+      <c r="E498" s="159"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -9181,9 +9182,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="160"/>
-      <c r="D515" s="161"/>
-      <c r="E515" s="161"/>
+      <c r="C515" s="158"/>
+      <c r="D515" s="159"/>
+      <c r="E515" s="159"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9334,9 +9335,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="160"/>
-      <c r="D532" s="161"/>
-      <c r="E532" s="161"/>
+      <c r="C532" s="158"/>
+      <c r="D532" s="159"/>
+      <c r="E532" s="159"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9487,18 +9488,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="166"/>
-      <c r="D549" s="167"/>
-      <c r="E549" s="167"/>
+      <c r="C549" s="172"/>
+      <c r="D549" s="173"/>
+      <c r="E549" s="173"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="160"/>
-      <c r="D550" s="161"/>
-      <c r="E550" s="161"/>
+      <c r="C550" s="158"/>
+      <c r="D550" s="159"/>
+      <c r="E550" s="159"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9649,9 +9650,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="162"/>
-      <c r="D567" s="163"/>
-      <c r="E567" s="163"/>
+      <c r="C567" s="160"/>
+      <c r="D567" s="161"/>
+      <c r="E567" s="161"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9802,9 +9803,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="160"/>
-      <c r="D584" s="161"/>
-      <c r="E584" s="161"/>
+      <c r="C584" s="158"/>
+      <c r="D584" s="159"/>
+      <c r="E584" s="159"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9955,9 +9956,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="160"/>
-      <c r="D601" s="161"/>
-      <c r="E601" s="161"/>
+      <c r="C601" s="158"/>
+      <c r="D601" s="159"/>
+      <c r="E601" s="159"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -10108,9 +10109,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="160"/>
-      <c r="D618" s="161"/>
-      <c r="E618" s="161"/>
+      <c r="C618" s="158"/>
+      <c r="D618" s="159"/>
+      <c r="E618" s="159"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10261,9 +10262,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="160"/>
-      <c r="D635" s="161"/>
-      <c r="E635" s="161"/>
+      <c r="C635" s="158"/>
+      <c r="D635" s="159"/>
+      <c r="E635" s="159"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10414,9 +10415,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="160"/>
-      <c r="D652" s="161"/>
-      <c r="E652" s="161"/>
+      <c r="C652" s="158"/>
+      <c r="D652" s="159"/>
+      <c r="E652" s="159"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10567,9 +10568,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="160"/>
-      <c r="D669" s="161"/>
-      <c r="E669" s="161"/>
+      <c r="C669" s="158"/>
+      <c r="D669" s="159"/>
+      <c r="E669" s="159"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10720,9 +10721,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="160"/>
-      <c r="D686" s="161"/>
-      <c r="E686" s="161"/>
+      <c r="C686" s="158"/>
+      <c r="D686" s="159"/>
+      <c r="E686" s="159"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10873,9 +10874,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="160"/>
-      <c r="D703" s="161"/>
-      <c r="E703" s="161"/>
+      <c r="C703" s="158"/>
+      <c r="D703" s="159"/>
+      <c r="E703" s="159"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -11026,9 +11027,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="160"/>
-      <c r="D720" s="161"/>
-      <c r="E720" s="161"/>
+      <c r="C720" s="158"/>
+      <c r="D720" s="159"/>
+      <c r="E720" s="159"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -11179,9 +11180,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="160"/>
-      <c r="D737" s="161"/>
-      <c r="E737" s="161"/>
+      <c r="C737" s="158"/>
+      <c r="D737" s="159"/>
+      <c r="E737" s="159"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11332,9 +11333,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="160"/>
-      <c r="D754" s="161"/>
-      <c r="E754" s="161"/>
+      <c r="C754" s="158"/>
+      <c r="D754" s="159"/>
+      <c r="E754" s="159"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11485,9 +11486,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="160"/>
-      <c r="D771" s="161"/>
-      <c r="E771" s="161"/>
+      <c r="C771" s="158"/>
+      <c r="D771" s="159"/>
+      <c r="E771" s="159"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11638,9 +11639,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="160"/>
-      <c r="D788" s="161"/>
-      <c r="E788" s="161"/>
+      <c r="C788" s="158"/>
+      <c r="D788" s="159"/>
+      <c r="E788" s="159"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11791,9 +11792,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="160"/>
-      <c r="D805" s="161"/>
-      <c r="E805" s="161"/>
+      <c r="C805" s="158"/>
+      <c r="D805" s="159"/>
+      <c r="E805" s="159"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11944,18 +11945,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="168"/>
-      <c r="D822" s="169"/>
-      <c r="E822" s="169"/>
+      <c r="C822" s="170"/>
+      <c r="D822" s="171"/>
+      <c r="E822" s="171"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="160"/>
-      <c r="D823" s="161"/>
-      <c r="E823" s="161"/>
+      <c r="C823" s="158"/>
+      <c r="D823" s="159"/>
+      <c r="E823" s="159"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -12106,9 +12107,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="162"/>
-      <c r="D840" s="163"/>
-      <c r="E840" s="163"/>
+      <c r="C840" s="160"/>
+      <c r="D840" s="161"/>
+      <c r="E840" s="161"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12259,9 +12260,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="160"/>
-      <c r="D857" s="161"/>
-      <c r="E857" s="161"/>
+      <c r="C857" s="158"/>
+      <c r="D857" s="159"/>
+      <c r="E857" s="159"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12412,9 +12413,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="160"/>
-      <c r="D874" s="161"/>
-      <c r="E874" s="161"/>
+      <c r="C874" s="158"/>
+      <c r="D874" s="159"/>
+      <c r="E874" s="159"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12565,9 +12566,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="160"/>
-      <c r="D891" s="161"/>
-      <c r="E891" s="161"/>
+      <c r="C891" s="158"/>
+      <c r="D891" s="159"/>
+      <c r="E891" s="159"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12718,9 +12719,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="160"/>
-      <c r="D908" s="161"/>
-      <c r="E908" s="161"/>
+      <c r="C908" s="158"/>
+      <c r="D908" s="159"/>
+      <c r="E908" s="159"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12871,9 +12872,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="160"/>
-      <c r="D925" s="161"/>
-      <c r="E925" s="161"/>
+      <c r="C925" s="158"/>
+      <c r="D925" s="159"/>
+      <c r="E925" s="159"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -13024,9 +13025,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="160"/>
-      <c r="D942" s="161"/>
-      <c r="E942" s="161"/>
+      <c r="C942" s="158"/>
+      <c r="D942" s="159"/>
+      <c r="E942" s="159"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -13177,9 +13178,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="160"/>
-      <c r="D959" s="161"/>
-      <c r="E959" s="161"/>
+      <c r="C959" s="158"/>
+      <c r="D959" s="159"/>
+      <c r="E959" s="159"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13330,9 +13331,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="160"/>
-      <c r="D976" s="161"/>
-      <c r="E976" s="161"/>
+      <c r="C976" s="158"/>
+      <c r="D976" s="159"/>
+      <c r="E976" s="159"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13483,9 +13484,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="160"/>
-      <c r="D993" s="161"/>
-      <c r="E993" s="161"/>
+      <c r="C993" s="158"/>
+      <c r="D993" s="159"/>
+      <c r="E993" s="159"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13636,9 +13637,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="160"/>
-      <c r="D1010" s="161"/>
-      <c r="E1010" s="161"/>
+      <c r="C1010" s="158"/>
+      <c r="D1010" s="159"/>
+      <c r="E1010" s="159"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13789,9 +13790,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="160"/>
-      <c r="D1027" s="161"/>
-      <c r="E1027" s="161"/>
+      <c r="C1027" s="158"/>
+      <c r="D1027" s="159"/>
+      <c r="E1027" s="159"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13942,9 +13943,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="160"/>
-      <c r="D1044" s="161"/>
-      <c r="E1044" s="161"/>
+      <c r="C1044" s="158"/>
+      <c r="D1044" s="159"/>
+      <c r="E1044" s="159"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -14095,9 +14096,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="160"/>
-      <c r="D1061" s="161"/>
-      <c r="E1061" s="161"/>
+      <c r="C1061" s="158"/>
+      <c r="D1061" s="159"/>
+      <c r="E1061" s="159"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14248,9 +14249,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="160"/>
-      <c r="D1078" s="161"/>
-      <c r="E1078" s="161"/>
+      <c r="C1078" s="158"/>
+      <c r="D1078" s="159"/>
+      <c r="E1078" s="159"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14401,18 +14402,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="170"/>
-      <c r="D1095" s="171"/>
-      <c r="E1095" s="171"/>
+      <c r="C1095" s="168"/>
+      <c r="D1095" s="169"/>
+      <c r="E1095" s="169"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="160"/>
-      <c r="D1096" s="161"/>
-      <c r="E1096" s="161"/>
+      <c r="C1096" s="158"/>
+      <c r="D1096" s="159"/>
+      <c r="E1096" s="159"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14563,9 +14564,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="162"/>
-      <c r="D1113" s="163"/>
-      <c r="E1113" s="163"/>
+      <c r="C1113" s="160"/>
+      <c r="D1113" s="161"/>
+      <c r="E1113" s="161"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14716,9 +14717,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="160"/>
-      <c r="D1130" s="161"/>
-      <c r="E1130" s="161"/>
+      <c r="C1130" s="158"/>
+      <c r="D1130" s="159"/>
+      <c r="E1130" s="159"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14869,9 +14870,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="160"/>
-      <c r="D1147" s="161"/>
-      <c r="E1147" s="161"/>
+      <c r="C1147" s="158"/>
+      <c r="D1147" s="159"/>
+      <c r="E1147" s="159"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -15022,9 +15023,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="160"/>
-      <c r="D1164" s="161"/>
-      <c r="E1164" s="161"/>
+      <c r="C1164" s="158"/>
+      <c r="D1164" s="159"/>
+      <c r="E1164" s="159"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -15175,9 +15176,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="160"/>
-      <c r="D1181" s="161"/>
-      <c r="E1181" s="161"/>
+      <c r="C1181" s="158"/>
+      <c r="D1181" s="159"/>
+      <c r="E1181" s="159"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15328,9 +15329,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="160"/>
-      <c r="D1198" s="161"/>
-      <c r="E1198" s="161"/>
+      <c r="C1198" s="158"/>
+      <c r="D1198" s="159"/>
+      <c r="E1198" s="159"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15481,9 +15482,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="160"/>
-      <c r="D1215" s="161"/>
-      <c r="E1215" s="161"/>
+      <c r="C1215" s="158"/>
+      <c r="D1215" s="159"/>
+      <c r="E1215" s="159"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15634,9 +15635,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="160"/>
-      <c r="D1232" s="161"/>
-      <c r="E1232" s="161"/>
+      <c r="C1232" s="158"/>
+      <c r="D1232" s="159"/>
+      <c r="E1232" s="159"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15787,9 +15788,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="160"/>
-      <c r="D1249" s="161"/>
-      <c r="E1249" s="161"/>
+      <c r="C1249" s="158"/>
+      <c r="D1249" s="159"/>
+      <c r="E1249" s="159"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15940,9 +15941,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="160"/>
-      <c r="D1266" s="161"/>
-      <c r="E1266" s="161"/>
+      <c r="C1266" s="158"/>
+      <c r="D1266" s="159"/>
+      <c r="E1266" s="159"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -16093,9 +16094,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="160"/>
-      <c r="D1283" s="161"/>
-      <c r="E1283" s="161"/>
+      <c r="C1283" s="158"/>
+      <c r="D1283" s="159"/>
+      <c r="E1283" s="159"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16246,9 +16247,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="160"/>
-      <c r="D1300" s="161"/>
-      <c r="E1300" s="161"/>
+      <c r="C1300" s="158"/>
+      <c r="D1300" s="159"/>
+      <c r="E1300" s="159"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16399,9 +16400,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="160"/>
-      <c r="D1317" s="161"/>
-      <c r="E1317" s="161"/>
+      <c r="C1317" s="158"/>
+      <c r="D1317" s="159"/>
+      <c r="E1317" s="159"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16552,9 +16553,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="160"/>
-      <c r="D1334" s="161"/>
-      <c r="E1334" s="161"/>
+      <c r="C1334" s="158"/>
+      <c r="D1334" s="159"/>
+      <c r="E1334" s="159"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16705,9 +16706,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="160"/>
-      <c r="D1351" s="161"/>
-      <c r="E1351" s="161"/>
+      <c r="C1351" s="158"/>
+      <c r="D1351" s="159"/>
+      <c r="E1351" s="159"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16858,18 +16859,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="172"/>
-      <c r="D1368" s="173"/>
-      <c r="E1368" s="173"/>
+      <c r="C1368" s="166"/>
+      <c r="D1368" s="167"/>
+      <c r="E1368" s="167"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="160"/>
-      <c r="D1369" s="161"/>
-      <c r="E1369" s="161"/>
+      <c r="C1369" s="158"/>
+      <c r="D1369" s="159"/>
+      <c r="E1369" s="159"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -17020,9 +17021,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="162"/>
-      <c r="D1386" s="163"/>
-      <c r="E1386" s="163"/>
+      <c r="C1386" s="160"/>
+      <c r="D1386" s="161"/>
+      <c r="E1386" s="161"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -17173,9 +17174,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="160"/>
-      <c r="D1403" s="161"/>
-      <c r="E1403" s="161"/>
+      <c r="C1403" s="158"/>
+      <c r="D1403" s="159"/>
+      <c r="E1403" s="159"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17326,9 +17327,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="160"/>
-      <c r="D1420" s="161"/>
-      <c r="E1420" s="161"/>
+      <c r="C1420" s="158"/>
+      <c r="D1420" s="159"/>
+      <c r="E1420" s="159"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17479,9 +17480,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="160"/>
-      <c r="D1437" s="161"/>
-      <c r="E1437" s="161"/>
+      <c r="C1437" s="158"/>
+      <c r="D1437" s="159"/>
+      <c r="E1437" s="159"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17632,9 +17633,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="160"/>
-      <c r="D1454" s="161"/>
-      <c r="E1454" s="161"/>
+      <c r="C1454" s="158"/>
+      <c r="D1454" s="159"/>
+      <c r="E1454" s="159"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17785,9 +17786,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="160"/>
-      <c r="D1471" s="161"/>
-      <c r="E1471" s="161"/>
+      <c r="C1471" s="158"/>
+      <c r="D1471" s="159"/>
+      <c r="E1471" s="159"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17938,9 +17939,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="160"/>
-      <c r="D1488" s="161"/>
-      <c r="E1488" s="161"/>
+      <c r="C1488" s="158"/>
+      <c r="D1488" s="159"/>
+      <c r="E1488" s="159"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -18091,9 +18092,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="160"/>
-      <c r="D1505" s="161"/>
-      <c r="E1505" s="161"/>
+      <c r="C1505" s="158"/>
+      <c r="D1505" s="159"/>
+      <c r="E1505" s="159"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18244,9 +18245,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="160"/>
-      <c r="D1522" s="161"/>
-      <c r="E1522" s="161"/>
+      <c r="C1522" s="158"/>
+      <c r="D1522" s="159"/>
+      <c r="E1522" s="159"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18397,9 +18398,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="160"/>
-      <c r="D1539" s="161"/>
-      <c r="E1539" s="161"/>
+      <c r="C1539" s="158"/>
+      <c r="D1539" s="159"/>
+      <c r="E1539" s="159"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18550,9 +18551,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="160"/>
-      <c r="D1556" s="161"/>
-      <c r="E1556" s="161"/>
+      <c r="C1556" s="158"/>
+      <c r="D1556" s="159"/>
+      <c r="E1556" s="159"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18703,9 +18704,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="160"/>
-      <c r="D1573" s="161"/>
-      <c r="E1573" s="161"/>
+      <c r="C1573" s="158"/>
+      <c r="D1573" s="159"/>
+      <c r="E1573" s="159"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18856,9 +18857,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="160"/>
-      <c r="D1590" s="161"/>
-      <c r="E1590" s="161"/>
+      <c r="C1590" s="158"/>
+      <c r="D1590" s="159"/>
+      <c r="E1590" s="159"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -19009,9 +19010,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="160"/>
-      <c r="D1607" s="161"/>
-      <c r="E1607" s="161"/>
+      <c r="C1607" s="158"/>
+      <c r="D1607" s="159"/>
+      <c r="E1607" s="159"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -19162,9 +19163,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="160"/>
-      <c r="D1624" s="161"/>
-      <c r="E1624" s="161"/>
+      <c r="C1624" s="158"/>
+      <c r="D1624" s="159"/>
+      <c r="E1624" s="159"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19315,18 +19316,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="174"/>
-      <c r="D1641" s="175"/>
-      <c r="E1641" s="175"/>
+      <c r="C1641" s="164"/>
+      <c r="D1641" s="165"/>
+      <c r="E1641" s="165"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="160"/>
-      <c r="D1642" s="161"/>
-      <c r="E1642" s="161"/>
+      <c r="C1642" s="158"/>
+      <c r="D1642" s="159"/>
+      <c r="E1642" s="159"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19477,9 +19478,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="162"/>
-      <c r="D1659" s="163"/>
-      <c r="E1659" s="163"/>
+      <c r="C1659" s="160"/>
+      <c r="D1659" s="161"/>
+      <c r="E1659" s="161"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19630,9 +19631,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="160"/>
-      <c r="D1676" s="161"/>
-      <c r="E1676" s="161"/>
+      <c r="C1676" s="158"/>
+      <c r="D1676" s="159"/>
+      <c r="E1676" s="159"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19783,9 +19784,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="160"/>
-      <c r="D1693" s="161"/>
-      <c r="E1693" s="161"/>
+      <c r="C1693" s="158"/>
+      <c r="D1693" s="159"/>
+      <c r="E1693" s="159"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19936,9 +19937,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="160"/>
-      <c r="D1710" s="161"/>
-      <c r="E1710" s="161"/>
+      <c r="C1710" s="158"/>
+      <c r="D1710" s="159"/>
+      <c r="E1710" s="159"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -20089,9 +20090,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="160"/>
-      <c r="D1727" s="161"/>
-      <c r="E1727" s="161"/>
+      <c r="C1727" s="158"/>
+      <c r="D1727" s="159"/>
+      <c r="E1727" s="159"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20242,9 +20243,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="160"/>
-      <c r="D1744" s="161"/>
-      <c r="E1744" s="161"/>
+      <c r="C1744" s="158"/>
+      <c r="D1744" s="159"/>
+      <c r="E1744" s="159"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20395,9 +20396,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="160"/>
-      <c r="D1761" s="161"/>
-      <c r="E1761" s="161"/>
+      <c r="C1761" s="158"/>
+      <c r="D1761" s="159"/>
+      <c r="E1761" s="159"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20548,9 +20549,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="160"/>
-      <c r="D1778" s="161"/>
-      <c r="E1778" s="161"/>
+      <c r="C1778" s="158"/>
+      <c r="D1778" s="159"/>
+      <c r="E1778" s="159"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20701,9 +20702,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="160"/>
-      <c r="D1795" s="161"/>
-      <c r="E1795" s="161"/>
+      <c r="C1795" s="158"/>
+      <c r="D1795" s="159"/>
+      <c r="E1795" s="159"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20854,9 +20855,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="160"/>
-      <c r="D1812" s="161"/>
-      <c r="E1812" s="161"/>
+      <c r="C1812" s="158"/>
+      <c r="D1812" s="159"/>
+      <c r="E1812" s="159"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -21007,9 +21008,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="160"/>
-      <c r="D1829" s="161"/>
-      <c r="E1829" s="161"/>
+      <c r="C1829" s="158"/>
+      <c r="D1829" s="159"/>
+      <c r="E1829" s="159"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -21160,9 +21161,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="160"/>
-      <c r="D1846" s="161"/>
-      <c r="E1846" s="161"/>
+      <c r="C1846" s="158"/>
+      <c r="D1846" s="159"/>
+      <c r="E1846" s="159"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21313,9 +21314,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="160"/>
-      <c r="D1863" s="161"/>
-      <c r="E1863" s="161"/>
+      <c r="C1863" s="158"/>
+      <c r="D1863" s="159"/>
+      <c r="E1863" s="159"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21466,9 +21467,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="160"/>
-      <c r="D1880" s="161"/>
-      <c r="E1880" s="161"/>
+      <c r="C1880" s="158"/>
+      <c r="D1880" s="159"/>
+      <c r="E1880" s="159"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21619,9 +21620,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="160"/>
-      <c r="D1897" s="161"/>
-      <c r="E1897" s="161"/>
+      <c r="C1897" s="158"/>
+      <c r="D1897" s="159"/>
+      <c r="E1897" s="159"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21772,18 +21773,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="176"/>
-      <c r="D1914" s="177"/>
-      <c r="E1914" s="177"/>
+      <c r="C1914" s="162"/>
+      <c r="D1914" s="163"/>
+      <c r="E1914" s="163"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="160"/>
-      <c r="D1915" s="161"/>
-      <c r="E1915" s="161"/>
+      <c r="C1915" s="158"/>
+      <c r="D1915" s="159"/>
+      <c r="E1915" s="159"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21934,9 +21935,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="162"/>
-      <c r="D1932" s="163"/>
-      <c r="E1932" s="163"/>
+      <c r="C1932" s="160"/>
+      <c r="D1932" s="161"/>
+      <c r="E1932" s="161"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -22087,9 +22088,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="160"/>
-      <c r="D1949" s="161"/>
-      <c r="E1949" s="161"/>
+      <c r="C1949" s="158"/>
+      <c r="D1949" s="159"/>
+      <c r="E1949" s="159"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22240,9 +22241,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="160"/>
-      <c r="D1966" s="161"/>
-      <c r="E1966" s="161"/>
+      <c r="C1966" s="158"/>
+      <c r="D1966" s="159"/>
+      <c r="E1966" s="159"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22393,9 +22394,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="160"/>
-      <c r="D1983" s="161"/>
-      <c r="E1983" s="161"/>
+      <c r="C1983" s="158"/>
+      <c r="D1983" s="159"/>
+      <c r="E1983" s="159"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22546,9 +22547,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="160"/>
-      <c r="D2000" s="161"/>
-      <c r="E2000" s="161"/>
+      <c r="C2000" s="158"/>
+      <c r="D2000" s="159"/>
+      <c r="E2000" s="159"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22699,9 +22700,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="160"/>
-      <c r="D2017" s="161"/>
-      <c r="E2017" s="161"/>
+      <c r="C2017" s="158"/>
+      <c r="D2017" s="159"/>
+      <c r="E2017" s="159"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22852,9 +22853,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="160"/>
-      <c r="D2034" s="161"/>
-      <c r="E2034" s="161"/>
+      <c r="C2034" s="158"/>
+      <c r="D2034" s="159"/>
+      <c r="E2034" s="159"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -23005,9 +23006,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="160"/>
-      <c r="D2051" s="161"/>
-      <c r="E2051" s="161"/>
+      <c r="C2051" s="158"/>
+      <c r="D2051" s="159"/>
+      <c r="E2051" s="159"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -23158,9 +23159,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="160"/>
-      <c r="D2068" s="161"/>
-      <c r="E2068" s="161"/>
+      <c r="C2068" s="158"/>
+      <c r="D2068" s="159"/>
+      <c r="E2068" s="159"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23311,9 +23312,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="160"/>
-      <c r="D2085" s="161"/>
-      <c r="E2085" s="161"/>
+      <c r="C2085" s="158"/>
+      <c r="D2085" s="159"/>
+      <c r="E2085" s="159"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23464,9 +23465,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="160"/>
-      <c r="D2102" s="161"/>
-      <c r="E2102" s="161"/>
+      <c r="C2102" s="158"/>
+      <c r="D2102" s="159"/>
+      <c r="E2102" s="159"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23617,9 +23618,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="160"/>
-      <c r="D2119" s="161"/>
-      <c r="E2119" s="161"/>
+      <c r="C2119" s="158"/>
+      <c r="D2119" s="159"/>
+      <c r="E2119" s="159"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23770,9 +23771,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="160"/>
-      <c r="D2136" s="161"/>
-      <c r="E2136" s="161"/>
+      <c r="C2136" s="158"/>
+      <c r="D2136" s="159"/>
+      <c r="E2136" s="159"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23923,9 +23924,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="160"/>
-      <c r="D2153" s="161"/>
-      <c r="E2153" s="161"/>
+      <c r="C2153" s="158"/>
+      <c r="D2153" s="159"/>
+      <c r="E2153" s="159"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -24076,9 +24077,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="160"/>
-      <c r="D2170" s="161"/>
-      <c r="E2170" s="161"/>
+      <c r="C2170" s="158"/>
+      <c r="D2170" s="159"/>
+      <c r="E2170" s="159"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -24226,15 +24227,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24247,124 +24355,17 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24389,51 +24390,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="185" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
-      <c r="G1" s="184"/>
-      <c r="H1" s="184"/>
-      <c r="I1" s="184"/>
-      <c r="J1" s="184"/>
-      <c r="K1" s="184"/>
-      <c r="L1" s="184"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="185"/>
+      <c r="K1" s="185"/>
+      <c r="L1" s="185"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="181" t="s">
+      <c r="A2" s="182" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="183"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="183"/>
+      <c r="K2" s="183"/>
+      <c r="L2" s="184"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="178" t="s">
+      <c r="A3" s="179" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="179"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="179"/>
-      <c r="I3" s="179"/>
-      <c r="J3" s="179"/>
-      <c r="K3" s="180"/>
+      <c r="B3" s="180"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
+      <c r="F3" s="180"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="180"/>
+      <c r="J3" s="180"/>
+      <c r="K3" s="181"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -24650,19 +24651,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="178" t="s">
+      <c r="A20" s="179" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="179"/>
-      <c r="C20" s="179"/>
-      <c r="D20" s="179"/>
-      <c r="E20" s="179"/>
-      <c r="F20" s="179"/>
-      <c r="G20" s="179"/>
-      <c r="H20" s="179"/>
-      <c r="I20" s="179"/>
-      <c r="J20" s="179"/>
-      <c r="K20" s="180"/>
+      <c r="B20" s="180"/>
+      <c r="C20" s="180"/>
+      <c r="D20" s="180"/>
+      <c r="E20" s="180"/>
+      <c r="F20" s="180"/>
+      <c r="G20" s="180"/>
+      <c r="H20" s="180"/>
+      <c r="I20" s="180"/>
+      <c r="J20" s="180"/>
+      <c r="K20" s="181"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -24879,19 +24880,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="178" t="s">
+      <c r="A37" s="179" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="179"/>
-      <c r="C37" s="179"/>
-      <c r="D37" s="179"/>
-      <c r="E37" s="179"/>
-      <c r="F37" s="179"/>
-      <c r="G37" s="179"/>
-      <c r="H37" s="179"/>
-      <c r="I37" s="179"/>
-      <c r="J37" s="179"/>
-      <c r="K37" s="180"/>
+      <c r="B37" s="180"/>
+      <c r="C37" s="180"/>
+      <c r="D37" s="180"/>
+      <c r="E37" s="180"/>
+      <c r="F37" s="180"/>
+      <c r="G37" s="180"/>
+      <c r="H37" s="180"/>
+      <c r="I37" s="180"/>
+      <c r="J37" s="180"/>
+      <c r="K37" s="181"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -25115,7 +25116,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25149,28 +25150,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="185"/>
+      <c r="A3" s="186"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="186"/>
+      <c r="A4" s="187"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="186"/>
+      <c r="A5" s="187"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="186"/>
+      <c r="A6" s="187"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="186"/>
+      <c r="A7" s="187"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="186"/>
+      <c r="A8" s="187"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="186"/>
+      <c r="A9" s="187"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="187"/>
+      <c r="A10" s="188"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -25326,7 +25327,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25353,10 +25354,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="188" t="s">
+      <c r="B1" s="189" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="189"/>
+      <c r="C1" s="190"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25367,7 +25368,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="191" t="s">
         <v>213</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25381,7 +25382,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="191"/>
+      <c r="A4" s="192"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25393,7 +25394,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="191"/>
+      <c r="A5" s="192"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25402,7 +25403,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="191"/>
+      <c r="A6" s="192"/>
       <c r="B6" s="139" t="s">
         <v>215</v>
       </c>
@@ -25414,7 +25415,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="191"/>
+      <c r="A7" s="192"/>
       <c r="B7" s="128" t="s">
         <v>178</v>
       </c>
@@ -25426,7 +25427,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="191"/>
+      <c r="A8" s="192"/>
       <c r="B8" s="128" t="s">
         <v>179</v>
       </c>
@@ -25435,7 +25436,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="192"/>
+      <c r="A9" s="193"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25450,7 +25451,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="190" t="s">
+      <c r="A11" s="191" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25464,7 +25465,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="191"/>
+      <c r="A12" s="192"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25476,7 +25477,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="191"/>
+      <c r="A13" s="192"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25485,7 +25486,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="191"/>
+      <c r="A14" s="192"/>
       <c r="B14" s="139" t="s">
         <v>215</v>
       </c>
@@ -25497,7 +25498,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="191"/>
+      <c r="A15" s="192"/>
       <c r="B15" s="128" t="s">
         <v>178</v>
       </c>
@@ -25509,7 +25510,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="191"/>
+      <c r="A16" s="192"/>
       <c r="B16" s="128" t="s">
         <v>179</v>
       </c>
@@ -25518,7 +25519,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="192"/>
+      <c r="A17" s="193"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25533,7 +25534,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="190" t="s">
+      <c r="A19" s="191" t="s">
         <v>214</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25542,7 +25543,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="191"/>
+      <c r="A20" s="192"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25552,14 +25553,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="191"/>
+      <c r="A21" s="192"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="191"/>
+      <c r="A22" s="192"/>
       <c r="B22" s="139" t="s">
         <v>215</v>
       </c>
@@ -25569,7 +25570,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="191"/>
+      <c r="A23" s="192"/>
       <c r="B23" s="128" t="s">
         <v>178</v>
       </c>
@@ -25579,14 +25580,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="191"/>
+      <c r="A24" s="192"/>
       <c r="B24" s="128" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="192"/>
+      <c r="A25" s="193"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25599,7 +25600,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25630,17 +25631,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="209" t="s">
+      <c r="A2" s="200" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="210"/>
+      <c r="B2" s="201"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="211" t="s">
+      <c r="A3" s="202" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="210"/>
+      <c r="B3" s="201"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -25656,115 +25657,128 @@
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="197" t="s">
+      <c r="A7" s="211" t="s">
         <v>197</v>
       </c>
-      <c r="B7" s="198"/>
+      <c r="B7" s="212"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="199" t="s">
+      <c r="A9" s="209" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="200"/>
+      <c r="B9" s="210"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="201"/>
-      <c r="B10" s="202"/>
+      <c r="A10" s="196"/>
+      <c r="B10" s="197"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="193" t="s">
+      <c r="A11" s="198" t="s">
         <v>199</v>
       </c>
-      <c r="B11" s="194"/>
+      <c r="B11" s="199"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="193" t="s">
+      <c r="A12" s="198" t="s">
         <v>200</v>
       </c>
-      <c r="B12" s="194"/>
+      <c r="B12" s="199"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="193" t="s">
+      <c r="A13" s="198" t="s">
         <v>201</v>
       </c>
-      <c r="B13" s="194"/>
+      <c r="B13" s="199"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="193" t="s">
+      <c r="A14" s="198" t="s">
         <v>202</v>
       </c>
-      <c r="B14" s="194"/>
+      <c r="B14" s="199"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="193" t="s">
+      <c r="A15" s="198" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="194"/>
+      <c r="B15" s="199"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="193" t="s">
+      <c r="A16" s="198" t="s">
         <v>204</v>
       </c>
-      <c r="B16" s="194"/>
+      <c r="B16" s="199"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="195" t="s">
+      <c r="A17" s="194" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="196"/>
+      <c r="B17" s="195"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="197" t="s">
+      <c r="A19" s="211" t="s">
         <v>208</v>
       </c>
-      <c r="B19" s="198"/>
+      <c r="B19" s="212"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="199" t="s">
+      <c r="A21" s="209" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="200"/>
+      <c r="B21" s="210"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="201"/>
-      <c r="B22" s="202"/>
+      <c r="A22" s="196"/>
+      <c r="B22" s="197"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="193" t="s">
+      <c r="A23" s="198" t="s">
         <v>210</v>
       </c>
-      <c r="B23" s="194"/>
+      <c r="B23" s="199"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="193"/>
-      <c r="B24" s="194"/>
+      <c r="A24" s="198"/>
+      <c r="B24" s="199"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="193" t="s">
+      <c r="A25" s="198" t="s">
         <v>211</v>
       </c>
-      <c r="B25" s="194"/>
+      <c r="B25" s="199"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="193" t="s">
+      <c r="A26" s="198" t="s">
         <v>212</v>
       </c>
-      <c r="B26" s="194"/>
+      <c r="B26" s="199"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="195"/>
-      <c r="B27" s="196"/>
+      <c r="A27" s="194"/>
+      <c r="B27" s="195"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25775,19 +25789,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Flintstones - more of level 3 redone using the crazy speed acceleration trick, 505 frames ahead of the published movie
</commit_message>
<xml_diff>
--- a/Flintstones/Compare/Flintstones.xlsx
+++ b/Flintstones/Compare/Flintstones.xlsx
@@ -1967,6 +1967,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1988,29 +1991,29 @@
     <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2046,34 +2049,20 @@
     <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2083,9 +2072,20 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2403,8 +2403,8 @@
   <dimension ref="A1:K159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+      <pane ySplit="6" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2420,16 +2420,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="156" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="156" t="s">
+      <c r="B1" s="155"/>
+      <c r="C1" s="157" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="158"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65541)</f>
@@ -2507,10 +2507,10 @@
       <c r="B5" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="154" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="153"/>
+      <c r="D5" s="154"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2526,10 +2526,10 @@
       <c r="B6" s="147" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="154" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="155"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2547,7 +2547,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="158" t="s">
+      <c r="A8" s="159" t="s">
         <v>190</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2567,7 +2567,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="151"/>
+      <c r="A9" s="152"/>
       <c r="B9" s="98" t="s">
         <v>185</v>
       </c>
@@ -2577,7 +2577,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="151"/>
+      <c r="A10" s="152"/>
       <c r="B10" s="100"/>
       <c r="C10" s="101"/>
       <c r="D10" s="101"/>
@@ -2588,7 +2588,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="151"/>
+      <c r="A11" s="152"/>
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
       <c r="D11" s="101"/>
@@ -2599,7 +2599,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="151"/>
+      <c r="A12" s="152"/>
       <c r="B12" s="100"/>
       <c r="C12" s="101"/>
       <c r="D12" s="101"/>
@@ -2610,7 +2610,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="151"/>
+      <c r="A13" s="152"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2621,7 +2621,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="151"/>
+      <c r="A14" s="152"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2632,7 +2632,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="151"/>
+      <c r="A15" s="152"/>
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
@@ -2643,7 +2643,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="151"/>
+      <c r="A16" s="152"/>
       <c r="B16" s="98" t="s">
         <v>188</v>
       </c>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="152" t="s">
+      <c r="A19" s="153" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2706,7 +2706,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="151"/>
+      <c r="A20" s="152"/>
       <c r="B20" s="98" t="s">
         <v>185</v>
       </c>
@@ -2719,7 +2719,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="151"/>
+      <c r="A21" s="152"/>
       <c r="B21" s="100"/>
       <c r="C21" s="101"/>
       <c r="D21" s="101"/>
@@ -2730,7 +2730,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="151"/>
+      <c r="A22" s="152"/>
       <c r="B22" s="100"/>
       <c r="C22" s="101"/>
       <c r="D22" s="101"/>
@@ -2741,7 +2741,7 @@
       <c r="F22" s="105"/>
     </row>
     <row r="23" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="151"/>
+      <c r="A23" s="152"/>
       <c r="B23" s="100"/>
       <c r="C23" s="101"/>
       <c r="D23" s="101"/>
@@ -2752,7 +2752,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="151"/>
+      <c r="A24" s="152"/>
       <c r="B24" s="100"/>
       <c r="C24" s="101"/>
       <c r="D24" s="101"/>
@@ -2763,7 +2763,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="151"/>
+      <c r="A25" s="152"/>
       <c r="B25" s="100"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -2774,7 +2774,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="151"/>
+      <c r="A26" s="152"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -2785,7 +2785,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="151"/>
+      <c r="A27" s="152"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -2796,7 +2796,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="151"/>
+      <c r="A28" s="152"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2807,7 +2807,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="151"/>
+      <c r="A29" s="152"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2818,7 +2818,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="151"/>
+      <c r="A30" s="152"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2829,7 +2829,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="151"/>
+      <c r="A31" s="152"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2840,7 +2840,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="151"/>
+      <c r="A32" s="152"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2851,7 +2851,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="151"/>
+      <c r="A33" s="152"/>
       <c r="B33" s="98" t="s">
         <v>188</v>
       </c>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="150" t="s">
+      <c r="A36" s="151" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2910,7 +2910,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="151"/>
+      <c r="A37" s="152"/>
       <c r="B37" s="98" t="s">
         <v>185</v>
       </c>
@@ -2927,7 +2927,7 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="151"/>
+      <c r="A38" s="152"/>
       <c r="B38" s="148" t="s">
         <v>216</v>
       </c>
@@ -2944,7 +2944,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="151"/>
+      <c r="A39" s="152"/>
       <c r="B39" s="148" t="s">
         <v>217</v>
       </c>
@@ -2961,7 +2961,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="151"/>
+      <c r="A40" s="152"/>
       <c r="B40" s="148" t="s">
         <v>218</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="151"/>
+      <c r="A41" s="152"/>
       <c r="B41" s="148" t="s">
         <v>219</v>
       </c>
@@ -2995,7 +2995,7 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="151"/>
+      <c r="A42" s="152"/>
       <c r="B42" s="148" t="s">
         <v>217</v>
       </c>
@@ -3012,7 +3012,7 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="151"/>
+      <c r="A43" s="152"/>
       <c r="B43" s="148" t="s">
         <v>220</v>
       </c>
@@ -3029,7 +3029,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="151"/>
+      <c r="A44" s="152"/>
       <c r="B44" s="148" t="s">
         <v>221</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="151"/>
+      <c r="A45" s="152"/>
       <c r="B45" s="148" t="s">
         <v>169</v>
       </c>
@@ -3063,7 +3063,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="151"/>
+      <c r="A46" s="152"/>
       <c r="B46" s="148" t="s">
         <v>217</v>
       </c>
@@ -3080,7 +3080,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="151"/>
+      <c r="A47" s="152"/>
       <c r="B47" s="148" t="s">
         <v>169</v>
       </c>
@@ -3097,7 +3097,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="151"/>
+      <c r="A48" s="152"/>
       <c r="B48" s="148" t="s">
         <v>216</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="151"/>
+      <c r="A49" s="152"/>
       <c r="B49" s="148" t="s">
         <v>217</v>
       </c>
@@ -3131,7 +3131,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="151"/>
+      <c r="A50" s="152"/>
       <c r="B50" s="148" t="s">
         <v>169</v>
       </c>
@@ -3148,7 +3148,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="151"/>
+      <c r="A51" s="152"/>
       <c r="B51" s="148"/>
       <c r="C51" s="101"/>
       <c r="D51" s="101"/>
@@ -3156,7 +3156,7 @@
       <c r="F51" s="105"/>
     </row>
     <row r="52" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="151"/>
+      <c r="A52" s="152"/>
       <c r="B52" s="148"/>
       <c r="C52" s="101"/>
       <c r="D52" s="101"/>
@@ -3164,7 +3164,7 @@
       <c r="F52" s="105"/>
     </row>
     <row r="53" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="151"/>
+      <c r="A53" s="152"/>
       <c r="B53" s="100"/>
       <c r="C53" s="101"/>
       <c r="D53" s="101"/>
@@ -3175,7 +3175,7 @@
       <c r="F53" s="105"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="151"/>
+      <c r="A54" s="152"/>
       <c r="B54" s="98" t="s">
         <v>188</v>
       </c>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="56" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="152" t="s">
+      <c r="A57" s="153" t="s">
         <v>171</v>
       </c>
       <c r="B57" s="109" t="s">
@@ -3238,7 +3238,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="151"/>
+      <c r="A58" s="152"/>
       <c r="B58" s="98" t="s">
         <v>185</v>
       </c>
@@ -3255,7 +3255,7 @@
       <c r="F58" s="104"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="151"/>
+      <c r="A59" s="152"/>
       <c r="B59" s="148" t="s">
         <v>216</v>
       </c>
@@ -3272,24 +3272,24 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="151"/>
+      <c r="A60" s="152"/>
       <c r="B60" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C60" s="101">
-        <v>14450</v>
+        <v>14360</v>
       </c>
       <c r="D60" s="101">
         <v>14480</v>
       </c>
       <c r="E60" s="123">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="151"/>
+      <c r="A61" s="152"/>
       <c r="B61" s="148" t="s">
         <v>222</v>
       </c>
@@ -3304,41 +3304,41 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="151"/>
+      <c r="A62" s="152"/>
       <c r="B62" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C62" s="101">
-        <v>14820</v>
+        <v>14625</v>
       </c>
       <c r="D62" s="101">
         <v>14857</v>
       </c>
       <c r="E62" s="123">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>232</v>
       </c>
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="151"/>
+      <c r="A63" s="152"/>
       <c r="B63" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C63" s="101">
-        <v>14925</v>
+        <v>14733</v>
       </c>
       <c r="D63" s="101">
         <v>14964</v>
       </c>
       <c r="E63" s="123">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>231</v>
       </c>
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="151"/>
+      <c r="A64" s="152"/>
       <c r="B64" s="148" t="s">
         <v>223</v>
       </c>
@@ -3353,41 +3353,41 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="151"/>
+      <c r="A65" s="152"/>
       <c r="B65" s="148" t="s">
         <v>217</v>
       </c>
       <c r="C65" s="101">
-        <v>15418</v>
+        <v>14980</v>
       </c>
       <c r="D65" s="101">
         <v>15466</v>
       </c>
       <c r="E65" s="123">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>486</v>
       </c>
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="151"/>
+      <c r="A66" s="152"/>
       <c r="B66" s="148" t="s">
         <v>224</v>
       </c>
       <c r="C66" s="101">
-        <v>15652</v>
+        <v>15195</v>
       </c>
       <c r="D66" s="101">
         <v>15700</v>
       </c>
       <c r="E66" s="123">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>505</v>
       </c>
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="151"/>
+      <c r="A67" s="152"/>
       <c r="B67" s="148" t="s">
         <v>225</v>
       </c>
@@ -3404,7 +3404,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="151"/>
+      <c r="A68" s="152"/>
       <c r="B68" s="149" t="s">
         <v>217</v>
       </c>
@@ -3421,8 +3421,8 @@
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="151"/>
-      <c r="B69" s="214" t="s">
+      <c r="A69" s="152"/>
+      <c r="B69" s="150" t="s">
         <v>226</v>
       </c>
       <c r="C69" s="101">
@@ -3438,8 +3438,8 @@
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="151"/>
-      <c r="B70" s="214" t="s">
+      <c r="A70" s="152"/>
+      <c r="B70" s="150" t="s">
         <v>217</v>
       </c>
       <c r="C70" s="101">
@@ -3455,7 +3455,7 @@
       <c r="F70" s="105"/>
     </row>
     <row r="71" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="151"/>
+      <c r="A71" s="152"/>
       <c r="B71" s="149"/>
       <c r="C71" s="101"/>
       <c r="D71" s="101"/>
@@ -3466,7 +3466,7 @@
       <c r="F71" s="105"/>
     </row>
     <row r="72" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="151"/>
+      <c r="A72" s="152"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
@@ -3477,7 +3477,7 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="151"/>
+      <c r="A73" s="152"/>
       <c r="B73" s="98" t="s">
         <v>188</v>
       </c>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="75" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="150" t="s">
+      <c r="A76" s="151" t="s">
         <v>172</v>
       </c>
       <c r="B76" s="113" t="s">
@@ -3536,7 +3536,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="151"/>
+      <c r="A77" s="152"/>
       <c r="B77" s="98" t="s">
         <v>185</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="F77" s="104"/>
     </row>
     <row r="78" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="151"/>
+      <c r="A78" s="152"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3560,7 +3560,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="151"/>
+      <c r="A79" s="152"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3571,7 +3571,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="151"/>
+      <c r="A80" s="152"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3582,7 +3582,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="151"/>
+      <c r="A81" s="152"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3593,7 +3593,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="151"/>
+      <c r="A82" s="152"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3604,7 +3604,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="151"/>
+      <c r="A83" s="152"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3615,7 +3615,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="151"/>
+      <c r="A84" s="152"/>
       <c r="B84" s="100"/>
       <c r="C84" s="101"/>
       <c r="D84" s="101"/>
@@ -3626,7 +3626,7 @@
       <c r="F84" s="105"/>
     </row>
     <row r="85" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="151"/>
+      <c r="A85" s="152"/>
       <c r="B85" s="100"/>
       <c r="C85" s="101"/>
       <c r="D85" s="101"/>
@@ -3637,7 +3637,7 @@
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="151"/>
+      <c r="A86" s="152"/>
       <c r="B86" s="100"/>
       <c r="C86" s="101"/>
       <c r="D86" s="101"/>
@@ -3648,7 +3648,7 @@
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="151"/>
+      <c r="A87" s="152"/>
       <c r="B87" s="100"/>
       <c r="C87" s="101"/>
       <c r="D87" s="101"/>
@@ -3659,7 +3659,7 @@
       <c r="F87" s="105"/>
     </row>
     <row r="88" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="151"/>
+      <c r="A88" s="152"/>
       <c r="B88" s="100"/>
       <c r="C88" s="101"/>
       <c r="D88" s="101"/>
@@ -3670,7 +3670,7 @@
       <c r="F88" s="105"/>
     </row>
     <row r="89" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="151"/>
+      <c r="A89" s="152"/>
       <c r="B89" s="100"/>
       <c r="C89" s="101"/>
       <c r="D89" s="101"/>
@@ -3681,7 +3681,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="151"/>
+      <c r="A90" s="152"/>
       <c r="B90" s="98" t="s">
         <v>188</v>
       </c>
@@ -3720,7 +3720,7 @@
     </row>
     <row r="92" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="93" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="152" t="s">
+      <c r="A93" s="153" t="s">
         <v>173</v>
       </c>
       <c r="B93" s="109" t="s">
@@ -3740,7 +3740,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="151"/>
+      <c r="A94" s="152"/>
       <c r="B94" s="98" t="s">
         <v>185</v>
       </c>
@@ -3753,7 +3753,7 @@
       <c r="F94" s="104"/>
     </row>
     <row r="95" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="151"/>
+      <c r="A95" s="152"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3764,7 +3764,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="151"/>
+      <c r="A96" s="152"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3775,7 +3775,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="151"/>
+      <c r="A97" s="152"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3786,7 +3786,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="151"/>
+      <c r="A98" s="152"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3797,7 +3797,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="151"/>
+      <c r="A99" s="152"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3808,7 +3808,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="151"/>
+      <c r="A100" s="152"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3819,7 +3819,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="151"/>
+      <c r="A101" s="152"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -3830,7 +3830,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="151"/>
+      <c r="A102" s="152"/>
       <c r="B102" s="100"/>
       <c r="C102" s="101"/>
       <c r="D102" s="101"/>
@@ -3841,7 +3841,7 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="151"/>
+      <c r="A103" s="152"/>
       <c r="B103" s="100"/>
       <c r="C103" s="101"/>
       <c r="D103" s="101"/>
@@ -3852,7 +3852,7 @@
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="151"/>
+      <c r="A104" s="152"/>
       <c r="B104" s="100"/>
       <c r="C104" s="101"/>
       <c r="D104" s="101"/>
@@ -3863,7 +3863,7 @@
       <c r="F104" s="105"/>
     </row>
     <row r="105" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="151"/>
+      <c r="A105" s="152"/>
       <c r="B105" s="100"/>
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
@@ -3874,7 +3874,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="151"/>
+      <c r="A106" s="152"/>
       <c r="B106" s="100"/>
       <c r="C106" s="101"/>
       <c r="D106" s="101"/>
@@ -3885,7 +3885,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="151"/>
+      <c r="A107" s="152"/>
       <c r="B107" s="98" t="s">
         <v>188</v>
       </c>
@@ -3923,7 +3923,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="150" t="s">
+      <c r="A110" s="151" t="s">
         <v>174</v>
       </c>
       <c r="B110" s="113" t="s">
@@ -3943,7 +3943,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="151"/>
+      <c r="A111" s="152"/>
       <c r="B111" s="98" t="s">
         <v>185</v>
       </c>
@@ -3956,7 +3956,7 @@
       <c r="F111" s="104"/>
     </row>
     <row r="112" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="151"/>
+      <c r="A112" s="152"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3967,7 +3967,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="151"/>
+      <c r="A113" s="152"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3978,7 +3978,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="151"/>
+      <c r="A114" s="152"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3989,7 +3989,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="151"/>
+      <c r="A115" s="152"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -4000,7 +4000,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="151"/>
+      <c r="A116" s="152"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -4011,7 +4011,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="151"/>
+      <c r="A117" s="152"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -4022,7 +4022,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="151"/>
+      <c r="A118" s="152"/>
       <c r="B118" s="100"/>
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
@@ -4033,7 +4033,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="151"/>
+      <c r="A119" s="152"/>
       <c r="B119" s="100"/>
       <c r="C119" s="101"/>
       <c r="D119" s="101"/>
@@ -4044,7 +4044,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="151"/>
+      <c r="A120" s="152"/>
       <c r="B120" s="100"/>
       <c r="C120" s="101"/>
       <c r="D120" s="101"/>
@@ -4055,7 +4055,7 @@
       <c r="F120" s="105"/>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="151"/>
+      <c r="A121" s="152"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -4066,7 +4066,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="151"/>
+      <c r="A122" s="152"/>
       <c r="B122" s="100"/>
       <c r="C122" s="101"/>
       <c r="D122" s="101"/>
@@ -4077,7 +4077,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="151"/>
+      <c r="A123" s="152"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -4088,7 +4088,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="151"/>
+      <c r="A124" s="152"/>
       <c r="B124" s="98" t="s">
         <v>188</v>
       </c>
@@ -4126,7 +4126,7 @@
       </c>
     </row>
     <row r="127" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="152" t="s">
+      <c r="A127" s="153" t="s">
         <v>175</v>
       </c>
       <c r="B127" s="109" t="s">
@@ -4146,7 +4146,7 @@
       </c>
     </row>
     <row r="128" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="151"/>
+      <c r="A128" s="152"/>
       <c r="B128" s="98" t="s">
         <v>185</v>
       </c>
@@ -4159,7 +4159,7 @@
       <c r="F128" s="104"/>
     </row>
     <row r="129" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="151"/>
+      <c r="A129" s="152"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4170,7 +4170,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="151"/>
+      <c r="A130" s="152"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4181,7 +4181,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="151"/>
+      <c r="A131" s="152"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4192,7 +4192,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="151"/>
+      <c r="A132" s="152"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4203,7 +4203,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="151"/>
+      <c r="A133" s="152"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4214,7 +4214,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="151"/>
+      <c r="A134" s="152"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4225,7 +4225,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="151"/>
+      <c r="A135" s="152"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4236,7 +4236,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="151"/>
+      <c r="A136" s="152"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
       <c r="D136" s="101"/>
@@ -4247,7 +4247,7 @@
       <c r="F136" s="105"/>
     </row>
     <row r="137" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="151"/>
+      <c r="A137" s="152"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4258,7 +4258,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="151"/>
+      <c r="A138" s="152"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4269,7 +4269,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="151"/>
+      <c r="A139" s="152"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4280,7 +4280,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="151"/>
+      <c r="A140" s="152"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4291,7 +4291,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="151"/>
+      <c r="A141" s="152"/>
       <c r="B141" s="98" t="s">
         <v>188</v>
       </c>
@@ -4329,7 +4329,7 @@
       </c>
     </row>
     <row r="144" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A144" s="150" t="s">
+      <c r="A144" s="151" t="s">
         <v>176</v>
       </c>
       <c r="B144" s="113" t="s">
@@ -4349,7 +4349,7 @@
       </c>
     </row>
     <row r="145" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="151"/>
+      <c r="A145" s="152"/>
       <c r="B145" s="98" t="s">
         <v>185</v>
       </c>
@@ -4362,7 +4362,7 @@
       <c r="F145" s="104"/>
     </row>
     <row r="146" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="151"/>
+      <c r="A146" s="152"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4373,7 +4373,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A147" s="151"/>
+      <c r="A147" s="152"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4384,7 +4384,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A148" s="151"/>
+      <c r="A148" s="152"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4395,7 +4395,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A149" s="151"/>
+      <c r="A149" s="152"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
@@ -4406,7 +4406,7 @@
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A150" s="151"/>
+      <c r="A150" s="152"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -4417,7 +4417,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A151" s="151"/>
+      <c r="A151" s="152"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -4428,7 +4428,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A152" s="151"/>
+      <c r="A152" s="152"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
@@ -4439,7 +4439,7 @@
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A153" s="151"/>
+      <c r="A153" s="152"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
@@ -4450,7 +4450,7 @@
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A154" s="151"/>
+      <c r="A154" s="152"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -4461,7 +4461,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A155" s="151"/>
+      <c r="A155" s="152"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
@@ -4472,7 +4472,7 @@
       <c r="F155" s="105"/>
     </row>
     <row r="156" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A156" s="151"/>
+      <c r="A156" s="152"/>
       <c r="B156" s="100"/>
       <c r="C156" s="101"/>
       <c r="D156" s="101"/>
@@ -4483,7 +4483,7 @@
       <c r="F156" s="105"/>
     </row>
     <row r="157" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A157" s="151"/>
+      <c r="A157" s="152"/>
       <c r="B157" s="100"/>
       <c r="C157" s="101"/>
       <c r="D157" s="101"/>
@@ -4494,7 +4494,7 @@
       <c r="F157" s="105"/>
     </row>
     <row r="158" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="151"/>
+      <c r="A158" s="152"/>
       <c r="B158" s="98" t="s">
         <v>188</v>
       </c>
@@ -4533,11 +4533,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A144:A158"/>
-    <mergeCell ref="A110:A124"/>
-    <mergeCell ref="A76:A90"/>
-    <mergeCell ref="A127:A141"/>
-    <mergeCell ref="A93:A107"/>
     <mergeCell ref="A36:A54"/>
     <mergeCell ref="A57:A73"/>
     <mergeCell ref="C5:D5"/>
@@ -4546,6 +4541,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A144:A158"/>
+    <mergeCell ref="A110:A124"/>
+    <mergeCell ref="A76:A90"/>
+    <mergeCell ref="A127:A141"/>
+    <mergeCell ref="A93:A107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4577,13 +4577,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="178" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4613,18 +4613,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="162"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4776,9 +4776,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="164"/>
-      <c r="D21" s="165"/>
-      <c r="E21" s="165"/>
+      <c r="C21" s="162"/>
+      <c r="D21" s="163"/>
+      <c r="E21" s="163"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4929,9 +4929,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="162"/>
-      <c r="D38" s="163"/>
-      <c r="E38" s="163"/>
+      <c r="C38" s="160"/>
+      <c r="D38" s="161"/>
+      <c r="E38" s="161"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -5082,9 +5082,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="162"/>
-      <c r="D55" s="163"/>
-      <c r="E55" s="163"/>
+      <c r="C55" s="160"/>
+      <c r="D55" s="161"/>
+      <c r="E55" s="161"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -5235,9 +5235,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="162"/>
-      <c r="D72" s="163"/>
-      <c r="E72" s="163"/>
+      <c r="C72" s="160"/>
+      <c r="D72" s="161"/>
+      <c r="E72" s="161"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5388,9 +5388,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="162"/>
-      <c r="D89" s="163"/>
-      <c r="E89" s="163"/>
+      <c r="C89" s="160"/>
+      <c r="D89" s="161"/>
+      <c r="E89" s="161"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5541,9 +5541,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="162"/>
-      <c r="D106" s="163"/>
-      <c r="E106" s="163"/>
+      <c r="C106" s="160"/>
+      <c r="D106" s="161"/>
+      <c r="E106" s="161"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5694,9 +5694,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="162"/>
-      <c r="D123" s="163"/>
-      <c r="E123" s="163"/>
+      <c r="C123" s="160"/>
+      <c r="D123" s="161"/>
+      <c r="E123" s="161"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5847,9 +5847,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="162"/>
-      <c r="D140" s="163"/>
-      <c r="E140" s="163"/>
+      <c r="C140" s="160"/>
+      <c r="D140" s="161"/>
+      <c r="E140" s="161"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -6000,9 +6000,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="162"/>
-      <c r="D157" s="163"/>
-      <c r="E157" s="163"/>
+      <c r="C157" s="160"/>
+      <c r="D157" s="161"/>
+      <c r="E157" s="161"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -6153,9 +6153,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="162"/>
-      <c r="D174" s="163"/>
-      <c r="E174" s="163"/>
+      <c r="C174" s="160"/>
+      <c r="D174" s="161"/>
+      <c r="E174" s="161"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6306,9 +6306,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="162"/>
-      <c r="D191" s="163"/>
-      <c r="E191" s="163"/>
+      <c r="C191" s="160"/>
+      <c r="D191" s="161"/>
+      <c r="E191" s="161"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6459,9 +6459,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="162"/>
-      <c r="D208" s="163"/>
-      <c r="E208" s="163"/>
+      <c r="C208" s="160"/>
+      <c r="D208" s="161"/>
+      <c r="E208" s="161"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6612,9 +6612,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="162"/>
-      <c r="D225" s="163"/>
-      <c r="E225" s="163"/>
+      <c r="C225" s="160"/>
+      <c r="D225" s="161"/>
+      <c r="E225" s="161"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6765,9 +6765,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="162"/>
-      <c r="D242" s="163"/>
-      <c r="E242" s="163"/>
+      <c r="C242" s="160"/>
+      <c r="D242" s="161"/>
+      <c r="E242" s="161"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6918,9 +6918,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="162"/>
-      <c r="D259" s="163"/>
-      <c r="E259" s="163"/>
+      <c r="C259" s="160"/>
+      <c r="D259" s="161"/>
+      <c r="E259" s="161"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -7071,18 +7071,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="166"/>
-      <c r="D276" s="167"/>
-      <c r="E276" s="167"/>
+      <c r="C276" s="176"/>
+      <c r="D276" s="177"/>
+      <c r="E276" s="177"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="162"/>
-      <c r="D277" s="163"/>
-      <c r="E277" s="163"/>
+      <c r="C277" s="160"/>
+      <c r="D277" s="161"/>
+      <c r="E277" s="161"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -7233,9 +7233,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="164"/>
-      <c r="D294" s="165"/>
-      <c r="E294" s="165"/>
+      <c r="C294" s="162"/>
+      <c r="D294" s="163"/>
+      <c r="E294" s="163"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7386,9 +7386,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="162"/>
-      <c r="D311" s="163"/>
-      <c r="E311" s="163"/>
+      <c r="C311" s="160"/>
+      <c r="D311" s="161"/>
+      <c r="E311" s="161"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7539,9 +7539,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="162"/>
-      <c r="D328" s="163"/>
-      <c r="E328" s="163"/>
+      <c r="C328" s="160"/>
+      <c r="D328" s="161"/>
+      <c r="E328" s="161"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7692,9 +7692,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="162"/>
-      <c r="D345" s="163"/>
-      <c r="E345" s="163"/>
+      <c r="C345" s="160"/>
+      <c r="D345" s="161"/>
+      <c r="E345" s="161"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7845,9 +7845,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="162"/>
-      <c r="D362" s="163"/>
-      <c r="E362" s="163"/>
+      <c r="C362" s="160"/>
+      <c r="D362" s="161"/>
+      <c r="E362" s="161"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7998,9 +7998,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="162"/>
-      <c r="D379" s="163"/>
-      <c r="E379" s="163"/>
+      <c r="C379" s="160"/>
+      <c r="D379" s="161"/>
+      <c r="E379" s="161"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -8151,9 +8151,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="162"/>
-      <c r="D396" s="163"/>
-      <c r="E396" s="163"/>
+      <c r="C396" s="160"/>
+      <c r="D396" s="161"/>
+      <c r="E396" s="161"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8304,9 +8304,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="162"/>
-      <c r="D413" s="163"/>
-      <c r="E413" s="163"/>
+      <c r="C413" s="160"/>
+      <c r="D413" s="161"/>
+      <c r="E413" s="161"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8457,9 +8457,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="162"/>
-      <c r="D430" s="163"/>
-      <c r="E430" s="163"/>
+      <c r="C430" s="160"/>
+      <c r="D430" s="161"/>
+      <c r="E430" s="161"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8610,9 +8610,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="162"/>
-      <c r="D447" s="163"/>
-      <c r="E447" s="163"/>
+      <c r="C447" s="160"/>
+      <c r="D447" s="161"/>
+      <c r="E447" s="161"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8763,9 +8763,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="162"/>
-      <c r="D464" s="163"/>
-      <c r="E464" s="163"/>
+      <c r="C464" s="160"/>
+      <c r="D464" s="161"/>
+      <c r="E464" s="161"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8916,9 +8916,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="162"/>
-      <c r="D481" s="163"/>
-      <c r="E481" s="163"/>
+      <c r="C481" s="160"/>
+      <c r="D481" s="161"/>
+      <c r="E481" s="161"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -9069,9 +9069,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="162"/>
-      <c r="D498" s="163"/>
-      <c r="E498" s="163"/>
+      <c r="C498" s="160"/>
+      <c r="D498" s="161"/>
+      <c r="E498" s="161"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -9222,9 +9222,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="162"/>
-      <c r="D515" s="163"/>
-      <c r="E515" s="163"/>
+      <c r="C515" s="160"/>
+      <c r="D515" s="161"/>
+      <c r="E515" s="161"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9375,9 +9375,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="162"/>
-      <c r="D532" s="163"/>
-      <c r="E532" s="163"/>
+      <c r="C532" s="160"/>
+      <c r="D532" s="161"/>
+      <c r="E532" s="161"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9528,18 +9528,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="168"/>
-      <c r="D549" s="169"/>
-      <c r="E549" s="169"/>
+      <c r="C549" s="174"/>
+      <c r="D549" s="175"/>
+      <c r="E549" s="175"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="162"/>
-      <c r="D550" s="163"/>
-      <c r="E550" s="163"/>
+      <c r="C550" s="160"/>
+      <c r="D550" s="161"/>
+      <c r="E550" s="161"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9690,9 +9690,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="164"/>
-      <c r="D567" s="165"/>
-      <c r="E567" s="165"/>
+      <c r="C567" s="162"/>
+      <c r="D567" s="163"/>
+      <c r="E567" s="163"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9843,9 +9843,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="162"/>
-      <c r="D584" s="163"/>
-      <c r="E584" s="163"/>
+      <c r="C584" s="160"/>
+      <c r="D584" s="161"/>
+      <c r="E584" s="161"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9996,9 +9996,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="162"/>
-      <c r="D601" s="163"/>
-      <c r="E601" s="163"/>
+      <c r="C601" s="160"/>
+      <c r="D601" s="161"/>
+      <c r="E601" s="161"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -10149,9 +10149,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="162"/>
-      <c r="D618" s="163"/>
-      <c r="E618" s="163"/>
+      <c r="C618" s="160"/>
+      <c r="D618" s="161"/>
+      <c r="E618" s="161"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10302,9 +10302,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="162"/>
-      <c r="D635" s="163"/>
-      <c r="E635" s="163"/>
+      <c r="C635" s="160"/>
+      <c r="D635" s="161"/>
+      <c r="E635" s="161"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10455,9 +10455,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="162"/>
-      <c r="D652" s="163"/>
-      <c r="E652" s="163"/>
+      <c r="C652" s="160"/>
+      <c r="D652" s="161"/>
+      <c r="E652" s="161"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10608,9 +10608,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="162"/>
-      <c r="D669" s="163"/>
-      <c r="E669" s="163"/>
+      <c r="C669" s="160"/>
+      <c r="D669" s="161"/>
+      <c r="E669" s="161"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10761,9 +10761,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="162"/>
-      <c r="D686" s="163"/>
-      <c r="E686" s="163"/>
+      <c r="C686" s="160"/>
+      <c r="D686" s="161"/>
+      <c r="E686" s="161"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10914,9 +10914,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="162"/>
-      <c r="D703" s="163"/>
-      <c r="E703" s="163"/>
+      <c r="C703" s="160"/>
+      <c r="D703" s="161"/>
+      <c r="E703" s="161"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -11067,9 +11067,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="162"/>
-      <c r="D720" s="163"/>
-      <c r="E720" s="163"/>
+      <c r="C720" s="160"/>
+      <c r="D720" s="161"/>
+      <c r="E720" s="161"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -11220,9 +11220,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="162"/>
-      <c r="D737" s="163"/>
-      <c r="E737" s="163"/>
+      <c r="C737" s="160"/>
+      <c r="D737" s="161"/>
+      <c r="E737" s="161"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11373,9 +11373,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="162"/>
-      <c r="D754" s="163"/>
-      <c r="E754" s="163"/>
+      <c r="C754" s="160"/>
+      <c r="D754" s="161"/>
+      <c r="E754" s="161"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11526,9 +11526,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="162"/>
-      <c r="D771" s="163"/>
-      <c r="E771" s="163"/>
+      <c r="C771" s="160"/>
+      <c r="D771" s="161"/>
+      <c r="E771" s="161"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11679,9 +11679,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="162"/>
-      <c r="D788" s="163"/>
-      <c r="E788" s="163"/>
+      <c r="C788" s="160"/>
+      <c r="D788" s="161"/>
+      <c r="E788" s="161"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11832,9 +11832,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="162"/>
-      <c r="D805" s="163"/>
-      <c r="E805" s="163"/>
+      <c r="C805" s="160"/>
+      <c r="D805" s="161"/>
+      <c r="E805" s="161"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11985,18 +11985,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="170"/>
-      <c r="D822" s="171"/>
-      <c r="E822" s="171"/>
+      <c r="C822" s="172"/>
+      <c r="D822" s="173"/>
+      <c r="E822" s="173"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="162"/>
-      <c r="D823" s="163"/>
-      <c r="E823" s="163"/>
+      <c r="C823" s="160"/>
+      <c r="D823" s="161"/>
+      <c r="E823" s="161"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -12147,9 +12147,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="164"/>
-      <c r="D840" s="165"/>
-      <c r="E840" s="165"/>
+      <c r="C840" s="162"/>
+      <c r="D840" s="163"/>
+      <c r="E840" s="163"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12300,9 +12300,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="162"/>
-      <c r="D857" s="163"/>
-      <c r="E857" s="163"/>
+      <c r="C857" s="160"/>
+      <c r="D857" s="161"/>
+      <c r="E857" s="161"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12453,9 +12453,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="162"/>
-      <c r="D874" s="163"/>
-      <c r="E874" s="163"/>
+      <c r="C874" s="160"/>
+      <c r="D874" s="161"/>
+      <c r="E874" s="161"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12606,9 +12606,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="162"/>
-      <c r="D891" s="163"/>
-      <c r="E891" s="163"/>
+      <c r="C891" s="160"/>
+      <c r="D891" s="161"/>
+      <c r="E891" s="161"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12759,9 +12759,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="162"/>
-      <c r="D908" s="163"/>
-      <c r="E908" s="163"/>
+      <c r="C908" s="160"/>
+      <c r="D908" s="161"/>
+      <c r="E908" s="161"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12912,9 +12912,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="162"/>
-      <c r="D925" s="163"/>
-      <c r="E925" s="163"/>
+      <c r="C925" s="160"/>
+      <c r="D925" s="161"/>
+      <c r="E925" s="161"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -13065,9 +13065,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="162"/>
-      <c r="D942" s="163"/>
-      <c r="E942" s="163"/>
+      <c r="C942" s="160"/>
+      <c r="D942" s="161"/>
+      <c r="E942" s="161"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -13218,9 +13218,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="162"/>
-      <c r="D959" s="163"/>
-      <c r="E959" s="163"/>
+      <c r="C959" s="160"/>
+      <c r="D959" s="161"/>
+      <c r="E959" s="161"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13371,9 +13371,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="162"/>
-      <c r="D976" s="163"/>
-      <c r="E976" s="163"/>
+      <c r="C976" s="160"/>
+      <c r="D976" s="161"/>
+      <c r="E976" s="161"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13524,9 +13524,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="162"/>
-      <c r="D993" s="163"/>
-      <c r="E993" s="163"/>
+      <c r="C993" s="160"/>
+      <c r="D993" s="161"/>
+      <c r="E993" s="161"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13677,9 +13677,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="162"/>
-      <c r="D1010" s="163"/>
-      <c r="E1010" s="163"/>
+      <c r="C1010" s="160"/>
+      <c r="D1010" s="161"/>
+      <c r="E1010" s="161"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13830,9 +13830,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="162"/>
-      <c r="D1027" s="163"/>
-      <c r="E1027" s="163"/>
+      <c r="C1027" s="160"/>
+      <c r="D1027" s="161"/>
+      <c r="E1027" s="161"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13983,9 +13983,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="162"/>
-      <c r="D1044" s="163"/>
-      <c r="E1044" s="163"/>
+      <c r="C1044" s="160"/>
+      <c r="D1044" s="161"/>
+      <c r="E1044" s="161"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -14136,9 +14136,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="162"/>
-      <c r="D1061" s="163"/>
-      <c r="E1061" s="163"/>
+      <c r="C1061" s="160"/>
+      <c r="D1061" s="161"/>
+      <c r="E1061" s="161"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14289,9 +14289,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="162"/>
-      <c r="D1078" s="163"/>
-      <c r="E1078" s="163"/>
+      <c r="C1078" s="160"/>
+      <c r="D1078" s="161"/>
+      <c r="E1078" s="161"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14442,18 +14442,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="172"/>
-      <c r="D1095" s="173"/>
-      <c r="E1095" s="173"/>
+      <c r="C1095" s="170"/>
+      <c r="D1095" s="171"/>
+      <c r="E1095" s="171"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="162"/>
-      <c r="D1096" s="163"/>
-      <c r="E1096" s="163"/>
+      <c r="C1096" s="160"/>
+      <c r="D1096" s="161"/>
+      <c r="E1096" s="161"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14604,9 +14604,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="164"/>
-      <c r="D1113" s="165"/>
-      <c r="E1113" s="165"/>
+      <c r="C1113" s="162"/>
+      <c r="D1113" s="163"/>
+      <c r="E1113" s="163"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14757,9 +14757,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="162"/>
-      <c r="D1130" s="163"/>
-      <c r="E1130" s="163"/>
+      <c r="C1130" s="160"/>
+      <c r="D1130" s="161"/>
+      <c r="E1130" s="161"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14910,9 +14910,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="162"/>
-      <c r="D1147" s="163"/>
-      <c r="E1147" s="163"/>
+      <c r="C1147" s="160"/>
+      <c r="D1147" s="161"/>
+      <c r="E1147" s="161"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -15063,9 +15063,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="162"/>
-      <c r="D1164" s="163"/>
-      <c r="E1164" s="163"/>
+      <c r="C1164" s="160"/>
+      <c r="D1164" s="161"/>
+      <c r="E1164" s="161"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -15216,9 +15216,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="162"/>
-      <c r="D1181" s="163"/>
-      <c r="E1181" s="163"/>
+      <c r="C1181" s="160"/>
+      <c r="D1181" s="161"/>
+      <c r="E1181" s="161"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15369,9 +15369,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="162"/>
-      <c r="D1198" s="163"/>
-      <c r="E1198" s="163"/>
+      <c r="C1198" s="160"/>
+      <c r="D1198" s="161"/>
+      <c r="E1198" s="161"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15522,9 +15522,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="162"/>
-      <c r="D1215" s="163"/>
-      <c r="E1215" s="163"/>
+      <c r="C1215" s="160"/>
+      <c r="D1215" s="161"/>
+      <c r="E1215" s="161"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15675,9 +15675,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="162"/>
-      <c r="D1232" s="163"/>
-      <c r="E1232" s="163"/>
+      <c r="C1232" s="160"/>
+      <c r="D1232" s="161"/>
+      <c r="E1232" s="161"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15828,9 +15828,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="162"/>
-      <c r="D1249" s="163"/>
-      <c r="E1249" s="163"/>
+      <c r="C1249" s="160"/>
+      <c r="D1249" s="161"/>
+      <c r="E1249" s="161"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15981,9 +15981,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="162"/>
-      <c r="D1266" s="163"/>
-      <c r="E1266" s="163"/>
+      <c r="C1266" s="160"/>
+      <c r="D1266" s="161"/>
+      <c r="E1266" s="161"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -16134,9 +16134,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="162"/>
-      <c r="D1283" s="163"/>
-      <c r="E1283" s="163"/>
+      <c r="C1283" s="160"/>
+      <c r="D1283" s="161"/>
+      <c r="E1283" s="161"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16287,9 +16287,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="162"/>
-      <c r="D1300" s="163"/>
-      <c r="E1300" s="163"/>
+      <c r="C1300" s="160"/>
+      <c r="D1300" s="161"/>
+      <c r="E1300" s="161"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16440,9 +16440,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="162"/>
-      <c r="D1317" s="163"/>
-      <c r="E1317" s="163"/>
+      <c r="C1317" s="160"/>
+      <c r="D1317" s="161"/>
+      <c r="E1317" s="161"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16593,9 +16593,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="162"/>
-      <c r="D1334" s="163"/>
-      <c r="E1334" s="163"/>
+      <c r="C1334" s="160"/>
+      <c r="D1334" s="161"/>
+      <c r="E1334" s="161"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16746,9 +16746,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="162"/>
-      <c r="D1351" s="163"/>
-      <c r="E1351" s="163"/>
+      <c r="C1351" s="160"/>
+      <c r="D1351" s="161"/>
+      <c r="E1351" s="161"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16899,18 +16899,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="174"/>
-      <c r="D1368" s="175"/>
-      <c r="E1368" s="175"/>
+      <c r="C1368" s="168"/>
+      <c r="D1368" s="169"/>
+      <c r="E1368" s="169"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="162"/>
-      <c r="D1369" s="163"/>
-      <c r="E1369" s="163"/>
+      <c r="C1369" s="160"/>
+      <c r="D1369" s="161"/>
+      <c r="E1369" s="161"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -17061,9 +17061,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="164"/>
-      <c r="D1386" s="165"/>
-      <c r="E1386" s="165"/>
+      <c r="C1386" s="162"/>
+      <c r="D1386" s="163"/>
+      <c r="E1386" s="163"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -17214,9 +17214,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="162"/>
-      <c r="D1403" s="163"/>
-      <c r="E1403" s="163"/>
+      <c r="C1403" s="160"/>
+      <c r="D1403" s="161"/>
+      <c r="E1403" s="161"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17367,9 +17367,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="162"/>
-      <c r="D1420" s="163"/>
-      <c r="E1420" s="163"/>
+      <c r="C1420" s="160"/>
+      <c r="D1420" s="161"/>
+      <c r="E1420" s="161"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17520,9 +17520,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="162"/>
-      <c r="D1437" s="163"/>
-      <c r="E1437" s="163"/>
+      <c r="C1437" s="160"/>
+      <c r="D1437" s="161"/>
+      <c r="E1437" s="161"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17673,9 +17673,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="162"/>
-      <c r="D1454" s="163"/>
-      <c r="E1454" s="163"/>
+      <c r="C1454" s="160"/>
+      <c r="D1454" s="161"/>
+      <c r="E1454" s="161"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17826,9 +17826,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="162"/>
-      <c r="D1471" s="163"/>
-      <c r="E1471" s="163"/>
+      <c r="C1471" s="160"/>
+      <c r="D1471" s="161"/>
+      <c r="E1471" s="161"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17979,9 +17979,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="162"/>
-      <c r="D1488" s="163"/>
-      <c r="E1488" s="163"/>
+      <c r="C1488" s="160"/>
+      <c r="D1488" s="161"/>
+      <c r="E1488" s="161"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -18132,9 +18132,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="162"/>
-      <c r="D1505" s="163"/>
-      <c r="E1505" s="163"/>
+      <c r="C1505" s="160"/>
+      <c r="D1505" s="161"/>
+      <c r="E1505" s="161"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18285,9 +18285,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="162"/>
-      <c r="D1522" s="163"/>
-      <c r="E1522" s="163"/>
+      <c r="C1522" s="160"/>
+      <c r="D1522" s="161"/>
+      <c r="E1522" s="161"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18438,9 +18438,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="162"/>
-      <c r="D1539" s="163"/>
-      <c r="E1539" s="163"/>
+      <c r="C1539" s="160"/>
+      <c r="D1539" s="161"/>
+      <c r="E1539" s="161"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18591,9 +18591,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="162"/>
-      <c r="D1556" s="163"/>
-      <c r="E1556" s="163"/>
+      <c r="C1556" s="160"/>
+      <c r="D1556" s="161"/>
+      <c r="E1556" s="161"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18744,9 +18744,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="162"/>
-      <c r="D1573" s="163"/>
-      <c r="E1573" s="163"/>
+      <c r="C1573" s="160"/>
+      <c r="D1573" s="161"/>
+      <c r="E1573" s="161"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18897,9 +18897,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="162"/>
-      <c r="D1590" s="163"/>
-      <c r="E1590" s="163"/>
+      <c r="C1590" s="160"/>
+      <c r="D1590" s="161"/>
+      <c r="E1590" s="161"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -19050,9 +19050,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="162"/>
-      <c r="D1607" s="163"/>
-      <c r="E1607" s="163"/>
+      <c r="C1607" s="160"/>
+      <c r="D1607" s="161"/>
+      <c r="E1607" s="161"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -19203,9 +19203,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="162"/>
-      <c r="D1624" s="163"/>
-      <c r="E1624" s="163"/>
+      <c r="C1624" s="160"/>
+      <c r="D1624" s="161"/>
+      <c r="E1624" s="161"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19356,18 +19356,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="176"/>
-      <c r="D1641" s="177"/>
-      <c r="E1641" s="177"/>
+      <c r="C1641" s="166"/>
+      <c r="D1641" s="167"/>
+      <c r="E1641" s="167"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="162"/>
-      <c r="D1642" s="163"/>
-      <c r="E1642" s="163"/>
+      <c r="C1642" s="160"/>
+      <c r="D1642" s="161"/>
+      <c r="E1642" s="161"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19518,9 +19518,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="164"/>
-      <c r="D1659" s="165"/>
-      <c r="E1659" s="165"/>
+      <c r="C1659" s="162"/>
+      <c r="D1659" s="163"/>
+      <c r="E1659" s="163"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19671,9 +19671,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="162"/>
-      <c r="D1676" s="163"/>
-      <c r="E1676" s="163"/>
+      <c r="C1676" s="160"/>
+      <c r="D1676" s="161"/>
+      <c r="E1676" s="161"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19824,9 +19824,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="162"/>
-      <c r="D1693" s="163"/>
-      <c r="E1693" s="163"/>
+      <c r="C1693" s="160"/>
+      <c r="D1693" s="161"/>
+      <c r="E1693" s="161"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19977,9 +19977,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="162"/>
-      <c r="D1710" s="163"/>
-      <c r="E1710" s="163"/>
+      <c r="C1710" s="160"/>
+      <c r="D1710" s="161"/>
+      <c r="E1710" s="161"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -20130,9 +20130,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="162"/>
-      <c r="D1727" s="163"/>
-      <c r="E1727" s="163"/>
+      <c r="C1727" s="160"/>
+      <c r="D1727" s="161"/>
+      <c r="E1727" s="161"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20283,9 +20283,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="162"/>
-      <c r="D1744" s="163"/>
-      <c r="E1744" s="163"/>
+      <c r="C1744" s="160"/>
+      <c r="D1744" s="161"/>
+      <c r="E1744" s="161"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20436,9 +20436,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="162"/>
-      <c r="D1761" s="163"/>
-      <c r="E1761" s="163"/>
+      <c r="C1761" s="160"/>
+      <c r="D1761" s="161"/>
+      <c r="E1761" s="161"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20589,9 +20589,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="162"/>
-      <c r="D1778" s="163"/>
-      <c r="E1778" s="163"/>
+      <c r="C1778" s="160"/>
+      <c r="D1778" s="161"/>
+      <c r="E1778" s="161"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20742,9 +20742,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="162"/>
-      <c r="D1795" s="163"/>
-      <c r="E1795" s="163"/>
+      <c r="C1795" s="160"/>
+      <c r="D1795" s="161"/>
+      <c r="E1795" s="161"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20895,9 +20895,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="162"/>
-      <c r="D1812" s="163"/>
-      <c r="E1812" s="163"/>
+      <c r="C1812" s="160"/>
+      <c r="D1812" s="161"/>
+      <c r="E1812" s="161"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -21048,9 +21048,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="162"/>
-      <c r="D1829" s="163"/>
-      <c r="E1829" s="163"/>
+      <c r="C1829" s="160"/>
+      <c r="D1829" s="161"/>
+      <c r="E1829" s="161"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -21201,9 +21201,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="162"/>
-      <c r="D1846" s="163"/>
-      <c r="E1846" s="163"/>
+      <c r="C1846" s="160"/>
+      <c r="D1846" s="161"/>
+      <c r="E1846" s="161"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21354,9 +21354,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="162"/>
-      <c r="D1863" s="163"/>
-      <c r="E1863" s="163"/>
+      <c r="C1863" s="160"/>
+      <c r="D1863" s="161"/>
+      <c r="E1863" s="161"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21507,9 +21507,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="162"/>
-      <c r="D1880" s="163"/>
-      <c r="E1880" s="163"/>
+      <c r="C1880" s="160"/>
+      <c r="D1880" s="161"/>
+      <c r="E1880" s="161"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21660,9 +21660,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="162"/>
-      <c r="D1897" s="163"/>
-      <c r="E1897" s="163"/>
+      <c r="C1897" s="160"/>
+      <c r="D1897" s="161"/>
+      <c r="E1897" s="161"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21813,18 +21813,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="178"/>
-      <c r="D1914" s="179"/>
-      <c r="E1914" s="179"/>
+      <c r="C1914" s="164"/>
+      <c r="D1914" s="165"/>
+      <c r="E1914" s="165"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="162"/>
-      <c r="D1915" s="163"/>
-      <c r="E1915" s="163"/>
+      <c r="C1915" s="160"/>
+      <c r="D1915" s="161"/>
+      <c r="E1915" s="161"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21975,9 +21975,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="164"/>
-      <c r="D1932" s="165"/>
-      <c r="E1932" s="165"/>
+      <c r="C1932" s="162"/>
+      <c r="D1932" s="163"/>
+      <c r="E1932" s="163"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -22128,9 +22128,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="162"/>
-      <c r="D1949" s="163"/>
-      <c r="E1949" s="163"/>
+      <c r="C1949" s="160"/>
+      <c r="D1949" s="161"/>
+      <c r="E1949" s="161"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22281,9 +22281,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="162"/>
-      <c r="D1966" s="163"/>
-      <c r="E1966" s="163"/>
+      <c r="C1966" s="160"/>
+      <c r="D1966" s="161"/>
+      <c r="E1966" s="161"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22434,9 +22434,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="162"/>
-      <c r="D1983" s="163"/>
-      <c r="E1983" s="163"/>
+      <c r="C1983" s="160"/>
+      <c r="D1983" s="161"/>
+      <c r="E1983" s="161"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22587,9 +22587,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="162"/>
-      <c r="D2000" s="163"/>
-      <c r="E2000" s="163"/>
+      <c r="C2000" s="160"/>
+      <c r="D2000" s="161"/>
+      <c r="E2000" s="161"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22740,9 +22740,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="162"/>
-      <c r="D2017" s="163"/>
-      <c r="E2017" s="163"/>
+      <c r="C2017" s="160"/>
+      <c r="D2017" s="161"/>
+      <c r="E2017" s="161"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22893,9 +22893,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="162"/>
-      <c r="D2034" s="163"/>
-      <c r="E2034" s="163"/>
+      <c r="C2034" s="160"/>
+      <c r="D2034" s="161"/>
+      <c r="E2034" s="161"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -23046,9 +23046,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="162"/>
-      <c r="D2051" s="163"/>
-      <c r="E2051" s="163"/>
+      <c r="C2051" s="160"/>
+      <c r="D2051" s="161"/>
+      <c r="E2051" s="161"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -23199,9 +23199,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="162"/>
-      <c r="D2068" s="163"/>
-      <c r="E2068" s="163"/>
+      <c r="C2068" s="160"/>
+      <c r="D2068" s="161"/>
+      <c r="E2068" s="161"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23352,9 +23352,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="162"/>
-      <c r="D2085" s="163"/>
-      <c r="E2085" s="163"/>
+      <c r="C2085" s="160"/>
+      <c r="D2085" s="161"/>
+      <c r="E2085" s="161"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23505,9 +23505,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="162"/>
-      <c r="D2102" s="163"/>
-      <c r="E2102" s="163"/>
+      <c r="C2102" s="160"/>
+      <c r="D2102" s="161"/>
+      <c r="E2102" s="161"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23658,9 +23658,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="162"/>
-      <c r="D2119" s="163"/>
-      <c r="E2119" s="163"/>
+      <c r="C2119" s="160"/>
+      <c r="D2119" s="161"/>
+      <c r="E2119" s="161"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23811,9 +23811,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="162"/>
-      <c r="D2136" s="163"/>
-      <c r="E2136" s="163"/>
+      <c r="C2136" s="160"/>
+      <c r="D2136" s="161"/>
+      <c r="E2136" s="161"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23964,9 +23964,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="162"/>
-      <c r="D2153" s="163"/>
-      <c r="E2153" s="163"/>
+      <c r="C2153" s="160"/>
+      <c r="D2153" s="161"/>
+      <c r="E2153" s="161"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -24117,9 +24117,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="162"/>
-      <c r="D2170" s="163"/>
-      <c r="E2170" s="163"/>
+      <c r="C2170" s="160"/>
+      <c r="D2170" s="161"/>
+      <c r="E2170" s="161"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -24267,15 +24267,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24288,122 +24395,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24430,51 +24430,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
-      <c r="I1" s="186"/>
-      <c r="J1" s="186"/>
-      <c r="K1" s="186"/>
-      <c r="L1" s="186"/>
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="187"/>
+      <c r="I1" s="187"/>
+      <c r="J1" s="187"/>
+      <c r="K1" s="187"/>
+      <c r="L1" s="187"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="184" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184"/>
-      <c r="L2" s="185"/>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="185"/>
+      <c r="K2" s="185"/>
+      <c r="L2" s="186"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="181" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="181"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="181"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="182"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="183"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -24691,19 +24691,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="180" t="s">
+      <c r="A20" s="181" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="181"/>
-      <c r="C20" s="181"/>
-      <c r="D20" s="181"/>
-      <c r="E20" s="181"/>
-      <c r="F20" s="181"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="181"/>
-      <c r="J20" s="181"/>
-      <c r="K20" s="182"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="182"/>
+      <c r="J20" s="182"/>
+      <c r="K20" s="183"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -24920,19 +24920,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="180" t="s">
+      <c r="A37" s="181" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="181"/>
-      <c r="C37" s="181"/>
-      <c r="D37" s="181"/>
-      <c r="E37" s="181"/>
-      <c r="F37" s="181"/>
-      <c r="G37" s="181"/>
-      <c r="H37" s="181"/>
-      <c r="I37" s="181"/>
-      <c r="J37" s="181"/>
-      <c r="K37" s="182"/>
+      <c r="B37" s="182"/>
+      <c r="C37" s="182"/>
+      <c r="D37" s="182"/>
+      <c r="E37" s="182"/>
+      <c r="F37" s="182"/>
+      <c r="G37" s="182"/>
+      <c r="H37" s="182"/>
+      <c r="I37" s="182"/>
+      <c r="J37" s="182"/>
+      <c r="K37" s="183"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -25190,28 +25190,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="187"/>
+      <c r="A3" s="188"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="188"/>
+      <c r="A4" s="189"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="188"/>
+      <c r="A5" s="189"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="188"/>
+      <c r="A6" s="189"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="188"/>
+      <c r="A7" s="189"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="188"/>
+      <c r="A8" s="189"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="188"/>
+      <c r="A9" s="189"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="189"/>
+      <c r="A10" s="190"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -25394,10 +25394,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="190" t="s">
+      <c r="B1" s="191" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="191"/>
+      <c r="C1" s="192"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25408,7 +25408,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="193" t="s">
         <v>213</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25422,7 +25422,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="193"/>
+      <c r="A4" s="194"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25434,7 +25434,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="193"/>
+      <c r="A5" s="194"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25443,7 +25443,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="193"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="139" t="s">
         <v>215</v>
       </c>
@@ -25455,7 +25455,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="193"/>
+      <c r="A7" s="194"/>
       <c r="B7" s="128" t="s">
         <v>178</v>
       </c>
@@ -25467,7 +25467,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="193"/>
+      <c r="A8" s="194"/>
       <c r="B8" s="128" t="s">
         <v>179</v>
       </c>
@@ -25476,7 +25476,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="194"/>
+      <c r="A9" s="195"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25491,7 +25491,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="192" t="s">
+      <c r="A11" s="193" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25505,7 +25505,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="193"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25517,7 +25517,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="193"/>
+      <c r="A13" s="194"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25526,7 +25526,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="193"/>
+      <c r="A14" s="194"/>
       <c r="B14" s="139" t="s">
         <v>215</v>
       </c>
@@ -25538,7 +25538,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="193"/>
+      <c r="A15" s="194"/>
       <c r="B15" s="128" t="s">
         <v>178</v>
       </c>
@@ -25550,7 +25550,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="193"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="128" t="s">
         <v>179</v>
       </c>
@@ -25559,7 +25559,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="194"/>
+      <c r="A17" s="195"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25574,7 +25574,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="192" t="s">
+      <c r="A19" s="193" t="s">
         <v>214</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25583,7 +25583,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="193"/>
+      <c r="A20" s="194"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25593,14 +25593,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="193"/>
+      <c r="A21" s="194"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="193"/>
+      <c r="A22" s="194"/>
       <c r="B22" s="139" t="s">
         <v>215</v>
       </c>
@@ -25610,7 +25610,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="193"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="128" t="s">
         <v>178</v>
       </c>
@@ -25620,14 +25620,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="193"/>
+      <c r="A24" s="194"/>
       <c r="B24" s="128" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="194"/>
+      <c r="A25" s="195"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25671,17 +25671,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="202" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="212"/>
+      <c r="B2" s="203"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="213" t="s">
+      <c r="A3" s="204" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="212"/>
+      <c r="B3" s="203"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -25697,115 +25697,128 @@
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="199" t="s">
+      <c r="A7" s="213" t="s">
         <v>197</v>
       </c>
-      <c r="B7" s="200"/>
+      <c r="B7" s="214"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="201" t="s">
+      <c r="A9" s="211" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="202"/>
+      <c r="B9" s="212"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="203"/>
-      <c r="B10" s="204"/>
+      <c r="A10" s="198"/>
+      <c r="B10" s="199"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="195" t="s">
+      <c r="A11" s="200" t="s">
         <v>199</v>
       </c>
-      <c r="B11" s="196"/>
+      <c r="B11" s="201"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="195" t="s">
+      <c r="A12" s="200" t="s">
         <v>200</v>
       </c>
-      <c r="B12" s="196"/>
+      <c r="B12" s="201"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="195" t="s">
+      <c r="A13" s="200" t="s">
         <v>201</v>
       </c>
-      <c r="B13" s="196"/>
+      <c r="B13" s="201"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="195" t="s">
+      <c r="A14" s="200" t="s">
         <v>202</v>
       </c>
-      <c r="B14" s="196"/>
+      <c r="B14" s="201"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="195" t="s">
+      <c r="A15" s="200" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="196"/>
+      <c r="B15" s="201"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="195" t="s">
+      <c r="A16" s="200" t="s">
         <v>204</v>
       </c>
-      <c r="B16" s="196"/>
+      <c r="B16" s="201"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="197" t="s">
+      <c r="A17" s="196" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="198"/>
+      <c r="B17" s="197"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="199" t="s">
+      <c r="A19" s="213" t="s">
         <v>208</v>
       </c>
-      <c r="B19" s="200"/>
+      <c r="B19" s="214"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="201" t="s">
+      <c r="A21" s="211" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="202"/>
+      <c r="B21" s="212"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="203"/>
-      <c r="B22" s="204"/>
+      <c r="A22" s="198"/>
+      <c r="B22" s="199"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="195" t="s">
+      <c r="A23" s="200" t="s">
         <v>210</v>
       </c>
-      <c r="B23" s="196"/>
+      <c r="B23" s="201"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="195"/>
-      <c r="B24" s="196"/>
+      <c r="A24" s="200"/>
+      <c r="B24" s="201"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="195" t="s">
+      <c r="A25" s="200" t="s">
         <v>211</v>
       </c>
-      <c r="B25" s="196"/>
+      <c r="B25" s="201"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="195" t="s">
+      <c r="A26" s="200" t="s">
         <v>212</v>
       </c>
-      <c r="B26" s="196"/>
+      <c r="B26" s="201"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="197"/>
-      <c r="B27" s="198"/>
+      <c r="A27" s="196"/>
+      <c r="B27" s="197"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25816,19 +25829,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Flintstones - up to the level 3 boss, about 1150 frames ahead
</commit_message>
<xml_diff>
--- a/Flintstones/Compare/Flintstones.xlsx
+++ b/Flintstones/Compare/Flintstones.xlsx
@@ -1991,29 +1991,29 @@
     <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2049,20 +2049,34 @@
     <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2072,20 +2086,6 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2404,7 +2404,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -3392,14 +3392,14 @@
         <v>225</v>
       </c>
       <c r="C67" s="101">
-        <v>16439</v>
+        <v>15639</v>
       </c>
       <c r="D67" s="101">
         <v>16490</v>
       </c>
       <c r="E67" s="123">
         <f t="shared" si="3"/>
-        <v>51</v>
+        <v>851</v>
       </c>
       <c r="F67" s="105"/>
     </row>
@@ -3443,14 +3443,14 @@
         <v>217</v>
       </c>
       <c r="C70" s="101">
-        <v>17213</v>
+        <v>16131</v>
       </c>
       <c r="D70" s="101">
         <v>17274</v>
       </c>
       <c r="E70" s="123">
         <f t="shared" si="3"/>
-        <v>61</v>
+        <v>1143</v>
       </c>
       <c r="F70" s="105"/>
     </row>
@@ -4533,6 +4533,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A144:A158"/>
+    <mergeCell ref="A110:A124"/>
+    <mergeCell ref="A76:A90"/>
+    <mergeCell ref="A127:A141"/>
+    <mergeCell ref="A93:A107"/>
     <mergeCell ref="A36:A54"/>
     <mergeCell ref="A57:A73"/>
     <mergeCell ref="C5:D5"/>
@@ -4541,11 +4546,6 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
-    <mergeCell ref="A144:A158"/>
-    <mergeCell ref="A110:A124"/>
-    <mergeCell ref="A76:A90"/>
-    <mergeCell ref="A127:A141"/>
-    <mergeCell ref="A93:A107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4577,13 +4577,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4613,18 +4613,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="164"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4776,9 +4776,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="162"/>
-      <c r="D21" s="163"/>
-      <c r="E21" s="163"/>
+      <c r="C21" s="165"/>
+      <c r="D21" s="166"/>
+      <c r="E21" s="166"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4929,9 +4929,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="160"/>
-      <c r="D38" s="161"/>
-      <c r="E38" s="161"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="164"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -5082,9 +5082,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="160"/>
-      <c r="D55" s="161"/>
-      <c r="E55" s="161"/>
+      <c r="C55" s="163"/>
+      <c r="D55" s="164"/>
+      <c r="E55" s="164"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -5235,9 +5235,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="160"/>
-      <c r="D72" s="161"/>
-      <c r="E72" s="161"/>
+      <c r="C72" s="163"/>
+      <c r="D72" s="164"/>
+      <c r="E72" s="164"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5388,9 +5388,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="160"/>
-      <c r="D89" s="161"/>
-      <c r="E89" s="161"/>
+      <c r="C89" s="163"/>
+      <c r="D89" s="164"/>
+      <c r="E89" s="164"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5541,9 +5541,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="160"/>
-      <c r="D106" s="161"/>
-      <c r="E106" s="161"/>
+      <c r="C106" s="163"/>
+      <c r="D106" s="164"/>
+      <c r="E106" s="164"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5694,9 +5694,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="160"/>
-      <c r="D123" s="161"/>
-      <c r="E123" s="161"/>
+      <c r="C123" s="163"/>
+      <c r="D123" s="164"/>
+      <c r="E123" s="164"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5847,9 +5847,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="160"/>
-      <c r="D140" s="161"/>
-      <c r="E140" s="161"/>
+      <c r="C140" s="163"/>
+      <c r="D140" s="164"/>
+      <c r="E140" s="164"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -6000,9 +6000,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="160"/>
-      <c r="D157" s="161"/>
-      <c r="E157" s="161"/>
+      <c r="C157" s="163"/>
+      <c r="D157" s="164"/>
+      <c r="E157" s="164"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -6153,9 +6153,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="160"/>
-      <c r="D174" s="161"/>
-      <c r="E174" s="161"/>
+      <c r="C174" s="163"/>
+      <c r="D174" s="164"/>
+      <c r="E174" s="164"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6306,9 +6306,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="160"/>
-      <c r="D191" s="161"/>
-      <c r="E191" s="161"/>
+      <c r="C191" s="163"/>
+      <c r="D191" s="164"/>
+      <c r="E191" s="164"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6459,9 +6459,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="160"/>
-      <c r="D208" s="161"/>
-      <c r="E208" s="161"/>
+      <c r="C208" s="163"/>
+      <c r="D208" s="164"/>
+      <c r="E208" s="164"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6612,9 +6612,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="160"/>
-      <c r="D225" s="161"/>
-      <c r="E225" s="161"/>
+      <c r="C225" s="163"/>
+      <c r="D225" s="164"/>
+      <c r="E225" s="164"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6765,9 +6765,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="160"/>
-      <c r="D242" s="161"/>
-      <c r="E242" s="161"/>
+      <c r="C242" s="163"/>
+      <c r="D242" s="164"/>
+      <c r="E242" s="164"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6918,9 +6918,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="160"/>
-      <c r="D259" s="161"/>
-      <c r="E259" s="161"/>
+      <c r="C259" s="163"/>
+      <c r="D259" s="164"/>
+      <c r="E259" s="164"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -7071,18 +7071,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="176"/>
-      <c r="D276" s="177"/>
-      <c r="E276" s="177"/>
+      <c r="C276" s="167"/>
+      <c r="D276" s="168"/>
+      <c r="E276" s="168"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="160"/>
-      <c r="D277" s="161"/>
-      <c r="E277" s="161"/>
+      <c r="C277" s="163"/>
+      <c r="D277" s="164"/>
+      <c r="E277" s="164"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -7233,9 +7233,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="162"/>
-      <c r="D294" s="163"/>
-      <c r="E294" s="163"/>
+      <c r="C294" s="165"/>
+      <c r="D294" s="166"/>
+      <c r="E294" s="166"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7386,9 +7386,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="160"/>
-      <c r="D311" s="161"/>
-      <c r="E311" s="161"/>
+      <c r="C311" s="163"/>
+      <c r="D311" s="164"/>
+      <c r="E311" s="164"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7539,9 +7539,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="160"/>
-      <c r="D328" s="161"/>
-      <c r="E328" s="161"/>
+      <c r="C328" s="163"/>
+      <c r="D328" s="164"/>
+      <c r="E328" s="164"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7692,9 +7692,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="160"/>
-      <c r="D345" s="161"/>
-      <c r="E345" s="161"/>
+      <c r="C345" s="163"/>
+      <c r="D345" s="164"/>
+      <c r="E345" s="164"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7845,9 +7845,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="160"/>
-      <c r="D362" s="161"/>
-      <c r="E362" s="161"/>
+      <c r="C362" s="163"/>
+      <c r="D362" s="164"/>
+      <c r="E362" s="164"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7998,9 +7998,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="160"/>
-      <c r="D379" s="161"/>
-      <c r="E379" s="161"/>
+      <c r="C379" s="163"/>
+      <c r="D379" s="164"/>
+      <c r="E379" s="164"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -8151,9 +8151,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="160"/>
-      <c r="D396" s="161"/>
-      <c r="E396" s="161"/>
+      <c r="C396" s="163"/>
+      <c r="D396" s="164"/>
+      <c r="E396" s="164"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8304,9 +8304,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="160"/>
-      <c r="D413" s="161"/>
-      <c r="E413" s="161"/>
+      <c r="C413" s="163"/>
+      <c r="D413" s="164"/>
+      <c r="E413" s="164"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8457,9 +8457,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="160"/>
-      <c r="D430" s="161"/>
-      <c r="E430" s="161"/>
+      <c r="C430" s="163"/>
+      <c r="D430" s="164"/>
+      <c r="E430" s="164"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8610,9 +8610,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="160"/>
-      <c r="D447" s="161"/>
-      <c r="E447" s="161"/>
+      <c r="C447" s="163"/>
+      <c r="D447" s="164"/>
+      <c r="E447" s="164"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8763,9 +8763,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="160"/>
-      <c r="D464" s="161"/>
-      <c r="E464" s="161"/>
+      <c r="C464" s="163"/>
+      <c r="D464" s="164"/>
+      <c r="E464" s="164"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8916,9 +8916,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="160"/>
-      <c r="D481" s="161"/>
-      <c r="E481" s="161"/>
+      <c r="C481" s="163"/>
+      <c r="D481" s="164"/>
+      <c r="E481" s="164"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -9069,9 +9069,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="160"/>
-      <c r="D498" s="161"/>
-      <c r="E498" s="161"/>
+      <c r="C498" s="163"/>
+      <c r="D498" s="164"/>
+      <c r="E498" s="164"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -9222,9 +9222,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="160"/>
-      <c r="D515" s="161"/>
-      <c r="E515" s="161"/>
+      <c r="C515" s="163"/>
+      <c r="D515" s="164"/>
+      <c r="E515" s="164"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9375,9 +9375,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="160"/>
-      <c r="D532" s="161"/>
-      <c r="E532" s="161"/>
+      <c r="C532" s="163"/>
+      <c r="D532" s="164"/>
+      <c r="E532" s="164"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9528,18 +9528,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="174"/>
-      <c r="D549" s="175"/>
-      <c r="E549" s="175"/>
+      <c r="C549" s="169"/>
+      <c r="D549" s="170"/>
+      <c r="E549" s="170"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="160"/>
-      <c r="D550" s="161"/>
-      <c r="E550" s="161"/>
+      <c r="C550" s="163"/>
+      <c r="D550" s="164"/>
+      <c r="E550" s="164"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9690,9 +9690,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="162"/>
-      <c r="D567" s="163"/>
-      <c r="E567" s="163"/>
+      <c r="C567" s="165"/>
+      <c r="D567" s="166"/>
+      <c r="E567" s="166"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9843,9 +9843,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="160"/>
-      <c r="D584" s="161"/>
-      <c r="E584" s="161"/>
+      <c r="C584" s="163"/>
+      <c r="D584" s="164"/>
+      <c r="E584" s="164"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9996,9 +9996,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="160"/>
-      <c r="D601" s="161"/>
-      <c r="E601" s="161"/>
+      <c r="C601" s="163"/>
+      <c r="D601" s="164"/>
+      <c r="E601" s="164"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -10149,9 +10149,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="160"/>
-      <c r="D618" s="161"/>
-      <c r="E618" s="161"/>
+      <c r="C618" s="163"/>
+      <c r="D618" s="164"/>
+      <c r="E618" s="164"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10302,9 +10302,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="160"/>
-      <c r="D635" s="161"/>
-      <c r="E635" s="161"/>
+      <c r="C635" s="163"/>
+      <c r="D635" s="164"/>
+      <c r="E635" s="164"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10455,9 +10455,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="160"/>
-      <c r="D652" s="161"/>
-      <c r="E652" s="161"/>
+      <c r="C652" s="163"/>
+      <c r="D652" s="164"/>
+      <c r="E652" s="164"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10608,9 +10608,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="160"/>
-      <c r="D669" s="161"/>
-      <c r="E669" s="161"/>
+      <c r="C669" s="163"/>
+      <c r="D669" s="164"/>
+      <c r="E669" s="164"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10761,9 +10761,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="160"/>
-      <c r="D686" s="161"/>
-      <c r="E686" s="161"/>
+      <c r="C686" s="163"/>
+      <c r="D686" s="164"/>
+      <c r="E686" s="164"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10914,9 +10914,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="160"/>
-      <c r="D703" s="161"/>
-      <c r="E703" s="161"/>
+      <c r="C703" s="163"/>
+      <c r="D703" s="164"/>
+      <c r="E703" s="164"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -11067,9 +11067,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="160"/>
-      <c r="D720" s="161"/>
-      <c r="E720" s="161"/>
+      <c r="C720" s="163"/>
+      <c r="D720" s="164"/>
+      <c r="E720" s="164"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -11220,9 +11220,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="160"/>
-      <c r="D737" s="161"/>
-      <c r="E737" s="161"/>
+      <c r="C737" s="163"/>
+      <c r="D737" s="164"/>
+      <c r="E737" s="164"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11373,9 +11373,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="160"/>
-      <c r="D754" s="161"/>
-      <c r="E754" s="161"/>
+      <c r="C754" s="163"/>
+      <c r="D754" s="164"/>
+      <c r="E754" s="164"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11526,9 +11526,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="160"/>
-      <c r="D771" s="161"/>
-      <c r="E771" s="161"/>
+      <c r="C771" s="163"/>
+      <c r="D771" s="164"/>
+      <c r="E771" s="164"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11679,9 +11679,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="160"/>
-      <c r="D788" s="161"/>
-      <c r="E788" s="161"/>
+      <c r="C788" s="163"/>
+      <c r="D788" s="164"/>
+      <c r="E788" s="164"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11832,9 +11832,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="160"/>
-      <c r="D805" s="161"/>
-      <c r="E805" s="161"/>
+      <c r="C805" s="163"/>
+      <c r="D805" s="164"/>
+      <c r="E805" s="164"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11985,18 +11985,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="172"/>
-      <c r="D822" s="173"/>
-      <c r="E822" s="173"/>
+      <c r="C822" s="171"/>
+      <c r="D822" s="172"/>
+      <c r="E822" s="172"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="160"/>
-      <c r="D823" s="161"/>
-      <c r="E823" s="161"/>
+      <c r="C823" s="163"/>
+      <c r="D823" s="164"/>
+      <c r="E823" s="164"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -12147,9 +12147,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="162"/>
-      <c r="D840" s="163"/>
-      <c r="E840" s="163"/>
+      <c r="C840" s="165"/>
+      <c r="D840" s="166"/>
+      <c r="E840" s="166"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12300,9 +12300,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="160"/>
-      <c r="D857" s="161"/>
-      <c r="E857" s="161"/>
+      <c r="C857" s="163"/>
+      <c r="D857" s="164"/>
+      <c r="E857" s="164"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12453,9 +12453,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="160"/>
-      <c r="D874" s="161"/>
-      <c r="E874" s="161"/>
+      <c r="C874" s="163"/>
+      <c r="D874" s="164"/>
+      <c r="E874" s="164"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12606,9 +12606,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="160"/>
-      <c r="D891" s="161"/>
-      <c r="E891" s="161"/>
+      <c r="C891" s="163"/>
+      <c r="D891" s="164"/>
+      <c r="E891" s="164"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12759,9 +12759,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="160"/>
-      <c r="D908" s="161"/>
-      <c r="E908" s="161"/>
+      <c r="C908" s="163"/>
+      <c r="D908" s="164"/>
+      <c r="E908" s="164"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12912,9 +12912,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="160"/>
-      <c r="D925" s="161"/>
-      <c r="E925" s="161"/>
+      <c r="C925" s="163"/>
+      <c r="D925" s="164"/>
+      <c r="E925" s="164"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -13065,9 +13065,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="160"/>
-      <c r="D942" s="161"/>
-      <c r="E942" s="161"/>
+      <c r="C942" s="163"/>
+      <c r="D942" s="164"/>
+      <c r="E942" s="164"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -13218,9 +13218,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="160"/>
-      <c r="D959" s="161"/>
-      <c r="E959" s="161"/>
+      <c r="C959" s="163"/>
+      <c r="D959" s="164"/>
+      <c r="E959" s="164"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13371,9 +13371,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="160"/>
-      <c r="D976" s="161"/>
-      <c r="E976" s="161"/>
+      <c r="C976" s="163"/>
+      <c r="D976" s="164"/>
+      <c r="E976" s="164"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13524,9 +13524,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="160"/>
-      <c r="D993" s="161"/>
-      <c r="E993" s="161"/>
+      <c r="C993" s="163"/>
+      <c r="D993" s="164"/>
+      <c r="E993" s="164"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13677,9 +13677,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="160"/>
-      <c r="D1010" s="161"/>
-      <c r="E1010" s="161"/>
+      <c r="C1010" s="163"/>
+      <c r="D1010" s="164"/>
+      <c r="E1010" s="164"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13830,9 +13830,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="160"/>
-      <c r="D1027" s="161"/>
-      <c r="E1027" s="161"/>
+      <c r="C1027" s="163"/>
+      <c r="D1027" s="164"/>
+      <c r="E1027" s="164"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13983,9 +13983,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="160"/>
-      <c r="D1044" s="161"/>
-      <c r="E1044" s="161"/>
+      <c r="C1044" s="163"/>
+      <c r="D1044" s="164"/>
+      <c r="E1044" s="164"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -14136,9 +14136,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="160"/>
-      <c r="D1061" s="161"/>
-      <c r="E1061" s="161"/>
+      <c r="C1061" s="163"/>
+      <c r="D1061" s="164"/>
+      <c r="E1061" s="164"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14289,9 +14289,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="160"/>
-      <c r="D1078" s="161"/>
-      <c r="E1078" s="161"/>
+      <c r="C1078" s="163"/>
+      <c r="D1078" s="164"/>
+      <c r="E1078" s="164"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14442,18 +14442,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="170"/>
-      <c r="D1095" s="171"/>
-      <c r="E1095" s="171"/>
+      <c r="C1095" s="173"/>
+      <c r="D1095" s="174"/>
+      <c r="E1095" s="174"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="160"/>
-      <c r="D1096" s="161"/>
-      <c r="E1096" s="161"/>
+      <c r="C1096" s="163"/>
+      <c r="D1096" s="164"/>
+      <c r="E1096" s="164"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14604,9 +14604,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="162"/>
-      <c r="D1113" s="163"/>
-      <c r="E1113" s="163"/>
+      <c r="C1113" s="165"/>
+      <c r="D1113" s="166"/>
+      <c r="E1113" s="166"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14757,9 +14757,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="160"/>
-      <c r="D1130" s="161"/>
-      <c r="E1130" s="161"/>
+      <c r="C1130" s="163"/>
+      <c r="D1130" s="164"/>
+      <c r="E1130" s="164"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14910,9 +14910,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="160"/>
-      <c r="D1147" s="161"/>
-      <c r="E1147" s="161"/>
+      <c r="C1147" s="163"/>
+      <c r="D1147" s="164"/>
+      <c r="E1147" s="164"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -15063,9 +15063,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="160"/>
-      <c r="D1164" s="161"/>
-      <c r="E1164" s="161"/>
+      <c r="C1164" s="163"/>
+      <c r="D1164" s="164"/>
+      <c r="E1164" s="164"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -15216,9 +15216,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="160"/>
-      <c r="D1181" s="161"/>
-      <c r="E1181" s="161"/>
+      <c r="C1181" s="163"/>
+      <c r="D1181" s="164"/>
+      <c r="E1181" s="164"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15369,9 +15369,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="160"/>
-      <c r="D1198" s="161"/>
-      <c r="E1198" s="161"/>
+      <c r="C1198" s="163"/>
+      <c r="D1198" s="164"/>
+      <c r="E1198" s="164"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15522,9 +15522,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="160"/>
-      <c r="D1215" s="161"/>
-      <c r="E1215" s="161"/>
+      <c r="C1215" s="163"/>
+      <c r="D1215" s="164"/>
+      <c r="E1215" s="164"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15675,9 +15675,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="160"/>
-      <c r="D1232" s="161"/>
-      <c r="E1232" s="161"/>
+      <c r="C1232" s="163"/>
+      <c r="D1232" s="164"/>
+      <c r="E1232" s="164"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15828,9 +15828,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="160"/>
-      <c r="D1249" s="161"/>
-      <c r="E1249" s="161"/>
+      <c r="C1249" s="163"/>
+      <c r="D1249" s="164"/>
+      <c r="E1249" s="164"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15981,9 +15981,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="160"/>
-      <c r="D1266" s="161"/>
-      <c r="E1266" s="161"/>
+      <c r="C1266" s="163"/>
+      <c r="D1266" s="164"/>
+      <c r="E1266" s="164"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -16134,9 +16134,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="160"/>
-      <c r="D1283" s="161"/>
-      <c r="E1283" s="161"/>
+      <c r="C1283" s="163"/>
+      <c r="D1283" s="164"/>
+      <c r="E1283" s="164"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16287,9 +16287,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="160"/>
-      <c r="D1300" s="161"/>
-      <c r="E1300" s="161"/>
+      <c r="C1300" s="163"/>
+      <c r="D1300" s="164"/>
+      <c r="E1300" s="164"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16440,9 +16440,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="160"/>
-      <c r="D1317" s="161"/>
-      <c r="E1317" s="161"/>
+      <c r="C1317" s="163"/>
+      <c r="D1317" s="164"/>
+      <c r="E1317" s="164"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16593,9 +16593,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="160"/>
-      <c r="D1334" s="161"/>
-      <c r="E1334" s="161"/>
+      <c r="C1334" s="163"/>
+      <c r="D1334" s="164"/>
+      <c r="E1334" s="164"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16746,9 +16746,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="160"/>
-      <c r="D1351" s="161"/>
-      <c r="E1351" s="161"/>
+      <c r="C1351" s="163"/>
+      <c r="D1351" s="164"/>
+      <c r="E1351" s="164"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16899,18 +16899,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="168"/>
-      <c r="D1368" s="169"/>
-      <c r="E1368" s="169"/>
+      <c r="C1368" s="175"/>
+      <c r="D1368" s="176"/>
+      <c r="E1368" s="176"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="160"/>
-      <c r="D1369" s="161"/>
-      <c r="E1369" s="161"/>
+      <c r="C1369" s="163"/>
+      <c r="D1369" s="164"/>
+      <c r="E1369" s="164"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -17061,9 +17061,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="162"/>
-      <c r="D1386" s="163"/>
-      <c r="E1386" s="163"/>
+      <c r="C1386" s="165"/>
+      <c r="D1386" s="166"/>
+      <c r="E1386" s="166"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -17214,9 +17214,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="160"/>
-      <c r="D1403" s="161"/>
-      <c r="E1403" s="161"/>
+      <c r="C1403" s="163"/>
+      <c r="D1403" s="164"/>
+      <c r="E1403" s="164"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17367,9 +17367,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="160"/>
-      <c r="D1420" s="161"/>
-      <c r="E1420" s="161"/>
+      <c r="C1420" s="163"/>
+      <c r="D1420" s="164"/>
+      <c r="E1420" s="164"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17520,9 +17520,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="160"/>
-      <c r="D1437" s="161"/>
-      <c r="E1437" s="161"/>
+      <c r="C1437" s="163"/>
+      <c r="D1437" s="164"/>
+      <c r="E1437" s="164"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17673,9 +17673,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="160"/>
-      <c r="D1454" s="161"/>
-      <c r="E1454" s="161"/>
+      <c r="C1454" s="163"/>
+      <c r="D1454" s="164"/>
+      <c r="E1454" s="164"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17826,9 +17826,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="160"/>
-      <c r="D1471" s="161"/>
-      <c r="E1471" s="161"/>
+      <c r="C1471" s="163"/>
+      <c r="D1471" s="164"/>
+      <c r="E1471" s="164"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17979,9 +17979,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="160"/>
-      <c r="D1488" s="161"/>
-      <c r="E1488" s="161"/>
+      <c r="C1488" s="163"/>
+      <c r="D1488" s="164"/>
+      <c r="E1488" s="164"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -18132,9 +18132,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="160"/>
-      <c r="D1505" s="161"/>
-      <c r="E1505" s="161"/>
+      <c r="C1505" s="163"/>
+      <c r="D1505" s="164"/>
+      <c r="E1505" s="164"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18285,9 +18285,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="160"/>
-      <c r="D1522" s="161"/>
-      <c r="E1522" s="161"/>
+      <c r="C1522" s="163"/>
+      <c r="D1522" s="164"/>
+      <c r="E1522" s="164"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18438,9 +18438,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="160"/>
-      <c r="D1539" s="161"/>
-      <c r="E1539" s="161"/>
+      <c r="C1539" s="163"/>
+      <c r="D1539" s="164"/>
+      <c r="E1539" s="164"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18591,9 +18591,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="160"/>
-      <c r="D1556" s="161"/>
-      <c r="E1556" s="161"/>
+      <c r="C1556" s="163"/>
+      <c r="D1556" s="164"/>
+      <c r="E1556" s="164"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18744,9 +18744,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="160"/>
-      <c r="D1573" s="161"/>
-      <c r="E1573" s="161"/>
+      <c r="C1573" s="163"/>
+      <c r="D1573" s="164"/>
+      <c r="E1573" s="164"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18897,9 +18897,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="160"/>
-      <c r="D1590" s="161"/>
-      <c r="E1590" s="161"/>
+      <c r="C1590" s="163"/>
+      <c r="D1590" s="164"/>
+      <c r="E1590" s="164"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -19050,9 +19050,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="160"/>
-      <c r="D1607" s="161"/>
-      <c r="E1607" s="161"/>
+      <c r="C1607" s="163"/>
+      <c r="D1607" s="164"/>
+      <c r="E1607" s="164"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -19203,9 +19203,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="160"/>
-      <c r="D1624" s="161"/>
-      <c r="E1624" s="161"/>
+      <c r="C1624" s="163"/>
+      <c r="D1624" s="164"/>
+      <c r="E1624" s="164"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19356,18 +19356,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="166"/>
-      <c r="D1641" s="167"/>
-      <c r="E1641" s="167"/>
+      <c r="C1641" s="177"/>
+      <c r="D1641" s="178"/>
+      <c r="E1641" s="178"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="160"/>
-      <c r="D1642" s="161"/>
-      <c r="E1642" s="161"/>
+      <c r="C1642" s="163"/>
+      <c r="D1642" s="164"/>
+      <c r="E1642" s="164"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19518,9 +19518,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="162"/>
-      <c r="D1659" s="163"/>
-      <c r="E1659" s="163"/>
+      <c r="C1659" s="165"/>
+      <c r="D1659" s="166"/>
+      <c r="E1659" s="166"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19671,9 +19671,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="160"/>
-      <c r="D1676" s="161"/>
-      <c r="E1676" s="161"/>
+      <c r="C1676" s="163"/>
+      <c r="D1676" s="164"/>
+      <c r="E1676" s="164"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19824,9 +19824,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="160"/>
-      <c r="D1693" s="161"/>
-      <c r="E1693" s="161"/>
+      <c r="C1693" s="163"/>
+      <c r="D1693" s="164"/>
+      <c r="E1693" s="164"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19977,9 +19977,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="160"/>
-      <c r="D1710" s="161"/>
-      <c r="E1710" s="161"/>
+      <c r="C1710" s="163"/>
+      <c r="D1710" s="164"/>
+      <c r="E1710" s="164"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -20130,9 +20130,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="160"/>
-      <c r="D1727" s="161"/>
-      <c r="E1727" s="161"/>
+      <c r="C1727" s="163"/>
+      <c r="D1727" s="164"/>
+      <c r="E1727" s="164"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20283,9 +20283,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="160"/>
-      <c r="D1744" s="161"/>
-      <c r="E1744" s="161"/>
+      <c r="C1744" s="163"/>
+      <c r="D1744" s="164"/>
+      <c r="E1744" s="164"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20436,9 +20436,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="160"/>
-      <c r="D1761" s="161"/>
-      <c r="E1761" s="161"/>
+      <c r="C1761" s="163"/>
+      <c r="D1761" s="164"/>
+      <c r="E1761" s="164"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20589,9 +20589,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="160"/>
-      <c r="D1778" s="161"/>
-      <c r="E1778" s="161"/>
+      <c r="C1778" s="163"/>
+      <c r="D1778" s="164"/>
+      <c r="E1778" s="164"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20742,9 +20742,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="160"/>
-      <c r="D1795" s="161"/>
-      <c r="E1795" s="161"/>
+      <c r="C1795" s="163"/>
+      <c r="D1795" s="164"/>
+      <c r="E1795" s="164"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20895,9 +20895,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="160"/>
-      <c r="D1812" s="161"/>
-      <c r="E1812" s="161"/>
+      <c r="C1812" s="163"/>
+      <c r="D1812" s="164"/>
+      <c r="E1812" s="164"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -21048,9 +21048,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="160"/>
-      <c r="D1829" s="161"/>
-      <c r="E1829" s="161"/>
+      <c r="C1829" s="163"/>
+      <c r="D1829" s="164"/>
+      <c r="E1829" s="164"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -21201,9 +21201,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="160"/>
-      <c r="D1846" s="161"/>
-      <c r="E1846" s="161"/>
+      <c r="C1846" s="163"/>
+      <c r="D1846" s="164"/>
+      <c r="E1846" s="164"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21354,9 +21354,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="160"/>
-      <c r="D1863" s="161"/>
-      <c r="E1863" s="161"/>
+      <c r="C1863" s="163"/>
+      <c r="D1863" s="164"/>
+      <c r="E1863" s="164"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21507,9 +21507,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="160"/>
-      <c r="D1880" s="161"/>
-      <c r="E1880" s="161"/>
+      <c r="C1880" s="163"/>
+      <c r="D1880" s="164"/>
+      <c r="E1880" s="164"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21660,9 +21660,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="160"/>
-      <c r="D1897" s="161"/>
-      <c r="E1897" s="161"/>
+      <c r="C1897" s="163"/>
+      <c r="D1897" s="164"/>
+      <c r="E1897" s="164"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21813,18 +21813,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="164"/>
-      <c r="D1914" s="165"/>
-      <c r="E1914" s="165"/>
+      <c r="C1914" s="179"/>
+      <c r="D1914" s="180"/>
+      <c r="E1914" s="180"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="160"/>
-      <c r="D1915" s="161"/>
-      <c r="E1915" s="161"/>
+      <c r="C1915" s="163"/>
+      <c r="D1915" s="164"/>
+      <c r="E1915" s="164"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21975,9 +21975,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="162"/>
-      <c r="D1932" s="163"/>
-      <c r="E1932" s="163"/>
+      <c r="C1932" s="165"/>
+      <c r="D1932" s="166"/>
+      <c r="E1932" s="166"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -22128,9 +22128,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="160"/>
-      <c r="D1949" s="161"/>
-      <c r="E1949" s="161"/>
+      <c r="C1949" s="163"/>
+      <c r="D1949" s="164"/>
+      <c r="E1949" s="164"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22281,9 +22281,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="160"/>
-      <c r="D1966" s="161"/>
-      <c r="E1966" s="161"/>
+      <c r="C1966" s="163"/>
+      <c r="D1966" s="164"/>
+      <c r="E1966" s="164"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22434,9 +22434,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="160"/>
-      <c r="D1983" s="161"/>
-      <c r="E1983" s="161"/>
+      <c r="C1983" s="163"/>
+      <c r="D1983" s="164"/>
+      <c r="E1983" s="164"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22587,9 +22587,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="160"/>
-      <c r="D2000" s="161"/>
-      <c r="E2000" s="161"/>
+      <c r="C2000" s="163"/>
+      <c r="D2000" s="164"/>
+      <c r="E2000" s="164"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22740,9 +22740,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="160"/>
-      <c r="D2017" s="161"/>
-      <c r="E2017" s="161"/>
+      <c r="C2017" s="163"/>
+      <c r="D2017" s="164"/>
+      <c r="E2017" s="164"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22893,9 +22893,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="160"/>
-      <c r="D2034" s="161"/>
-      <c r="E2034" s="161"/>
+      <c r="C2034" s="163"/>
+      <c r="D2034" s="164"/>
+      <c r="E2034" s="164"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -23046,9 +23046,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="160"/>
-      <c r="D2051" s="161"/>
-      <c r="E2051" s="161"/>
+      <c r="C2051" s="163"/>
+      <c r="D2051" s="164"/>
+      <c r="E2051" s="164"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -23199,9 +23199,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="160"/>
-      <c r="D2068" s="161"/>
-      <c r="E2068" s="161"/>
+      <c r="C2068" s="163"/>
+      <c r="D2068" s="164"/>
+      <c r="E2068" s="164"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23352,9 +23352,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="160"/>
-      <c r="D2085" s="161"/>
-      <c r="E2085" s="161"/>
+      <c r="C2085" s="163"/>
+      <c r="D2085" s="164"/>
+      <c r="E2085" s="164"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23505,9 +23505,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="160"/>
-      <c r="D2102" s="161"/>
-      <c r="E2102" s="161"/>
+      <c r="C2102" s="163"/>
+      <c r="D2102" s="164"/>
+      <c r="E2102" s="164"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23658,9 +23658,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="160"/>
-      <c r="D2119" s="161"/>
-      <c r="E2119" s="161"/>
+      <c r="C2119" s="163"/>
+      <c r="D2119" s="164"/>
+      <c r="E2119" s="164"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23811,9 +23811,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="160"/>
-      <c r="D2136" s="161"/>
-      <c r="E2136" s="161"/>
+      <c r="C2136" s="163"/>
+      <c r="D2136" s="164"/>
+      <c r="E2136" s="164"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23964,9 +23964,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="160"/>
-      <c r="D2153" s="161"/>
-      <c r="E2153" s="161"/>
+      <c r="C2153" s="163"/>
+      <c r="D2153" s="164"/>
+      <c r="E2153" s="164"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -24117,9 +24117,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="160"/>
-      <c r="D2170" s="161"/>
-      <c r="E2170" s="161"/>
+      <c r="C2170" s="163"/>
+      <c r="D2170" s="164"/>
+      <c r="E2170" s="164"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -24267,26 +24267,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24299,111 +24384,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25662,163 +25662,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="205" t="s">
+      <c r="A1" s="206" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="206"/>
+      <c r="B1" s="207"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="202" t="s">
+      <c r="A2" s="212" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="203"/>
+      <c r="B2" s="213"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="204" t="s">
+      <c r="A3" s="214" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="203"/>
+      <c r="B3" s="213"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="209"/>
-      <c r="B4" s="210"/>
+      <c r="A4" s="210"/>
+      <c r="B4" s="211"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="207" t="s">
+      <c r="A5" s="208" t="s">
         <v>205</v>
       </c>
-      <c r="B5" s="208"/>
+      <c r="B5" s="209"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="213" t="s">
+      <c r="A7" s="200" t="s">
         <v>197</v>
       </c>
-      <c r="B7" s="214"/>
+      <c r="B7" s="201"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="211" t="s">
+      <c r="A9" s="202" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="212"/>
+      <c r="B9" s="203"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="198"/>
-      <c r="B10" s="199"/>
+      <c r="A10" s="204"/>
+      <c r="B10" s="205"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="200" t="s">
+      <c r="A11" s="196" t="s">
         <v>199</v>
       </c>
-      <c r="B11" s="201"/>
+      <c r="B11" s="197"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="200" t="s">
+      <c r="A12" s="196" t="s">
         <v>200</v>
       </c>
-      <c r="B12" s="201"/>
+      <c r="B12" s="197"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="200" t="s">
+      <c r="A13" s="196" t="s">
         <v>201</v>
       </c>
-      <c r="B13" s="201"/>
+      <c r="B13" s="197"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="200" t="s">
+      <c r="A14" s="196" t="s">
         <v>202</v>
       </c>
-      <c r="B14" s="201"/>
+      <c r="B14" s="197"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="200" t="s">
+      <c r="A15" s="196" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="201"/>
+      <c r="B15" s="197"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="200" t="s">
+      <c r="A16" s="196" t="s">
         <v>204</v>
       </c>
-      <c r="B16" s="201"/>
+      <c r="B16" s="197"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="196" t="s">
+      <c r="A17" s="198" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="197"/>
+      <c r="B17" s="199"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="213" t="s">
+      <c r="A19" s="200" t="s">
         <v>208</v>
       </c>
-      <c r="B19" s="214"/>
+      <c r="B19" s="201"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="211" t="s">
+      <c r="A21" s="202" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="212"/>
+      <c r="B21" s="203"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="198"/>
-      <c r="B22" s="199"/>
+      <c r="A22" s="204"/>
+      <c r="B22" s="205"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="200" t="s">
+      <c r="A23" s="196" t="s">
         <v>210</v>
       </c>
-      <c r="B23" s="201"/>
+      <c r="B23" s="197"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="200"/>
-      <c r="B24" s="201"/>
+      <c r="A24" s="196"/>
+      <c r="B24" s="197"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="200" t="s">
+      <c r="A25" s="196" t="s">
         <v>211</v>
       </c>
-      <c r="B25" s="201"/>
+      <c r="B25" s="197"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="200" t="s">
+      <c r="A26" s="196" t="s">
         <v>212</v>
       </c>
-      <c r="B26" s="201"/>
+      <c r="B26" s="197"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="196"/>
-      <c r="B27" s="197"/>
+      <c r="A27" s="198"/>
+      <c r="B27" s="199"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25829,6 +25816,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Flintstones - level 3 done 1134 frames ahead
</commit_message>
<xml_diff>
--- a/Flintstones/Compare/Flintstones.xlsx
+++ b/Flintstones/Compare/Flintstones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="229">
   <si>
     <t>Notes</t>
   </si>
@@ -741,6 +741,12 @@
   <si>
     <t>X=87</t>
   </si>
+  <si>
+    <t>Black Screen</t>
+  </si>
+  <si>
+    <t>losing 9 frames to save weapon energy for later</t>
+  </si>
 </sst>
 </file>
 
@@ -750,10 +756,24 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1679,34 +1699,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1714,208 +1734,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="29" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1925,10 +1945,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1949,143 +1969,147 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="47" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2404,7 +2428,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2420,16 +2444,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="157" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="157" t="s">
+      <c r="B1" s="156"/>
+      <c r="C1" s="158" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="159"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65541)</f>
@@ -2507,10 +2531,10 @@
       <c r="B5" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="154" t="s">
+      <c r="C5" s="155" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="154"/>
+      <c r="D5" s="155"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2526,10 +2550,10 @@
       <c r="B6" s="147" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="154" t="s">
+      <c r="C6" s="155" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="155"/>
+      <c r="D6" s="156"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2547,7 +2571,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="159" t="s">
+      <c r="A8" s="160" t="s">
         <v>190</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2567,7 +2591,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="152"/>
+      <c r="A9" s="153"/>
       <c r="B9" s="98" t="s">
         <v>185</v>
       </c>
@@ -2577,7 +2601,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="152"/>
+      <c r="A10" s="153"/>
       <c r="B10" s="100"/>
       <c r="C10" s="101"/>
       <c r="D10" s="101"/>
@@ -2588,7 +2612,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="152"/>
+      <c r="A11" s="153"/>
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
       <c r="D11" s="101"/>
@@ -2599,7 +2623,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="152"/>
+      <c r="A12" s="153"/>
       <c r="B12" s="100"/>
       <c r="C12" s="101"/>
       <c r="D12" s="101"/>
@@ -2610,7 +2634,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="152"/>
+      <c r="A13" s="153"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2621,7 +2645,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="152"/>
+      <c r="A14" s="153"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2632,7 +2656,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="152"/>
+      <c r="A15" s="153"/>
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
@@ -2643,7 +2667,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="152"/>
+      <c r="A16" s="153"/>
       <c r="B16" s="98" t="s">
         <v>188</v>
       </c>
@@ -2686,7 +2710,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="153" t="s">
+      <c r="A19" s="154" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2706,7 +2730,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="152"/>
+      <c r="A20" s="153"/>
       <c r="B20" s="98" t="s">
         <v>185</v>
       </c>
@@ -2719,7 +2743,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="152"/>
+      <c r="A21" s="153"/>
       <c r="B21" s="100"/>
       <c r="C21" s="101"/>
       <c r="D21" s="101"/>
@@ -2730,7 +2754,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="152"/>
+      <c r="A22" s="153"/>
       <c r="B22" s="100"/>
       <c r="C22" s="101"/>
       <c r="D22" s="101"/>
@@ -2741,7 +2765,7 @@
       <c r="F22" s="105"/>
     </row>
     <row r="23" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="152"/>
+      <c r="A23" s="153"/>
       <c r="B23" s="100"/>
       <c r="C23" s="101"/>
       <c r="D23" s="101"/>
@@ -2752,7 +2776,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="152"/>
+      <c r="A24" s="153"/>
       <c r="B24" s="100"/>
       <c r="C24" s="101"/>
       <c r="D24" s="101"/>
@@ -2763,7 +2787,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="152"/>
+      <c r="A25" s="153"/>
       <c r="B25" s="100"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -2774,7 +2798,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="152"/>
+      <c r="A26" s="153"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -2785,7 +2809,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="152"/>
+      <c r="A27" s="153"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -2796,7 +2820,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="152"/>
+      <c r="A28" s="153"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2807,7 +2831,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="152"/>
+      <c r="A29" s="153"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2818,7 +2842,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="152"/>
+      <c r="A30" s="153"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2829,7 +2853,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="152"/>
+      <c r="A31" s="153"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2840,7 +2864,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="152"/>
+      <c r="A32" s="153"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2851,7 +2875,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="152"/>
+      <c r="A33" s="153"/>
       <c r="B33" s="98" t="s">
         <v>188</v>
       </c>
@@ -2890,7 +2914,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="151" t="s">
+      <c r="A36" s="152" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2910,7 +2934,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="152"/>
+      <c r="A37" s="153"/>
       <c r="B37" s="98" t="s">
         <v>185</v>
       </c>
@@ -2927,7 +2951,7 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="152"/>
+      <c r="A38" s="153"/>
       <c r="B38" s="148" t="s">
         <v>216</v>
       </c>
@@ -2944,7 +2968,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="152"/>
+      <c r="A39" s="153"/>
       <c r="B39" s="148" t="s">
         <v>217</v>
       </c>
@@ -2961,7 +2985,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="152"/>
+      <c r="A40" s="153"/>
       <c r="B40" s="148" t="s">
         <v>218</v>
       </c>
@@ -2978,7 +3002,7 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="152"/>
+      <c r="A41" s="153"/>
       <c r="B41" s="148" t="s">
         <v>219</v>
       </c>
@@ -2995,7 +3019,7 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="152"/>
+      <c r="A42" s="153"/>
       <c r="B42" s="148" t="s">
         <v>217</v>
       </c>
@@ -3012,7 +3036,7 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="152"/>
+      <c r="A43" s="153"/>
       <c r="B43" s="148" t="s">
         <v>220</v>
       </c>
@@ -3029,7 +3053,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="152"/>
+      <c r="A44" s="153"/>
       <c r="B44" s="148" t="s">
         <v>221</v>
       </c>
@@ -3046,7 +3070,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="152"/>
+      <c r="A45" s="153"/>
       <c r="B45" s="148" t="s">
         <v>169</v>
       </c>
@@ -3063,7 +3087,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="152"/>
+      <c r="A46" s="153"/>
       <c r="B46" s="148" t="s">
         <v>217</v>
       </c>
@@ -3080,7 +3104,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="152"/>
+      <c r="A47" s="153"/>
       <c r="B47" s="148" t="s">
         <v>169</v>
       </c>
@@ -3097,7 +3121,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="152"/>
+      <c r="A48" s="153"/>
       <c r="B48" s="148" t="s">
         <v>216</v>
       </c>
@@ -3114,7 +3138,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="152"/>
+      <c r="A49" s="153"/>
       <c r="B49" s="148" t="s">
         <v>217</v>
       </c>
@@ -3131,7 +3155,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="152"/>
+      <c r="A50" s="153"/>
       <c r="B50" s="148" t="s">
         <v>169</v>
       </c>
@@ -3148,7 +3172,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="152"/>
+      <c r="A51" s="153"/>
       <c r="B51" s="148"/>
       <c r="C51" s="101"/>
       <c r="D51" s="101"/>
@@ -3156,7 +3180,7 @@
       <c r="F51" s="105"/>
     </row>
     <row r="52" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="152"/>
+      <c r="A52" s="153"/>
       <c r="B52" s="148"/>
       <c r="C52" s="101"/>
       <c r="D52" s="101"/>
@@ -3164,7 +3188,7 @@
       <c r="F52" s="105"/>
     </row>
     <row r="53" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="152"/>
+      <c r="A53" s="153"/>
       <c r="B53" s="100"/>
       <c r="C53" s="101"/>
       <c r="D53" s="101"/>
@@ -3175,7 +3199,7 @@
       <c r="F53" s="105"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="152"/>
+      <c r="A54" s="153"/>
       <c r="B54" s="98" t="s">
         <v>188</v>
       </c>
@@ -3218,7 +3242,7 @@
     </row>
     <row r="56" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="153" t="s">
+      <c r="A57" s="154" t="s">
         <v>171</v>
       </c>
       <c r="B57" s="109" t="s">
@@ -3238,7 +3262,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="152"/>
+      <c r="A58" s="153"/>
       <c r="B58" s="98" t="s">
         <v>185</v>
       </c>
@@ -3255,7 +3279,7 @@
       <c r="F58" s="104"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="152"/>
+      <c r="A59" s="153"/>
       <c r="B59" s="148" t="s">
         <v>216</v>
       </c>
@@ -3272,7 +3296,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="152"/>
+      <c r="A60" s="153"/>
       <c r="B60" s="148" t="s">
         <v>217</v>
       </c>
@@ -3289,7 +3313,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="152"/>
+      <c r="A61" s="153"/>
       <c r="B61" s="148" t="s">
         <v>222</v>
       </c>
@@ -3304,7 +3328,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="152"/>
+      <c r="A62" s="153"/>
       <c r="B62" s="148" t="s">
         <v>217</v>
       </c>
@@ -3321,7 +3345,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="152"/>
+      <c r="A63" s="153"/>
       <c r="B63" s="148" t="s">
         <v>217</v>
       </c>
@@ -3338,7 +3362,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="152"/>
+      <c r="A64" s="153"/>
       <c r="B64" s="148" t="s">
         <v>223</v>
       </c>
@@ -3353,7 +3377,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="152"/>
+      <c r="A65" s="153"/>
       <c r="B65" s="148" t="s">
         <v>217</v>
       </c>
@@ -3370,7 +3394,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="152"/>
+      <c r="A66" s="153"/>
       <c r="B66" s="148" t="s">
         <v>224</v>
       </c>
@@ -3387,7 +3411,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="152"/>
+      <c r="A67" s="153"/>
       <c r="B67" s="148" t="s">
         <v>225</v>
       </c>
@@ -3404,7 +3428,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="152"/>
+      <c r="A68" s="153"/>
       <c r="B68" s="149" t="s">
         <v>217</v>
       </c>
@@ -3421,7 +3445,7 @@
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="152"/>
+      <c r="A69" s="153"/>
       <c r="B69" s="150" t="s">
         <v>226</v>
       </c>
@@ -3438,7 +3462,7 @@
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="152"/>
+      <c r="A70" s="153"/>
       <c r="B70" s="150" t="s">
         <v>217</v>
       </c>
@@ -3455,18 +3479,26 @@
       <c r="F70" s="105"/>
     </row>
     <row r="71" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="152"/>
-      <c r="B71" s="149"/>
-      <c r="C71" s="101"/>
-      <c r="D71" s="101"/>
+      <c r="A71" s="153"/>
+      <c r="B71" s="151" t="s">
+        <v>227</v>
+      </c>
+      <c r="C71" s="101">
+        <v>17371</v>
+      </c>
+      <c r="D71" s="101">
+        <v>18505</v>
+      </c>
       <c r="E71" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F71" s="105"/>
+        <v>1134</v>
+      </c>
+      <c r="F71" s="216" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="72" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="152"/>
+      <c r="A72" s="153"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
@@ -3477,7 +3509,7 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="152"/>
+      <c r="A73" s="153"/>
       <c r="B73" s="98" t="s">
         <v>188</v>
       </c>
@@ -3516,7 +3548,7 @@
     </row>
     <row r="75" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="151" t="s">
+      <c r="A76" s="152" t="s">
         <v>172</v>
       </c>
       <c r="B76" s="113" t="s">
@@ -3536,7 +3568,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="152"/>
+      <c r="A77" s="153"/>
       <c r="B77" s="98" t="s">
         <v>185</v>
       </c>
@@ -3549,7 +3581,7 @@
       <c r="F77" s="104"/>
     </row>
     <row r="78" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="152"/>
+      <c r="A78" s="153"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3560,7 +3592,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="152"/>
+      <c r="A79" s="153"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3571,7 +3603,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="152"/>
+      <c r="A80" s="153"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3582,7 +3614,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="152"/>
+      <c r="A81" s="153"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3593,7 +3625,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="152"/>
+      <c r="A82" s="153"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3604,7 +3636,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="152"/>
+      <c r="A83" s="153"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3615,7 +3647,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="152"/>
+      <c r="A84" s="153"/>
       <c r="B84" s="100"/>
       <c r="C84" s="101"/>
       <c r="D84" s="101"/>
@@ -3626,7 +3658,7 @@
       <c r="F84" s="105"/>
     </row>
     <row r="85" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="152"/>
+      <c r="A85" s="153"/>
       <c r="B85" s="100"/>
       <c r="C85" s="101"/>
       <c r="D85" s="101"/>
@@ -3637,7 +3669,7 @@
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="152"/>
+      <c r="A86" s="153"/>
       <c r="B86" s="100"/>
       <c r="C86" s="101"/>
       <c r="D86" s="101"/>
@@ -3648,7 +3680,7 @@
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="152"/>
+      <c r="A87" s="153"/>
       <c r="B87" s="100"/>
       <c r="C87" s="101"/>
       <c r="D87" s="101"/>
@@ -3659,7 +3691,7 @@
       <c r="F87" s="105"/>
     </row>
     <row r="88" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="152"/>
+      <c r="A88" s="153"/>
       <c r="B88" s="100"/>
       <c r="C88" s="101"/>
       <c r="D88" s="101"/>
@@ -3670,7 +3702,7 @@
       <c r="F88" s="105"/>
     </row>
     <row r="89" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="152"/>
+      <c r="A89" s="153"/>
       <c r="B89" s="100"/>
       <c r="C89" s="101"/>
       <c r="D89" s="101"/>
@@ -3681,7 +3713,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="152"/>
+      <c r="A90" s="153"/>
       <c r="B90" s="98" t="s">
         <v>188</v>
       </c>
@@ -3720,7 +3752,7 @@
     </row>
     <row r="92" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="93" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="153" t="s">
+      <c r="A93" s="154" t="s">
         <v>173</v>
       </c>
       <c r="B93" s="109" t="s">
@@ -3740,7 +3772,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="152"/>
+      <c r="A94" s="153"/>
       <c r="B94" s="98" t="s">
         <v>185</v>
       </c>
@@ -3753,7 +3785,7 @@
       <c r="F94" s="104"/>
     </row>
     <row r="95" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="152"/>
+      <c r="A95" s="153"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3764,7 +3796,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="152"/>
+      <c r="A96" s="153"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3775,7 +3807,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="152"/>
+      <c r="A97" s="153"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3786,7 +3818,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="152"/>
+      <c r="A98" s="153"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3797,7 +3829,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="152"/>
+      <c r="A99" s="153"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3808,7 +3840,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="152"/>
+      <c r="A100" s="153"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3819,7 +3851,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="152"/>
+      <c r="A101" s="153"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -3830,7 +3862,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="152"/>
+      <c r="A102" s="153"/>
       <c r="B102" s="100"/>
       <c r="C102" s="101"/>
       <c r="D102" s="101"/>
@@ -3841,7 +3873,7 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="152"/>
+      <c r="A103" s="153"/>
       <c r="B103" s="100"/>
       <c r="C103" s="101"/>
       <c r="D103" s="101"/>
@@ -3852,7 +3884,7 @@
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="152"/>
+      <c r="A104" s="153"/>
       <c r="B104" s="100"/>
       <c r="C104" s="101"/>
       <c r="D104" s="101"/>
@@ -3863,7 +3895,7 @@
       <c r="F104" s="105"/>
     </row>
     <row r="105" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="152"/>
+      <c r="A105" s="153"/>
       <c r="B105" s="100"/>
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
@@ -3874,7 +3906,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="152"/>
+      <c r="A106" s="153"/>
       <c r="B106" s="100"/>
       <c r="C106" s="101"/>
       <c r="D106" s="101"/>
@@ -3885,7 +3917,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="152"/>
+      <c r="A107" s="153"/>
       <c r="B107" s="98" t="s">
         <v>188</v>
       </c>
@@ -3923,7 +3955,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="151" t="s">
+      <c r="A110" s="152" t="s">
         <v>174</v>
       </c>
       <c r="B110" s="113" t="s">
@@ -3943,7 +3975,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="152"/>
+      <c r="A111" s="153"/>
       <c r="B111" s="98" t="s">
         <v>185</v>
       </c>
@@ -3956,7 +3988,7 @@
       <c r="F111" s="104"/>
     </row>
     <row r="112" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="152"/>
+      <c r="A112" s="153"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3967,7 +3999,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="152"/>
+      <c r="A113" s="153"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3978,7 +4010,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="152"/>
+      <c r="A114" s="153"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3989,7 +4021,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="152"/>
+      <c r="A115" s="153"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -4000,7 +4032,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="152"/>
+      <c r="A116" s="153"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -4011,7 +4043,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="152"/>
+      <c r="A117" s="153"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -4022,7 +4054,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="152"/>
+      <c r="A118" s="153"/>
       <c r="B118" s="100"/>
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
@@ -4033,7 +4065,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="152"/>
+      <c r="A119" s="153"/>
       <c r="B119" s="100"/>
       <c r="C119" s="101"/>
       <c r="D119" s="101"/>
@@ -4044,7 +4076,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="152"/>
+      <c r="A120" s="153"/>
       <c r="B120" s="100"/>
       <c r="C120" s="101"/>
       <c r="D120" s="101"/>
@@ -4055,7 +4087,7 @@
       <c r="F120" s="105"/>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="152"/>
+      <c r="A121" s="153"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -4066,7 +4098,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="152"/>
+      <c r="A122" s="153"/>
       <c r="B122" s="100"/>
       <c r="C122" s="101"/>
       <c r="D122" s="101"/>
@@ -4077,7 +4109,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="152"/>
+      <c r="A123" s="153"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -4088,7 +4120,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="152"/>
+      <c r="A124" s="153"/>
       <c r="B124" s="98" t="s">
         <v>188</v>
       </c>
@@ -4126,7 +4158,7 @@
       </c>
     </row>
     <row r="127" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="153" t="s">
+      <c r="A127" s="154" t="s">
         <v>175</v>
       </c>
       <c r="B127" s="109" t="s">
@@ -4146,7 +4178,7 @@
       </c>
     </row>
     <row r="128" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="152"/>
+      <c r="A128" s="153"/>
       <c r="B128" s="98" t="s">
         <v>185</v>
       </c>
@@ -4159,7 +4191,7 @@
       <c r="F128" s="104"/>
     </row>
     <row r="129" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="152"/>
+      <c r="A129" s="153"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4170,7 +4202,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="152"/>
+      <c r="A130" s="153"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4181,7 +4213,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="152"/>
+      <c r="A131" s="153"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4192,7 +4224,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="152"/>
+      <c r="A132" s="153"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4203,7 +4235,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="152"/>
+      <c r="A133" s="153"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4214,7 +4246,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="152"/>
+      <c r="A134" s="153"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4225,7 +4257,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="152"/>
+      <c r="A135" s="153"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4236,7 +4268,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="152"/>
+      <c r="A136" s="153"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
       <c r="D136" s="101"/>
@@ -4247,7 +4279,7 @@
       <c r="F136" s="105"/>
     </row>
     <row r="137" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="152"/>
+      <c r="A137" s="153"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4258,7 +4290,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="152"/>
+      <c r="A138" s="153"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4269,7 +4301,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="152"/>
+      <c r="A139" s="153"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4280,7 +4312,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="152"/>
+      <c r="A140" s="153"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4291,7 +4323,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="152"/>
+      <c r="A141" s="153"/>
       <c r="B141" s="98" t="s">
         <v>188</v>
       </c>
@@ -4329,7 +4361,7 @@
       </c>
     </row>
     <row r="144" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A144" s="151" t="s">
+      <c r="A144" s="152" t="s">
         <v>176</v>
       </c>
       <c r="B144" s="113" t="s">
@@ -4349,7 +4381,7 @@
       </c>
     </row>
     <row r="145" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="152"/>
+      <c r="A145" s="153"/>
       <c r="B145" s="98" t="s">
         <v>185</v>
       </c>
@@ -4362,7 +4394,7 @@
       <c r="F145" s="104"/>
     </row>
     <row r="146" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="152"/>
+      <c r="A146" s="153"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4373,7 +4405,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A147" s="152"/>
+      <c r="A147" s="153"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4384,7 +4416,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A148" s="152"/>
+      <c r="A148" s="153"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4395,7 +4427,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A149" s="152"/>
+      <c r="A149" s="153"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
@@ -4406,7 +4438,7 @@
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A150" s="152"/>
+      <c r="A150" s="153"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -4417,7 +4449,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A151" s="152"/>
+      <c r="A151" s="153"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -4428,7 +4460,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A152" s="152"/>
+      <c r="A152" s="153"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
@@ -4439,7 +4471,7 @@
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A153" s="152"/>
+      <c r="A153" s="153"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
@@ -4450,7 +4482,7 @@
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A154" s="152"/>
+      <c r="A154" s="153"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -4461,7 +4493,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A155" s="152"/>
+      <c r="A155" s="153"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
@@ -4472,7 +4504,7 @@
       <c r="F155" s="105"/>
     </row>
     <row r="156" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A156" s="152"/>
+      <c r="A156" s="153"/>
       <c r="B156" s="100"/>
       <c r="C156" s="101"/>
       <c r="D156" s="101"/>
@@ -4483,7 +4515,7 @@
       <c r="F156" s="105"/>
     </row>
     <row r="157" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A157" s="152"/>
+      <c r="A157" s="153"/>
       <c r="B157" s="100"/>
       <c r="C157" s="101"/>
       <c r="D157" s="101"/>
@@ -4494,7 +4526,7 @@
       <c r="F157" s="105"/>
     </row>
     <row r="158" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="152"/>
+      <c r="A158" s="153"/>
       <c r="B158" s="98" t="s">
         <v>188</v>
       </c>
@@ -4577,13 +4609,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4613,18 +4645,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="165"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4776,9 +4808,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="165"/>
-      <c r="D21" s="166"/>
-      <c r="E21" s="166"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4929,9 +4961,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="163"/>
-      <c r="D38" s="164"/>
-      <c r="E38" s="164"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="165"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -5082,9 +5114,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="163"/>
-      <c r="D55" s="164"/>
-      <c r="E55" s="164"/>
+      <c r="C55" s="164"/>
+      <c r="D55" s="165"/>
+      <c r="E55" s="165"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -5235,9 +5267,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="163"/>
-      <c r="D72" s="164"/>
-      <c r="E72" s="164"/>
+      <c r="C72" s="164"/>
+      <c r="D72" s="165"/>
+      <c r="E72" s="165"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5388,9 +5420,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="163"/>
-      <c r="D89" s="164"/>
-      <c r="E89" s="164"/>
+      <c r="C89" s="164"/>
+      <c r="D89" s="165"/>
+      <c r="E89" s="165"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5541,9 +5573,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="163"/>
-      <c r="D106" s="164"/>
-      <c r="E106" s="164"/>
+      <c r="C106" s="164"/>
+      <c r="D106" s="165"/>
+      <c r="E106" s="165"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5694,9 +5726,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="163"/>
-      <c r="D123" s="164"/>
-      <c r="E123" s="164"/>
+      <c r="C123" s="164"/>
+      <c r="D123" s="165"/>
+      <c r="E123" s="165"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5847,9 +5879,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="163"/>
-      <c r="D140" s="164"/>
-      <c r="E140" s="164"/>
+      <c r="C140" s="164"/>
+      <c r="D140" s="165"/>
+      <c r="E140" s="165"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -6000,9 +6032,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="163"/>
-      <c r="D157" s="164"/>
-      <c r="E157" s="164"/>
+      <c r="C157" s="164"/>
+      <c r="D157" s="165"/>
+      <c r="E157" s="165"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -6153,9 +6185,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="163"/>
-      <c r="D174" s="164"/>
-      <c r="E174" s="164"/>
+      <c r="C174" s="164"/>
+      <c r="D174" s="165"/>
+      <c r="E174" s="165"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6306,9 +6338,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="163"/>
-      <c r="D191" s="164"/>
-      <c r="E191" s="164"/>
+      <c r="C191" s="164"/>
+      <c r="D191" s="165"/>
+      <c r="E191" s="165"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6459,9 +6491,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="163"/>
-      <c r="D208" s="164"/>
-      <c r="E208" s="164"/>
+      <c r="C208" s="164"/>
+      <c r="D208" s="165"/>
+      <c r="E208" s="165"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6612,9 +6644,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="163"/>
-      <c r="D225" s="164"/>
-      <c r="E225" s="164"/>
+      <c r="C225" s="164"/>
+      <c r="D225" s="165"/>
+      <c r="E225" s="165"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6765,9 +6797,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="163"/>
-      <c r="D242" s="164"/>
-      <c r="E242" s="164"/>
+      <c r="C242" s="164"/>
+      <c r="D242" s="165"/>
+      <c r="E242" s="165"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6918,9 +6950,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="163"/>
-      <c r="D259" s="164"/>
-      <c r="E259" s="164"/>
+      <c r="C259" s="164"/>
+      <c r="D259" s="165"/>
+      <c r="E259" s="165"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -7071,18 +7103,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="167"/>
-      <c r="D276" s="168"/>
-      <c r="E276" s="168"/>
+      <c r="C276" s="168"/>
+      <c r="D276" s="169"/>
+      <c r="E276" s="169"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="163"/>
-      <c r="D277" s="164"/>
-      <c r="E277" s="164"/>
+      <c r="C277" s="164"/>
+      <c r="D277" s="165"/>
+      <c r="E277" s="165"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -7233,9 +7265,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="165"/>
-      <c r="D294" s="166"/>
-      <c r="E294" s="166"/>
+      <c r="C294" s="166"/>
+      <c r="D294" s="167"/>
+      <c r="E294" s="167"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7386,9 +7418,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="163"/>
-      <c r="D311" s="164"/>
-      <c r="E311" s="164"/>
+      <c r="C311" s="164"/>
+      <c r="D311" s="165"/>
+      <c r="E311" s="165"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7539,9 +7571,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="163"/>
-      <c r="D328" s="164"/>
-      <c r="E328" s="164"/>
+      <c r="C328" s="164"/>
+      <c r="D328" s="165"/>
+      <c r="E328" s="165"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7692,9 +7724,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="163"/>
-      <c r="D345" s="164"/>
-      <c r="E345" s="164"/>
+      <c r="C345" s="164"/>
+      <c r="D345" s="165"/>
+      <c r="E345" s="165"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7845,9 +7877,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="163"/>
-      <c r="D362" s="164"/>
-      <c r="E362" s="164"/>
+      <c r="C362" s="164"/>
+      <c r="D362" s="165"/>
+      <c r="E362" s="165"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -7998,9 +8030,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="163"/>
-      <c r="D379" s="164"/>
-      <c r="E379" s="164"/>
+      <c r="C379" s="164"/>
+      <c r="D379" s="165"/>
+      <c r="E379" s="165"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -8151,9 +8183,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="163"/>
-      <c r="D396" s="164"/>
-      <c r="E396" s="164"/>
+      <c r="C396" s="164"/>
+      <c r="D396" s="165"/>
+      <c r="E396" s="165"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8304,9 +8336,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="163"/>
-      <c r="D413" s="164"/>
-      <c r="E413" s="164"/>
+      <c r="C413" s="164"/>
+      <c r="D413" s="165"/>
+      <c r="E413" s="165"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8457,9 +8489,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="163"/>
-      <c r="D430" s="164"/>
-      <c r="E430" s="164"/>
+      <c r="C430" s="164"/>
+      <c r="D430" s="165"/>
+      <c r="E430" s="165"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8610,9 +8642,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="163"/>
-      <c r="D447" s="164"/>
-      <c r="E447" s="164"/>
+      <c r="C447" s="164"/>
+      <c r="D447" s="165"/>
+      <c r="E447" s="165"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8763,9 +8795,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="163"/>
-      <c r="D464" s="164"/>
-      <c r="E464" s="164"/>
+      <c r="C464" s="164"/>
+      <c r="D464" s="165"/>
+      <c r="E464" s="165"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8916,9 +8948,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="163"/>
-      <c r="D481" s="164"/>
-      <c r="E481" s="164"/>
+      <c r="C481" s="164"/>
+      <c r="D481" s="165"/>
+      <c r="E481" s="165"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -9069,9 +9101,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="163"/>
-      <c r="D498" s="164"/>
-      <c r="E498" s="164"/>
+      <c r="C498" s="164"/>
+      <c r="D498" s="165"/>
+      <c r="E498" s="165"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -9222,9 +9254,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="163"/>
-      <c r="D515" s="164"/>
-      <c r="E515" s="164"/>
+      <c r="C515" s="164"/>
+      <c r="D515" s="165"/>
+      <c r="E515" s="165"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9375,9 +9407,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="163"/>
-      <c r="D532" s="164"/>
-      <c r="E532" s="164"/>
+      <c r="C532" s="164"/>
+      <c r="D532" s="165"/>
+      <c r="E532" s="165"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9528,18 +9560,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="169"/>
-      <c r="D549" s="170"/>
-      <c r="E549" s="170"/>
+      <c r="C549" s="170"/>
+      <c r="D549" s="171"/>
+      <c r="E549" s="171"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="163"/>
-      <c r="D550" s="164"/>
-      <c r="E550" s="164"/>
+      <c r="C550" s="164"/>
+      <c r="D550" s="165"/>
+      <c r="E550" s="165"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9690,9 +9722,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="165"/>
-      <c r="D567" s="166"/>
-      <c r="E567" s="166"/>
+      <c r="C567" s="166"/>
+      <c r="D567" s="167"/>
+      <c r="E567" s="167"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9843,9 +9875,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="163"/>
-      <c r="D584" s="164"/>
-      <c r="E584" s="164"/>
+      <c r="C584" s="164"/>
+      <c r="D584" s="165"/>
+      <c r="E584" s="165"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -9996,9 +10028,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="163"/>
-      <c r="D601" s="164"/>
-      <c r="E601" s="164"/>
+      <c r="C601" s="164"/>
+      <c r="D601" s="165"/>
+      <c r="E601" s="165"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -10149,9 +10181,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="163"/>
-      <c r="D618" s="164"/>
-      <c r="E618" s="164"/>
+      <c r="C618" s="164"/>
+      <c r="D618" s="165"/>
+      <c r="E618" s="165"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10302,9 +10334,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="163"/>
-      <c r="D635" s="164"/>
-      <c r="E635" s="164"/>
+      <c r="C635" s="164"/>
+      <c r="D635" s="165"/>
+      <c r="E635" s="165"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10455,9 +10487,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="163"/>
-      <c r="D652" s="164"/>
-      <c r="E652" s="164"/>
+      <c r="C652" s="164"/>
+      <c r="D652" s="165"/>
+      <c r="E652" s="165"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10608,9 +10640,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="163"/>
-      <c r="D669" s="164"/>
-      <c r="E669" s="164"/>
+      <c r="C669" s="164"/>
+      <c r="D669" s="165"/>
+      <c r="E669" s="165"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10761,9 +10793,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="163"/>
-      <c r="D686" s="164"/>
-      <c r="E686" s="164"/>
+      <c r="C686" s="164"/>
+      <c r="D686" s="165"/>
+      <c r="E686" s="165"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10914,9 +10946,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="163"/>
-      <c r="D703" s="164"/>
-      <c r="E703" s="164"/>
+      <c r="C703" s="164"/>
+      <c r="D703" s="165"/>
+      <c r="E703" s="165"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -11067,9 +11099,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="163"/>
-      <c r="D720" s="164"/>
-      <c r="E720" s="164"/>
+      <c r="C720" s="164"/>
+      <c r="D720" s="165"/>
+      <c r="E720" s="165"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -11220,9 +11252,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="163"/>
-      <c r="D737" s="164"/>
-      <c r="E737" s="164"/>
+      <c r="C737" s="164"/>
+      <c r="D737" s="165"/>
+      <c r="E737" s="165"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11373,9 +11405,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="163"/>
-      <c r="D754" s="164"/>
-      <c r="E754" s="164"/>
+      <c r="C754" s="164"/>
+      <c r="D754" s="165"/>
+      <c r="E754" s="165"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11526,9 +11558,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="163"/>
-      <c r="D771" s="164"/>
-      <c r="E771" s="164"/>
+      <c r="C771" s="164"/>
+      <c r="D771" s="165"/>
+      <c r="E771" s="165"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11679,9 +11711,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="163"/>
-      <c r="D788" s="164"/>
-      <c r="E788" s="164"/>
+      <c r="C788" s="164"/>
+      <c r="D788" s="165"/>
+      <c r="E788" s="165"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11832,9 +11864,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="163"/>
-      <c r="D805" s="164"/>
-      <c r="E805" s="164"/>
+      <c r="C805" s="164"/>
+      <c r="D805" s="165"/>
+      <c r="E805" s="165"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -11985,18 +12017,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="171"/>
-      <c r="D822" s="172"/>
-      <c r="E822" s="172"/>
+      <c r="C822" s="172"/>
+      <c r="D822" s="173"/>
+      <c r="E822" s="173"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="163"/>
-      <c r="D823" s="164"/>
-      <c r="E823" s="164"/>
+      <c r="C823" s="164"/>
+      <c r="D823" s="165"/>
+      <c r="E823" s="165"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -12147,9 +12179,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="165"/>
-      <c r="D840" s="166"/>
-      <c r="E840" s="166"/>
+      <c r="C840" s="166"/>
+      <c r="D840" s="167"/>
+      <c r="E840" s="167"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12300,9 +12332,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="163"/>
-      <c r="D857" s="164"/>
-      <c r="E857" s="164"/>
+      <c r="C857" s="164"/>
+      <c r="D857" s="165"/>
+      <c r="E857" s="165"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12453,9 +12485,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="163"/>
-      <c r="D874" s="164"/>
-      <c r="E874" s="164"/>
+      <c r="C874" s="164"/>
+      <c r="D874" s="165"/>
+      <c r="E874" s="165"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12606,9 +12638,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="163"/>
-      <c r="D891" s="164"/>
-      <c r="E891" s="164"/>
+      <c r="C891" s="164"/>
+      <c r="D891" s="165"/>
+      <c r="E891" s="165"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12759,9 +12791,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="163"/>
-      <c r="D908" s="164"/>
-      <c r="E908" s="164"/>
+      <c r="C908" s="164"/>
+      <c r="D908" s="165"/>
+      <c r="E908" s="165"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12912,9 +12944,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="163"/>
-      <c r="D925" s="164"/>
-      <c r="E925" s="164"/>
+      <c r="C925" s="164"/>
+      <c r="D925" s="165"/>
+      <c r="E925" s="165"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -13065,9 +13097,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="163"/>
-      <c r="D942" s="164"/>
-      <c r="E942" s="164"/>
+      <c r="C942" s="164"/>
+      <c r="D942" s="165"/>
+      <c r="E942" s="165"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -13218,9 +13250,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="163"/>
-      <c r="D959" s="164"/>
-      <c r="E959" s="164"/>
+      <c r="C959" s="164"/>
+      <c r="D959" s="165"/>
+      <c r="E959" s="165"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13371,9 +13403,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="163"/>
-      <c r="D976" s="164"/>
-      <c r="E976" s="164"/>
+      <c r="C976" s="164"/>
+      <c r="D976" s="165"/>
+      <c r="E976" s="165"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13524,9 +13556,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="163"/>
-      <c r="D993" s="164"/>
-      <c r="E993" s="164"/>
+      <c r="C993" s="164"/>
+      <c r="D993" s="165"/>
+      <c r="E993" s="165"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13677,9 +13709,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="163"/>
-      <c r="D1010" s="164"/>
-      <c r="E1010" s="164"/>
+      <c r="C1010" s="164"/>
+      <c r="D1010" s="165"/>
+      <c r="E1010" s="165"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13830,9 +13862,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="163"/>
-      <c r="D1027" s="164"/>
-      <c r="E1027" s="164"/>
+      <c r="C1027" s="164"/>
+      <c r="D1027" s="165"/>
+      <c r="E1027" s="165"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -13983,9 +14015,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="163"/>
-      <c r="D1044" s="164"/>
-      <c r="E1044" s="164"/>
+      <c r="C1044" s="164"/>
+      <c r="D1044" s="165"/>
+      <c r="E1044" s="165"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -14136,9 +14168,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="163"/>
-      <c r="D1061" s="164"/>
-      <c r="E1061" s="164"/>
+      <c r="C1061" s="164"/>
+      <c r="D1061" s="165"/>
+      <c r="E1061" s="165"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14289,9 +14321,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="163"/>
-      <c r="D1078" s="164"/>
-      <c r="E1078" s="164"/>
+      <c r="C1078" s="164"/>
+      <c r="D1078" s="165"/>
+      <c r="E1078" s="165"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14442,18 +14474,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="173"/>
-      <c r="D1095" s="174"/>
-      <c r="E1095" s="174"/>
+      <c r="C1095" s="174"/>
+      <c r="D1095" s="175"/>
+      <c r="E1095" s="175"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="163"/>
-      <c r="D1096" s="164"/>
-      <c r="E1096" s="164"/>
+      <c r="C1096" s="164"/>
+      <c r="D1096" s="165"/>
+      <c r="E1096" s="165"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14604,9 +14636,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="165"/>
-      <c r="D1113" s="166"/>
-      <c r="E1113" s="166"/>
+      <c r="C1113" s="166"/>
+      <c r="D1113" s="167"/>
+      <c r="E1113" s="167"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14757,9 +14789,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="163"/>
-      <c r="D1130" s="164"/>
-      <c r="E1130" s="164"/>
+      <c r="C1130" s="164"/>
+      <c r="D1130" s="165"/>
+      <c r="E1130" s="165"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14910,9 +14942,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="163"/>
-      <c r="D1147" s="164"/>
-      <c r="E1147" s="164"/>
+      <c r="C1147" s="164"/>
+      <c r="D1147" s="165"/>
+      <c r="E1147" s="165"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -15063,9 +15095,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="163"/>
-      <c r="D1164" s="164"/>
-      <c r="E1164" s="164"/>
+      <c r="C1164" s="164"/>
+      <c r="D1164" s="165"/>
+      <c r="E1164" s="165"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -15216,9 +15248,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="163"/>
-      <c r="D1181" s="164"/>
-      <c r="E1181" s="164"/>
+      <c r="C1181" s="164"/>
+      <c r="D1181" s="165"/>
+      <c r="E1181" s="165"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15369,9 +15401,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="163"/>
-      <c r="D1198" s="164"/>
-      <c r="E1198" s="164"/>
+      <c r="C1198" s="164"/>
+      <c r="D1198" s="165"/>
+      <c r="E1198" s="165"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15522,9 +15554,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="163"/>
-      <c r="D1215" s="164"/>
-      <c r="E1215" s="164"/>
+      <c r="C1215" s="164"/>
+      <c r="D1215" s="165"/>
+      <c r="E1215" s="165"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15675,9 +15707,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="163"/>
-      <c r="D1232" s="164"/>
-      <c r="E1232" s="164"/>
+      <c r="C1232" s="164"/>
+      <c r="D1232" s="165"/>
+      <c r="E1232" s="165"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15828,9 +15860,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="163"/>
-      <c r="D1249" s="164"/>
-      <c r="E1249" s="164"/>
+      <c r="C1249" s="164"/>
+      <c r="D1249" s="165"/>
+      <c r="E1249" s="165"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -15981,9 +16013,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="163"/>
-      <c r="D1266" s="164"/>
-      <c r="E1266" s="164"/>
+      <c r="C1266" s="164"/>
+      <c r="D1266" s="165"/>
+      <c r="E1266" s="165"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -16134,9 +16166,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="163"/>
-      <c r="D1283" s="164"/>
-      <c r="E1283" s="164"/>
+      <c r="C1283" s="164"/>
+      <c r="D1283" s="165"/>
+      <c r="E1283" s="165"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16287,9 +16319,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="163"/>
-      <c r="D1300" s="164"/>
-      <c r="E1300" s="164"/>
+      <c r="C1300" s="164"/>
+      <c r="D1300" s="165"/>
+      <c r="E1300" s="165"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16440,9 +16472,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="163"/>
-      <c r="D1317" s="164"/>
-      <c r="E1317" s="164"/>
+      <c r="C1317" s="164"/>
+      <c r="D1317" s="165"/>
+      <c r="E1317" s="165"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16593,9 +16625,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="163"/>
-      <c r="D1334" s="164"/>
-      <c r="E1334" s="164"/>
+      <c r="C1334" s="164"/>
+      <c r="D1334" s="165"/>
+      <c r="E1334" s="165"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16746,9 +16778,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="163"/>
-      <c r="D1351" s="164"/>
-      <c r="E1351" s="164"/>
+      <c r="C1351" s="164"/>
+      <c r="D1351" s="165"/>
+      <c r="E1351" s="165"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16899,18 +16931,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="175"/>
-      <c r="D1368" s="176"/>
-      <c r="E1368" s="176"/>
+      <c r="C1368" s="176"/>
+      <c r="D1368" s="177"/>
+      <c r="E1368" s="177"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="163"/>
-      <c r="D1369" s="164"/>
-      <c r="E1369" s="164"/>
+      <c r="C1369" s="164"/>
+      <c r="D1369" s="165"/>
+      <c r="E1369" s="165"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -17061,9 +17093,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="165"/>
-      <c r="D1386" s="166"/>
-      <c r="E1386" s="166"/>
+      <c r="C1386" s="166"/>
+      <c r="D1386" s="167"/>
+      <c r="E1386" s="167"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -17214,9 +17246,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="163"/>
-      <c r="D1403" s="164"/>
-      <c r="E1403" s="164"/>
+      <c r="C1403" s="164"/>
+      <c r="D1403" s="165"/>
+      <c r="E1403" s="165"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17367,9 +17399,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="163"/>
-      <c r="D1420" s="164"/>
-      <c r="E1420" s="164"/>
+      <c r="C1420" s="164"/>
+      <c r="D1420" s="165"/>
+      <c r="E1420" s="165"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17520,9 +17552,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="163"/>
-      <c r="D1437" s="164"/>
-      <c r="E1437" s="164"/>
+      <c r="C1437" s="164"/>
+      <c r="D1437" s="165"/>
+      <c r="E1437" s="165"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17673,9 +17705,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="163"/>
-      <c r="D1454" s="164"/>
-      <c r="E1454" s="164"/>
+      <c r="C1454" s="164"/>
+      <c r="D1454" s="165"/>
+      <c r="E1454" s="165"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17826,9 +17858,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="163"/>
-      <c r="D1471" s="164"/>
-      <c r="E1471" s="164"/>
+      <c r="C1471" s="164"/>
+      <c r="D1471" s="165"/>
+      <c r="E1471" s="165"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -17979,9 +18011,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="163"/>
-      <c r="D1488" s="164"/>
-      <c r="E1488" s="164"/>
+      <c r="C1488" s="164"/>
+      <c r="D1488" s="165"/>
+      <c r="E1488" s="165"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -18132,9 +18164,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="163"/>
-      <c r="D1505" s="164"/>
-      <c r="E1505" s="164"/>
+      <c r="C1505" s="164"/>
+      <c r="D1505" s="165"/>
+      <c r="E1505" s="165"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18285,9 +18317,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="163"/>
-      <c r="D1522" s="164"/>
-      <c r="E1522" s="164"/>
+      <c r="C1522" s="164"/>
+      <c r="D1522" s="165"/>
+      <c r="E1522" s="165"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18438,9 +18470,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="163"/>
-      <c r="D1539" s="164"/>
-      <c r="E1539" s="164"/>
+      <c r="C1539" s="164"/>
+      <c r="D1539" s="165"/>
+      <c r="E1539" s="165"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18591,9 +18623,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="163"/>
-      <c r="D1556" s="164"/>
-      <c r="E1556" s="164"/>
+      <c r="C1556" s="164"/>
+      <c r="D1556" s="165"/>
+      <c r="E1556" s="165"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18744,9 +18776,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="163"/>
-      <c r="D1573" s="164"/>
-      <c r="E1573" s="164"/>
+      <c r="C1573" s="164"/>
+      <c r="D1573" s="165"/>
+      <c r="E1573" s="165"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18897,9 +18929,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="163"/>
-      <c r="D1590" s="164"/>
-      <c r="E1590" s="164"/>
+      <c r="C1590" s="164"/>
+      <c r="D1590" s="165"/>
+      <c r="E1590" s="165"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -19050,9 +19082,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="163"/>
-      <c r="D1607" s="164"/>
-      <c r="E1607" s="164"/>
+      <c r="C1607" s="164"/>
+      <c r="D1607" s="165"/>
+      <c r="E1607" s="165"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -19203,9 +19235,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="163"/>
-      <c r="D1624" s="164"/>
-      <c r="E1624" s="164"/>
+      <c r="C1624" s="164"/>
+      <c r="D1624" s="165"/>
+      <c r="E1624" s="165"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19356,18 +19388,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="177"/>
-      <c r="D1641" s="178"/>
-      <c r="E1641" s="178"/>
+      <c r="C1641" s="178"/>
+      <c r="D1641" s="179"/>
+      <c r="E1641" s="179"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="163"/>
-      <c r="D1642" s="164"/>
-      <c r="E1642" s="164"/>
+      <c r="C1642" s="164"/>
+      <c r="D1642" s="165"/>
+      <c r="E1642" s="165"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19518,9 +19550,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="165"/>
-      <c r="D1659" s="166"/>
-      <c r="E1659" s="166"/>
+      <c r="C1659" s="166"/>
+      <c r="D1659" s="167"/>
+      <c r="E1659" s="167"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19671,9 +19703,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="163"/>
-      <c r="D1676" s="164"/>
-      <c r="E1676" s="164"/>
+      <c r="C1676" s="164"/>
+      <c r="D1676" s="165"/>
+      <c r="E1676" s="165"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19824,9 +19856,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="163"/>
-      <c r="D1693" s="164"/>
-      <c r="E1693" s="164"/>
+      <c r="C1693" s="164"/>
+      <c r="D1693" s="165"/>
+      <c r="E1693" s="165"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -19977,9 +20009,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="163"/>
-      <c r="D1710" s="164"/>
-      <c r="E1710" s="164"/>
+      <c r="C1710" s="164"/>
+      <c r="D1710" s="165"/>
+      <c r="E1710" s="165"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -20130,9 +20162,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="163"/>
-      <c r="D1727" s="164"/>
-      <c r="E1727" s="164"/>
+      <c r="C1727" s="164"/>
+      <c r="D1727" s="165"/>
+      <c r="E1727" s="165"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20283,9 +20315,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="163"/>
-      <c r="D1744" s="164"/>
-      <c r="E1744" s="164"/>
+      <c r="C1744" s="164"/>
+      <c r="D1744" s="165"/>
+      <c r="E1744" s="165"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20436,9 +20468,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="163"/>
-      <c r="D1761" s="164"/>
-      <c r="E1761" s="164"/>
+      <c r="C1761" s="164"/>
+      <c r="D1761" s="165"/>
+      <c r="E1761" s="165"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20589,9 +20621,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="163"/>
-      <c r="D1778" s="164"/>
-      <c r="E1778" s="164"/>
+      <c r="C1778" s="164"/>
+      <c r="D1778" s="165"/>
+      <c r="E1778" s="165"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20742,9 +20774,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="163"/>
-      <c r="D1795" s="164"/>
-      <c r="E1795" s="164"/>
+      <c r="C1795" s="164"/>
+      <c r="D1795" s="165"/>
+      <c r="E1795" s="165"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20895,9 +20927,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="163"/>
-      <c r="D1812" s="164"/>
-      <c r="E1812" s="164"/>
+      <c r="C1812" s="164"/>
+      <c r="D1812" s="165"/>
+      <c r="E1812" s="165"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -21048,9 +21080,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="163"/>
-      <c r="D1829" s="164"/>
-      <c r="E1829" s="164"/>
+      <c r="C1829" s="164"/>
+      <c r="D1829" s="165"/>
+      <c r="E1829" s="165"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -21201,9 +21233,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="163"/>
-      <c r="D1846" s="164"/>
-      <c r="E1846" s="164"/>
+      <c r="C1846" s="164"/>
+      <c r="D1846" s="165"/>
+      <c r="E1846" s="165"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21354,9 +21386,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="163"/>
-      <c r="D1863" s="164"/>
-      <c r="E1863" s="164"/>
+      <c r="C1863" s="164"/>
+      <c r="D1863" s="165"/>
+      <c r="E1863" s="165"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21507,9 +21539,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="163"/>
-      <c r="D1880" s="164"/>
-      <c r="E1880" s="164"/>
+      <c r="C1880" s="164"/>
+      <c r="D1880" s="165"/>
+      <c r="E1880" s="165"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21660,9 +21692,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="163"/>
-      <c r="D1897" s="164"/>
-      <c r="E1897" s="164"/>
+      <c r="C1897" s="164"/>
+      <c r="D1897" s="165"/>
+      <c r="E1897" s="165"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21813,18 +21845,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="179"/>
-      <c r="D1914" s="180"/>
-      <c r="E1914" s="180"/>
+      <c r="C1914" s="180"/>
+      <c r="D1914" s="181"/>
+      <c r="E1914" s="181"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="163"/>
-      <c r="D1915" s="164"/>
-      <c r="E1915" s="164"/>
+      <c r="C1915" s="164"/>
+      <c r="D1915" s="165"/>
+      <c r="E1915" s="165"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -21975,9 +22007,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="165"/>
-      <c r="D1932" s="166"/>
-      <c r="E1932" s="166"/>
+      <c r="C1932" s="166"/>
+      <c r="D1932" s="167"/>
+      <c r="E1932" s="167"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -22128,9 +22160,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="163"/>
-      <c r="D1949" s="164"/>
-      <c r="E1949" s="164"/>
+      <c r="C1949" s="164"/>
+      <c r="D1949" s="165"/>
+      <c r="E1949" s="165"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22281,9 +22313,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="163"/>
-      <c r="D1966" s="164"/>
-      <c r="E1966" s="164"/>
+      <c r="C1966" s="164"/>
+      <c r="D1966" s="165"/>
+      <c r="E1966" s="165"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22434,9 +22466,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="163"/>
-      <c r="D1983" s="164"/>
-      <c r="E1983" s="164"/>
+      <c r="C1983" s="164"/>
+      <c r="D1983" s="165"/>
+      <c r="E1983" s="165"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22587,9 +22619,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="163"/>
-      <c r="D2000" s="164"/>
-      <c r="E2000" s="164"/>
+      <c r="C2000" s="164"/>
+      <c r="D2000" s="165"/>
+      <c r="E2000" s="165"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22740,9 +22772,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="163"/>
-      <c r="D2017" s="164"/>
-      <c r="E2017" s="164"/>
+      <c r="C2017" s="164"/>
+      <c r="D2017" s="165"/>
+      <c r="E2017" s="165"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22893,9 +22925,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="163"/>
-      <c r="D2034" s="164"/>
-      <c r="E2034" s="164"/>
+      <c r="C2034" s="164"/>
+      <c r="D2034" s="165"/>
+      <c r="E2034" s="165"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -23046,9 +23078,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="163"/>
-      <c r="D2051" s="164"/>
-      <c r="E2051" s="164"/>
+      <c r="C2051" s="164"/>
+      <c r="D2051" s="165"/>
+      <c r="E2051" s="165"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -23199,9 +23231,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="163"/>
-      <c r="D2068" s="164"/>
-      <c r="E2068" s="164"/>
+      <c r="C2068" s="164"/>
+      <c r="D2068" s="165"/>
+      <c r="E2068" s="165"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23352,9 +23384,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="163"/>
-      <c r="D2085" s="164"/>
-      <c r="E2085" s="164"/>
+      <c r="C2085" s="164"/>
+      <c r="D2085" s="165"/>
+      <c r="E2085" s="165"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23505,9 +23537,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="163"/>
-      <c r="D2102" s="164"/>
-      <c r="E2102" s="164"/>
+      <c r="C2102" s="164"/>
+      <c r="D2102" s="165"/>
+      <c r="E2102" s="165"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23658,9 +23690,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="163"/>
-      <c r="D2119" s="164"/>
-      <c r="E2119" s="164"/>
+      <c r="C2119" s="164"/>
+      <c r="D2119" s="165"/>
+      <c r="E2119" s="165"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23811,9 +23843,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="163"/>
-      <c r="D2136" s="164"/>
-      <c r="E2136" s="164"/>
+      <c r="C2136" s="164"/>
+      <c r="D2136" s="165"/>
+      <c r="E2136" s="165"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23964,9 +23996,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="163"/>
-      <c r="D2153" s="164"/>
-      <c r="E2153" s="164"/>
+      <c r="C2153" s="164"/>
+      <c r="D2153" s="165"/>
+      <c r="E2153" s="165"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -24117,9 +24149,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="163"/>
-      <c r="D2170" s="164"/>
-      <c r="E2170" s="164"/>
+      <c r="C2170" s="164"/>
+      <c r="D2170" s="165"/>
+      <c r="E2170" s="165"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -24405,7 +24437,7 @@
     <mergeCell ref="C72:E72"/>
     <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24430,51 +24462,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="187" t="s">
+      <c r="A1" s="188" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="187"/>
-      <c r="C1" s="187"/>
-      <c r="D1" s="187"/>
-      <c r="E1" s="187"/>
-      <c r="F1" s="187"/>
-      <c r="G1" s="187"/>
-      <c r="H1" s="187"/>
-      <c r="I1" s="187"/>
-      <c r="J1" s="187"/>
-      <c r="K1" s="187"/>
-      <c r="L1" s="187"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+      <c r="L1" s="188"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="185" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="185"/>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
-      <c r="G2" s="185"/>
-      <c r="H2" s="185"/>
-      <c r="I2" s="185"/>
-      <c r="J2" s="185"/>
-      <c r="K2" s="185"/>
-      <c r="L2" s="186"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="187"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="181" t="s">
+      <c r="A3" s="182" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="182"/>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="182"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="183"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="183"/>
+      <c r="J3" s="183"/>
+      <c r="K3" s="184"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -24691,19 +24723,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="181" t="s">
+      <c r="A20" s="182" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="182"/>
-      <c r="C20" s="182"/>
-      <c r="D20" s="182"/>
-      <c r="E20" s="182"/>
-      <c r="F20" s="182"/>
-      <c r="G20" s="182"/>
-      <c r="H20" s="182"/>
-      <c r="I20" s="182"/>
-      <c r="J20" s="182"/>
-      <c r="K20" s="183"/>
+      <c r="B20" s="183"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="183"/>
+      <c r="E20" s="183"/>
+      <c r="F20" s="183"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="183"/>
+      <c r="I20" s="183"/>
+      <c r="J20" s="183"/>
+      <c r="K20" s="184"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -24920,19 +24952,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="181" t="s">
+      <c r="A37" s="182" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="182"/>
-      <c r="C37" s="182"/>
-      <c r="D37" s="182"/>
-      <c r="E37" s="182"/>
-      <c r="F37" s="182"/>
-      <c r="G37" s="182"/>
-      <c r="H37" s="182"/>
-      <c r="I37" s="182"/>
-      <c r="J37" s="182"/>
-      <c r="K37" s="183"/>
+      <c r="B37" s="183"/>
+      <c r="C37" s="183"/>
+      <c r="D37" s="183"/>
+      <c r="E37" s="183"/>
+      <c r="F37" s="183"/>
+      <c r="G37" s="183"/>
+      <c r="H37" s="183"/>
+      <c r="I37" s="183"/>
+      <c r="J37" s="183"/>
+      <c r="K37" s="184"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -25156,7 +25188,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25190,28 +25222,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="188"/>
+      <c r="A3" s="189"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="189"/>
+      <c r="A4" s="190"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="189"/>
+      <c r="A5" s="190"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="189"/>
+      <c r="A6" s="190"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="189"/>
+      <c r="A7" s="190"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="189"/>
+      <c r="A8" s="190"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="189"/>
+      <c r="A9" s="190"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="190"/>
+      <c r="A10" s="191"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -25367,7 +25399,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25394,10 +25426,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="191" t="s">
+      <c r="B1" s="192" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="192"/>
+      <c r="C1" s="193"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25408,7 +25440,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="193" t="s">
+      <c r="A3" s="194" t="s">
         <v>213</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25422,7 +25454,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="194"/>
+      <c r="A4" s="195"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25434,7 +25466,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="194"/>
+      <c r="A5" s="195"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25443,7 +25475,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="194"/>
+      <c r="A6" s="195"/>
       <c r="B6" s="139" t="s">
         <v>215</v>
       </c>
@@ -25455,7 +25487,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="194"/>
+      <c r="A7" s="195"/>
       <c r="B7" s="128" t="s">
         <v>178</v>
       </c>
@@ -25467,7 +25499,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="194"/>
+      <c r="A8" s="195"/>
       <c r="B8" s="128" t="s">
         <v>179</v>
       </c>
@@ -25476,7 +25508,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="195"/>
+      <c r="A9" s="196"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25491,7 +25523,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="193" t="s">
+      <c r="A11" s="194" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25505,7 +25537,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="194"/>
+      <c r="A12" s="195"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25517,7 +25549,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="194"/>
+      <c r="A13" s="195"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25526,7 +25558,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="194"/>
+      <c r="A14" s="195"/>
       <c r="B14" s="139" t="s">
         <v>215</v>
       </c>
@@ -25538,7 +25570,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="194"/>
+      <c r="A15" s="195"/>
       <c r="B15" s="128" t="s">
         <v>178</v>
       </c>
@@ -25550,7 +25582,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="194"/>
+      <c r="A16" s="195"/>
       <c r="B16" s="128" t="s">
         <v>179</v>
       </c>
@@ -25559,7 +25591,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="195"/>
+      <c r="A17" s="196"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25574,7 +25606,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="193" t="s">
+      <c r="A19" s="194" t="s">
         <v>214</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25583,7 +25615,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="194"/>
+      <c r="A20" s="195"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25593,14 +25625,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="194"/>
+      <c r="A21" s="195"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="194"/>
+      <c r="A22" s="195"/>
       <c r="B22" s="139" t="s">
         <v>215</v>
       </c>
@@ -25610,7 +25642,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="194"/>
+      <c r="A23" s="195"/>
       <c r="B23" s="128" t="s">
         <v>178</v>
       </c>
@@ -25620,14 +25652,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="194"/>
+      <c r="A24" s="195"/>
       <c r="B24" s="128" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="195"/>
+      <c r="A25" s="196"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25640,7 +25672,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25662,147 +25694,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="206" t="s">
+      <c r="A1" s="207" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="207"/>
+      <c r="B1" s="208"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="212" t="s">
+      <c r="A2" s="213" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="213"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="214" t="s">
+      <c r="A3" s="215" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="213"/>
+      <c r="B3" s="214"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="210"/>
-      <c r="B4" s="211"/>
+      <c r="A4" s="211"/>
+      <c r="B4" s="212"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="208" t="s">
+      <c r="A5" s="209" t="s">
         <v>205</v>
       </c>
-      <c r="B5" s="209"/>
+      <c r="B5" s="210"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="200" t="s">
+      <c r="A7" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="B7" s="201"/>
+      <c r="B7" s="202"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="202" t="s">
+      <c r="A9" s="203" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="203"/>
+      <c r="B9" s="204"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="204"/>
-      <c r="B10" s="205"/>
+      <c r="A10" s="205"/>
+      <c r="B10" s="206"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="196" t="s">
+      <c r="A11" s="197" t="s">
         <v>199</v>
       </c>
-      <c r="B11" s="197"/>
+      <c r="B11" s="198"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="196" t="s">
+      <c r="A12" s="197" t="s">
         <v>200</v>
       </c>
-      <c r="B12" s="197"/>
+      <c r="B12" s="198"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="196" t="s">
+      <c r="A13" s="197" t="s">
         <v>201</v>
       </c>
-      <c r="B13" s="197"/>
+      <c r="B13" s="198"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="196" t="s">
+      <c r="A14" s="197" t="s">
         <v>202</v>
       </c>
-      <c r="B14" s="197"/>
+      <c r="B14" s="198"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="196" t="s">
+      <c r="A15" s="197" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="197"/>
+      <c r="B15" s="198"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="196" t="s">
+      <c r="A16" s="197" t="s">
         <v>204</v>
       </c>
-      <c r="B16" s="197"/>
+      <c r="B16" s="198"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="198" t="s">
+      <c r="A17" s="199" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="199"/>
+      <c r="B17" s="200"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="200" t="s">
+      <c r="A19" s="201" t="s">
         <v>208</v>
       </c>
-      <c r="B19" s="201"/>
+      <c r="B19" s="202"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="202" t="s">
+      <c r="A21" s="203" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="203"/>
+      <c r="B21" s="204"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="204"/>
-      <c r="B22" s="205"/>
+      <c r="A22" s="205"/>
+      <c r="B22" s="206"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="196" t="s">
+      <c r="A23" s="197" t="s">
         <v>210</v>
       </c>
-      <c r="B23" s="197"/>
+      <c r="B23" s="198"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="196"/>
-      <c r="B24" s="197"/>
+      <c r="A24" s="197"/>
+      <c r="B24" s="198"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="196" t="s">
+      <c r="A25" s="197" t="s">
         <v>211</v>
       </c>
-      <c r="B25" s="197"/>
+      <c r="B25" s="198"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="196" t="s">
+      <c r="A26" s="197" t="s">
         <v>212</v>
       </c>
-      <c r="B26" s="197"/>
+      <c r="B26" s="198"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="198"/>
-      <c r="B27" s="199"/>
+      <c r="A27" s="199"/>
+      <c r="B27" s="200"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
Flintstones - some of level 4 done, proving you don't need to use an egg at the beginning, saving 10 weapon points.  This is enough to use one on the boss of level 3 instead.  Need to redo now!
</commit_message>
<xml_diff>
--- a/Flintstones/Compare/Flintstones.xlsx
+++ b/Flintstones/Compare/Flintstones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="231">
   <si>
     <t>Notes</t>
   </si>
@@ -747,6 +747,12 @@
   <si>
     <t>losing 9 frames to save weapon energy for later</t>
   </si>
+  <si>
+    <t>Fred Appears</t>
+  </si>
+  <si>
+    <t>1st Grab</t>
+  </si>
 </sst>
 </file>
 
@@ -756,10 +762,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1699,34 +1712,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1734,208 +1747,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1945,10 +1958,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1969,18 +1982,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1990,126 +2006,126 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2427,8 +2443,8 @@
   <dimension ref="A1:K159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
+      <pane ySplit="6" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2444,16 +2460,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="158" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="158" t="s">
+      <c r="B1" s="157"/>
+      <c r="C1" s="159" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="160"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65541)</f>
@@ -2531,10 +2547,10 @@
       <c r="B5" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="155" t="s">
+      <c r="C5" s="156" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="155"/>
+      <c r="D5" s="156"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2550,10 +2566,10 @@
       <c r="B6" s="147" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="155" t="s">
+      <c r="C6" s="156" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="156"/>
+      <c r="D6" s="157"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2571,7 +2587,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="160" t="s">
+      <c r="A8" s="161" t="s">
         <v>190</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2591,7 +2607,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="153"/>
+      <c r="A9" s="154"/>
       <c r="B9" s="98" t="s">
         <v>185</v>
       </c>
@@ -2601,7 +2617,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="153"/>
+      <c r="A10" s="154"/>
       <c r="B10" s="100"/>
       <c r="C10" s="101"/>
       <c r="D10" s="101"/>
@@ -2612,7 +2628,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="153"/>
+      <c r="A11" s="154"/>
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
       <c r="D11" s="101"/>
@@ -2623,7 +2639,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="153"/>
+      <c r="A12" s="154"/>
       <c r="B12" s="100"/>
       <c r="C12" s="101"/>
       <c r="D12" s="101"/>
@@ -2634,7 +2650,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="153"/>
+      <c r="A13" s="154"/>
       <c r="B13" s="100"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
@@ -2645,7 +2661,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="153"/>
+      <c r="A14" s="154"/>
       <c r="B14" s="100"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
@@ -2656,7 +2672,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="153"/>
+      <c r="A15" s="154"/>
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
@@ -2667,7 +2683,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="153"/>
+      <c r="A16" s="154"/>
       <c r="B16" s="98" t="s">
         <v>188</v>
       </c>
@@ -2710,7 +2726,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="154" t="s">
+      <c r="A19" s="155" t="s">
         <v>168</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2730,7 +2746,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="153"/>
+      <c r="A20" s="154"/>
       <c r="B20" s="98" t="s">
         <v>185</v>
       </c>
@@ -2743,7 +2759,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="153"/>
+      <c r="A21" s="154"/>
       <c r="B21" s="100"/>
       <c r="C21" s="101"/>
       <c r="D21" s="101"/>
@@ -2754,7 +2770,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="153"/>
+      <c r="A22" s="154"/>
       <c r="B22" s="100"/>
       <c r="C22" s="101"/>
       <c r="D22" s="101"/>
@@ -2765,7 +2781,7 @@
       <c r="F22" s="105"/>
     </row>
     <row r="23" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="153"/>
+      <c r="A23" s="154"/>
       <c r="B23" s="100"/>
       <c r="C23" s="101"/>
       <c r="D23" s="101"/>
@@ -2776,7 +2792,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="153"/>
+      <c r="A24" s="154"/>
       <c r="B24" s="100"/>
       <c r="C24" s="101"/>
       <c r="D24" s="101"/>
@@ -2787,7 +2803,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="153"/>
+      <c r="A25" s="154"/>
       <c r="B25" s="100"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -2798,7 +2814,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="153"/>
+      <c r="A26" s="154"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -2809,7 +2825,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="153"/>
+      <c r="A27" s="154"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -2820,7 +2836,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="153"/>
+      <c r="A28" s="154"/>
       <c r="B28" s="100"/>
       <c r="C28" s="101"/>
       <c r="D28" s="101"/>
@@ -2831,7 +2847,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="153"/>
+      <c r="A29" s="154"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
       <c r="D29" s="101"/>
@@ -2842,7 +2858,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="153"/>
+      <c r="A30" s="154"/>
       <c r="B30" s="100"/>
       <c r="C30" s="101"/>
       <c r="D30" s="101"/>
@@ -2853,7 +2869,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="153"/>
+      <c r="A31" s="154"/>
       <c r="B31" s="100"/>
       <c r="C31" s="101"/>
       <c r="D31" s="101"/>
@@ -2864,7 +2880,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="153"/>
+      <c r="A32" s="154"/>
       <c r="B32" s="100"/>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2875,7 +2891,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="153"/>
+      <c r="A33" s="154"/>
       <c r="B33" s="98" t="s">
         <v>188</v>
       </c>
@@ -2914,7 +2930,7 @@
     </row>
     <row r="35" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="152" t="s">
+      <c r="A36" s="153" t="s">
         <v>170</v>
       </c>
       <c r="B36" s="113" t="s">
@@ -2934,7 +2950,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="153"/>
+      <c r="A37" s="154"/>
       <c r="B37" s="98" t="s">
         <v>185</v>
       </c>
@@ -2951,7 +2967,7 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="153"/>
+      <c r="A38" s="154"/>
       <c r="B38" s="148" t="s">
         <v>216</v>
       </c>
@@ -2968,7 +2984,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="153"/>
+      <c r="A39" s="154"/>
       <c r="B39" s="148" t="s">
         <v>217</v>
       </c>
@@ -2985,7 +3001,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="153"/>
+      <c r="A40" s="154"/>
       <c r="B40" s="148" t="s">
         <v>218</v>
       </c>
@@ -3002,7 +3018,7 @@
       <c r="F40" s="105"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="153"/>
+      <c r="A41" s="154"/>
       <c r="B41" s="148" t="s">
         <v>219</v>
       </c>
@@ -3019,7 +3035,7 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="153"/>
+      <c r="A42" s="154"/>
       <c r="B42" s="148" t="s">
         <v>217</v>
       </c>
@@ -3036,7 +3052,7 @@
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="153"/>
+      <c r="A43" s="154"/>
       <c r="B43" s="148" t="s">
         <v>220</v>
       </c>
@@ -3053,7 +3069,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="153"/>
+      <c r="A44" s="154"/>
       <c r="B44" s="148" t="s">
         <v>221</v>
       </c>
@@ -3070,7 +3086,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="153"/>
+      <c r="A45" s="154"/>
       <c r="B45" s="148" t="s">
         <v>169</v>
       </c>
@@ -3087,7 +3103,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="153"/>
+      <c r="A46" s="154"/>
       <c r="B46" s="148" t="s">
         <v>217</v>
       </c>
@@ -3104,7 +3120,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="153"/>
+      <c r="A47" s="154"/>
       <c r="B47" s="148" t="s">
         <v>169</v>
       </c>
@@ -3121,7 +3137,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="153"/>
+      <c r="A48" s="154"/>
       <c r="B48" s="148" t="s">
         <v>216</v>
       </c>
@@ -3138,7 +3154,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="153"/>
+      <c r="A49" s="154"/>
       <c r="B49" s="148" t="s">
         <v>217</v>
       </c>
@@ -3155,7 +3171,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="153"/>
+      <c r="A50" s="154"/>
       <c r="B50" s="148" t="s">
         <v>169</v>
       </c>
@@ -3172,7 +3188,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="153"/>
+      <c r="A51" s="154"/>
       <c r="B51" s="148"/>
       <c r="C51" s="101"/>
       <c r="D51" s="101"/>
@@ -3180,7 +3196,7 @@
       <c r="F51" s="105"/>
     </row>
     <row r="52" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="153"/>
+      <c r="A52" s="154"/>
       <c r="B52" s="148"/>
       <c r="C52" s="101"/>
       <c r="D52" s="101"/>
@@ -3188,7 +3204,7 @@
       <c r="F52" s="105"/>
     </row>
     <row r="53" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="153"/>
+      <c r="A53" s="154"/>
       <c r="B53" s="100"/>
       <c r="C53" s="101"/>
       <c r="D53" s="101"/>
@@ -3199,7 +3215,7 @@
       <c r="F53" s="105"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="153"/>
+      <c r="A54" s="154"/>
       <c r="B54" s="98" t="s">
         <v>188</v>
       </c>
@@ -3242,7 +3258,7 @@
     </row>
     <row r="56" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="154" t="s">
+      <c r="A57" s="155" t="s">
         <v>171</v>
       </c>
       <c r="B57" s="109" t="s">
@@ -3262,7 +3278,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="153"/>
+      <c r="A58" s="154"/>
       <c r="B58" s="98" t="s">
         <v>185</v>
       </c>
@@ -3279,7 +3295,7 @@
       <c r="F58" s="104"/>
     </row>
     <row r="59" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="153"/>
+      <c r="A59" s="154"/>
       <c r="B59" s="148" t="s">
         <v>216</v>
       </c>
@@ -3296,7 +3312,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="153"/>
+      <c r="A60" s="154"/>
       <c r="B60" s="148" t="s">
         <v>217</v>
       </c>
@@ -3313,7 +3329,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="153"/>
+      <c r="A61" s="154"/>
       <c r="B61" s="148" t="s">
         <v>222</v>
       </c>
@@ -3328,7 +3344,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="153"/>
+      <c r="A62" s="154"/>
       <c r="B62" s="148" t="s">
         <v>217</v>
       </c>
@@ -3345,7 +3361,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="153"/>
+      <c r="A63" s="154"/>
       <c r="B63" s="148" t="s">
         <v>217</v>
       </c>
@@ -3362,7 +3378,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="153"/>
+      <c r="A64" s="154"/>
       <c r="B64" s="148" t="s">
         <v>223</v>
       </c>
@@ -3377,7 +3393,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="153"/>
+      <c r="A65" s="154"/>
       <c r="B65" s="148" t="s">
         <v>217</v>
       </c>
@@ -3394,7 +3410,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="153"/>
+      <c r="A66" s="154"/>
       <c r="B66" s="148" t="s">
         <v>224</v>
       </c>
@@ -3411,7 +3427,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="153"/>
+      <c r="A67" s="154"/>
       <c r="B67" s="148" t="s">
         <v>225</v>
       </c>
@@ -3428,7 +3444,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="153"/>
+      <c r="A68" s="154"/>
       <c r="B68" s="149" t="s">
         <v>217</v>
       </c>
@@ -3445,7 +3461,7 @@
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="153"/>
+      <c r="A69" s="154"/>
       <c r="B69" s="150" t="s">
         <v>226</v>
       </c>
@@ -3462,7 +3478,7 @@
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="153"/>
+      <c r="A70" s="154"/>
       <c r="B70" s="150" t="s">
         <v>217</v>
       </c>
@@ -3479,7 +3495,7 @@
       <c r="F70" s="105"/>
     </row>
     <row r="71" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="153"/>
+      <c r="A71" s="154"/>
       <c r="B71" s="151" t="s">
         <v>227</v>
       </c>
@@ -3493,12 +3509,12 @@
         <f t="shared" si="3"/>
         <v>1134</v>
       </c>
-      <c r="F71" s="216" t="s">
+      <c r="F71" s="152" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="153"/>
+      <c r="A72" s="154"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
@@ -3509,15 +3525,19 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="153"/>
+      <c r="A73" s="154"/>
       <c r="B73" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="C73" s="99"/>
-      <c r="D73" s="99"/>
+      <c r="C73" s="99">
+        <v>18322</v>
+      </c>
+      <c r="D73" s="99">
+        <v>19456</v>
+      </c>
       <c r="E73" s="125">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1134</v>
       </c>
       <c r="F73" s="104"/>
     </row>
@@ -3530,25 +3550,25 @@
       </c>
       <c r="C74" s="103">
         <f>C73-C58</f>
-        <v>-14121</v>
+        <v>4201</v>
       </c>
       <c r="D74" s="103">
         <f>D73-D58</f>
-        <v>-14144</v>
+        <v>5312</v>
       </c>
       <c r="E74" s="126">
         <f>E73-E58</f>
-        <v>-23</v>
+        <v>1111</v>
       </c>
       <c r="F74" s="108"/>
       <c r="G74" s="112">
         <f>E74</f>
-        <v>-23</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="152" t="s">
+    <row r="76" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="153" t="s">
         <v>172</v>
       </c>
       <c r="B76" s="113" t="s">
@@ -3567,43 +3587,59 @@
         <v>184</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="153"/>
+    <row r="77" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="154"/>
       <c r="B77" s="98" t="s">
         <v>185</v>
       </c>
-      <c r="C77" s="99"/>
-      <c r="D77" s="99"/>
+      <c r="C77" s="99">
+        <v>18322</v>
+      </c>
+      <c r="D77" s="99">
+        <v>19456</v>
+      </c>
       <c r="E77" s="123">
         <f t="shared" ref="E77:E90" si="4">IF(AND(C77&gt;0,D77&gt;0), D77-C77, 0)</f>
-        <v>0</v>
+        <v>1134</v>
       </c>
       <c r="F77" s="104"/>
     </row>
-    <row r="78" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="153"/>
-      <c r="B78" s="100"/>
-      <c r="C78" s="101"/>
-      <c r="D78" s="101"/>
+    <row r="78" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="154"/>
+      <c r="B78" s="217" t="s">
+        <v>229</v>
+      </c>
+      <c r="C78" s="101">
+        <v>18322</v>
+      </c>
+      <c r="D78" s="101">
+        <v>19456</v>
+      </c>
       <c r="E78" s="124">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1134</v>
       </c>
       <c r="F78" s="105"/>
     </row>
-    <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="153"/>
-      <c r="B79" s="100"/>
-      <c r="C79" s="101"/>
-      <c r="D79" s="101"/>
+    <row r="79" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="154"/>
+      <c r="B79" s="217" t="s">
+        <v>230</v>
+      </c>
+      <c r="C79" s="101">
+        <v>18499</v>
+      </c>
+      <c r="D79" s="101">
+        <v>19634</v>
+      </c>
       <c r="E79" s="123">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1135</v>
       </c>
       <c r="F79" s="105"/>
     </row>
-    <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="153"/>
+    <row r="80" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="154"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3613,8 +3649,8 @@
       </c>
       <c r="F80" s="105"/>
     </row>
-    <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="153"/>
+    <row r="81" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="154"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3624,8 +3660,8 @@
       </c>
       <c r="F81" s="105"/>
     </row>
-    <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="153"/>
+    <row r="82" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="154"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3635,8 +3671,8 @@
       </c>
       <c r="F82" s="105"/>
     </row>
-    <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="153"/>
+    <row r="83" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="154"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3646,8 +3682,8 @@
       </c>
       <c r="F83" s="105"/>
     </row>
-    <row r="84" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="153"/>
+    <row r="84" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="154"/>
       <c r="B84" s="100"/>
       <c r="C84" s="101"/>
       <c r="D84" s="101"/>
@@ -3657,8 +3693,8 @@
       </c>
       <c r="F84" s="105"/>
     </row>
-    <row r="85" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="153"/>
+    <row r="85" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="154"/>
       <c r="B85" s="100"/>
       <c r="C85" s="101"/>
       <c r="D85" s="101"/>
@@ -3668,8 +3704,8 @@
       </c>
       <c r="F85" s="105"/>
     </row>
-    <row r="86" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="153"/>
+    <row r="86" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="154"/>
       <c r="B86" s="100"/>
       <c r="C86" s="101"/>
       <c r="D86" s="101"/>
@@ -3679,8 +3715,8 @@
       </c>
       <c r="F86" s="105"/>
     </row>
-    <row r="87" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="153"/>
+    <row r="87" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="154"/>
       <c r="B87" s="100"/>
       <c r="C87" s="101"/>
       <c r="D87" s="101"/>
@@ -3690,8 +3726,8 @@
       </c>
       <c r="F87" s="105"/>
     </row>
-    <row r="88" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="153"/>
+    <row r="88" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="154"/>
       <c r="B88" s="100"/>
       <c r="C88" s="101"/>
       <c r="D88" s="101"/>
@@ -3701,8 +3737,8 @@
       </c>
       <c r="F88" s="105"/>
     </row>
-    <row r="89" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="153"/>
+    <row r="89" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="154"/>
       <c r="B89" s="100"/>
       <c r="C89" s="101"/>
       <c r="D89" s="101"/>
@@ -3712,8 +3748,8 @@
       </c>
       <c r="F89" s="105"/>
     </row>
-    <row r="90" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="153"/>
+    <row r="90" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="154"/>
       <c r="B90" s="98" t="s">
         <v>188</v>
       </c>
@@ -3725,7 +3761,7 @@
       </c>
       <c r="F90" s="104"/>
     </row>
-    <row r="91" spans="1:7" ht="17.25" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="116">
         <v>4</v>
       </c>
@@ -3734,25 +3770,25 @@
       </c>
       <c r="C91" s="103">
         <f>C90-C77</f>
-        <v>0</v>
+        <v>-18322</v>
       </c>
       <c r="D91" s="103">
         <f>D90-D77</f>
-        <v>0</v>
+        <v>-19456</v>
       </c>
       <c r="E91" s="126">
         <f>E90-E77</f>
-        <v>0</v>
+        <v>-1134</v>
       </c>
       <c r="F91" s="107"/>
       <c r="G91" s="112">
         <f>E91</f>
-        <v>0</v>
+        <v>-1134</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="93" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="154" t="s">
+      <c r="A93" s="155" t="s">
         <v>173</v>
       </c>
       <c r="B93" s="109" t="s">
@@ -3772,7 +3808,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="153"/>
+      <c r="A94" s="154"/>
       <c r="B94" s="98" t="s">
         <v>185</v>
       </c>
@@ -3785,7 +3821,7 @@
       <c r="F94" s="104"/>
     </row>
     <row r="95" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="153"/>
+      <c r="A95" s="154"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3796,7 +3832,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="153"/>
+      <c r="A96" s="154"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3807,7 +3843,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="153"/>
+      <c r="A97" s="154"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3818,7 +3854,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="153"/>
+      <c r="A98" s="154"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3829,7 +3865,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="153"/>
+      <c r="A99" s="154"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3840,7 +3876,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="153"/>
+      <c r="A100" s="154"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3851,7 +3887,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="153"/>
+      <c r="A101" s="154"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -3862,7 +3898,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="153"/>
+      <c r="A102" s="154"/>
       <c r="B102" s="100"/>
       <c r="C102" s="101"/>
       <c r="D102" s="101"/>
@@ -3873,7 +3909,7 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="153"/>
+      <c r="A103" s="154"/>
       <c r="B103" s="100"/>
       <c r="C103" s="101"/>
       <c r="D103" s="101"/>
@@ -3884,7 +3920,7 @@
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="153"/>
+      <c r="A104" s="154"/>
       <c r="B104" s="100"/>
       <c r="C104" s="101"/>
       <c r="D104" s="101"/>
@@ -3895,7 +3931,7 @@
       <c r="F104" s="105"/>
     </row>
     <row r="105" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="153"/>
+      <c r="A105" s="154"/>
       <c r="B105" s="100"/>
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
@@ -3906,7 +3942,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="153"/>
+      <c r="A106" s="154"/>
       <c r="B106" s="100"/>
       <c r="C106" s="101"/>
       <c r="D106" s="101"/>
@@ -3917,7 +3953,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="153"/>
+      <c r="A107" s="154"/>
       <c r="B107" s="98" t="s">
         <v>188</v>
       </c>
@@ -3955,7 +3991,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="152" t="s">
+      <c r="A110" s="153" t="s">
         <v>174</v>
       </c>
       <c r="B110" s="113" t="s">
@@ -3975,7 +4011,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="153"/>
+      <c r="A111" s="154"/>
       <c r="B111" s="98" t="s">
         <v>185</v>
       </c>
@@ -3988,7 +4024,7 @@
       <c r="F111" s="104"/>
     </row>
     <row r="112" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="153"/>
+      <c r="A112" s="154"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3999,7 +4035,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="153"/>
+      <c r="A113" s="154"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -4010,7 +4046,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="153"/>
+      <c r="A114" s="154"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -4021,7 +4057,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="153"/>
+      <c r="A115" s="154"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -4032,7 +4068,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="153"/>
+      <c r="A116" s="154"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -4043,7 +4079,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="153"/>
+      <c r="A117" s="154"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -4054,7 +4090,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="153"/>
+      <c r="A118" s="154"/>
       <c r="B118" s="100"/>
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
@@ -4065,7 +4101,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="153"/>
+      <c r="A119" s="154"/>
       <c r="B119" s="100"/>
       <c r="C119" s="101"/>
       <c r="D119" s="101"/>
@@ -4076,7 +4112,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="153"/>
+      <c r="A120" s="154"/>
       <c r="B120" s="100"/>
       <c r="C120" s="101"/>
       <c r="D120" s="101"/>
@@ -4087,7 +4123,7 @@
       <c r="F120" s="105"/>
     </row>
     <row r="121" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="153"/>
+      <c r="A121" s="154"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -4098,7 +4134,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="153"/>
+      <c r="A122" s="154"/>
       <c r="B122" s="100"/>
       <c r="C122" s="101"/>
       <c r="D122" s="101"/>
@@ -4109,7 +4145,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="153"/>
+      <c r="A123" s="154"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -4120,7 +4156,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="153"/>
+      <c r="A124" s="154"/>
       <c r="B124" s="98" t="s">
         <v>188</v>
       </c>
@@ -4158,7 +4194,7 @@
       </c>
     </row>
     <row r="127" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="154" t="s">
+      <c r="A127" s="155" t="s">
         <v>175</v>
       </c>
       <c r="B127" s="109" t="s">
@@ -4178,7 +4214,7 @@
       </c>
     </row>
     <row r="128" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="153"/>
+      <c r="A128" s="154"/>
       <c r="B128" s="98" t="s">
         <v>185</v>
       </c>
@@ -4191,7 +4227,7 @@
       <c r="F128" s="104"/>
     </row>
     <row r="129" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="153"/>
+      <c r="A129" s="154"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4202,7 +4238,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="153"/>
+      <c r="A130" s="154"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4213,7 +4249,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="153"/>
+      <c r="A131" s="154"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4224,7 +4260,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="153"/>
+      <c r="A132" s="154"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4235,7 +4271,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="153"/>
+      <c r="A133" s="154"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4246,7 +4282,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="153"/>
+      <c r="A134" s="154"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4257,7 +4293,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="153"/>
+      <c r="A135" s="154"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4268,7 +4304,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="153"/>
+      <c r="A136" s="154"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
       <c r="D136" s="101"/>
@@ -4279,7 +4315,7 @@
       <c r="F136" s="105"/>
     </row>
     <row r="137" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="153"/>
+      <c r="A137" s="154"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4290,7 +4326,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="153"/>
+      <c r="A138" s="154"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4301,7 +4337,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="153"/>
+      <c r="A139" s="154"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4312,7 +4348,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="153"/>
+      <c r="A140" s="154"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4323,7 +4359,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="153"/>
+      <c r="A141" s="154"/>
       <c r="B141" s="98" t="s">
         <v>188</v>
       </c>
@@ -4361,7 +4397,7 @@
       </c>
     </row>
     <row r="144" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A144" s="152" t="s">
+      <c r="A144" s="153" t="s">
         <v>176</v>
       </c>
       <c r="B144" s="113" t="s">
@@ -4381,7 +4417,7 @@
       </c>
     </row>
     <row r="145" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="153"/>
+      <c r="A145" s="154"/>
       <c r="B145" s="98" t="s">
         <v>185</v>
       </c>
@@ -4394,7 +4430,7 @@
       <c r="F145" s="104"/>
     </row>
     <row r="146" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="153"/>
+      <c r="A146" s="154"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4405,7 +4441,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A147" s="153"/>
+      <c r="A147" s="154"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4416,7 +4452,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A148" s="153"/>
+      <c r="A148" s="154"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4427,7 +4463,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A149" s="153"/>
+      <c r="A149" s="154"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
@@ -4438,7 +4474,7 @@
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A150" s="153"/>
+      <c r="A150" s="154"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -4449,7 +4485,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A151" s="153"/>
+      <c r="A151" s="154"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -4460,7 +4496,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A152" s="153"/>
+      <c r="A152" s="154"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
@@ -4471,7 +4507,7 @@
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A153" s="153"/>
+      <c r="A153" s="154"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
@@ -4482,7 +4518,7 @@
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A154" s="153"/>
+      <c r="A154" s="154"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -4493,7 +4529,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A155" s="153"/>
+      <c r="A155" s="154"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
@@ -4504,7 +4540,7 @@
       <c r="F155" s="105"/>
     </row>
     <row r="156" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A156" s="153"/>
+      <c r="A156" s="154"/>
       <c r="B156" s="100"/>
       <c r="C156" s="101"/>
       <c r="D156" s="101"/>
@@ -4515,7 +4551,7 @@
       <c r="F156" s="105"/>
     </row>
     <row r="157" spans="1:7" ht="15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A157" s="153"/>
+      <c r="A157" s="154"/>
       <c r="B157" s="100"/>
       <c r="C157" s="101"/>
       <c r="D157" s="101"/>
@@ -4526,7 +4562,7 @@
       <c r="F157" s="105"/>
     </row>
     <row r="158" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="153"/>
+      <c r="A158" s="154"/>
       <c r="B158" s="98" t="s">
         <v>188</v>
       </c>
@@ -4565,11 +4601,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A144:A158"/>
-    <mergeCell ref="A110:A124"/>
-    <mergeCell ref="A76:A90"/>
-    <mergeCell ref="A127:A141"/>
-    <mergeCell ref="A93:A107"/>
     <mergeCell ref="A36:A54"/>
     <mergeCell ref="A57:A73"/>
     <mergeCell ref="C5:D5"/>
@@ -4578,6 +4609,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A33"/>
+    <mergeCell ref="A144:A158"/>
+    <mergeCell ref="A110:A124"/>
+    <mergeCell ref="A76:A90"/>
+    <mergeCell ref="A127:A141"/>
+    <mergeCell ref="A93:A107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4609,13 +4645,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="180" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4645,18 +4681,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
@@ -4808,9 +4844,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="164"/>
+      <c r="D21" s="165"/>
+      <c r="E21" s="165"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
@@ -4961,9 +4997,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="164"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="165"/>
+      <c r="C38" s="162"/>
+      <c r="D38" s="163"/>
+      <c r="E38" s="163"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
@@ -5114,9 +5150,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="164"/>
-      <c r="D55" s="165"/>
-      <c r="E55" s="165"/>
+      <c r="C55" s="162"/>
+      <c r="D55" s="163"/>
+      <c r="E55" s="163"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
@@ -5267,9 +5303,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="164"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="165"/>
+      <c r="C72" s="162"/>
+      <c r="D72" s="163"/>
+      <c r="E72" s="163"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A73" s="47">
@@ -5420,9 +5456,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="164"/>
-      <c r="D89" s="165"/>
-      <c r="E89" s="165"/>
+      <c r="C89" s="162"/>
+      <c r="D89" s="163"/>
+      <c r="E89" s="163"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="47">
@@ -5573,9 +5609,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="164"/>
-      <c r="D106" s="165"/>
-      <c r="E106" s="165"/>
+      <c r="C106" s="162"/>
+      <c r="D106" s="163"/>
+      <c r="E106" s="163"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="47">
@@ -5726,9 +5762,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="164"/>
-      <c r="D123" s="165"/>
-      <c r="E123" s="165"/>
+      <c r="C123" s="162"/>
+      <c r="D123" s="163"/>
+      <c r="E123" s="163"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A124" s="47">
@@ -5879,9 +5915,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="164"/>
-      <c r="D140" s="165"/>
-      <c r="E140" s="165"/>
+      <c r="C140" s="162"/>
+      <c r="D140" s="163"/>
+      <c r="E140" s="163"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A141" s="47">
@@ -6032,9 +6068,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="164"/>
-      <c r="D157" s="165"/>
-      <c r="E157" s="165"/>
+      <c r="C157" s="162"/>
+      <c r="D157" s="163"/>
+      <c r="E157" s="163"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A158" s="47">
@@ -6185,9 +6221,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="164"/>
-      <c r="D174" s="165"/>
-      <c r="E174" s="165"/>
+      <c r="C174" s="162"/>
+      <c r="D174" s="163"/>
+      <c r="E174" s="163"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A175" s="47">
@@ -6338,9 +6374,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="164"/>
-      <c r="D191" s="165"/>
-      <c r="E191" s="165"/>
+      <c r="C191" s="162"/>
+      <c r="D191" s="163"/>
+      <c r="E191" s="163"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A192" s="47">
@@ -6491,9 +6527,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="164"/>
-      <c r="D208" s="165"/>
-      <c r="E208" s="165"/>
+      <c r="C208" s="162"/>
+      <c r="D208" s="163"/>
+      <c r="E208" s="163"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A209" s="47">
@@ -6644,9 +6680,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="164"/>
-      <c r="D225" s="165"/>
-      <c r="E225" s="165"/>
+      <c r="C225" s="162"/>
+      <c r="D225" s="163"/>
+      <c r="E225" s="163"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A226" s="47">
@@ -6797,9 +6833,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="164"/>
-      <c r="D242" s="165"/>
-      <c r="E242" s="165"/>
+      <c r="C242" s="162"/>
+      <c r="D242" s="163"/>
+      <c r="E242" s="163"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A243" s="47">
@@ -6950,9 +6986,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="164"/>
-      <c r="D259" s="165"/>
-      <c r="E259" s="165"/>
+      <c r="C259" s="162"/>
+      <c r="D259" s="163"/>
+      <c r="E259" s="163"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A260" s="47">
@@ -7103,18 +7139,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="168"/>
-      <c r="D276" s="169"/>
-      <c r="E276" s="169"/>
+      <c r="C276" s="178"/>
+      <c r="D276" s="179"/>
+      <c r="E276" s="179"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="164"/>
-      <c r="D277" s="165"/>
-      <c r="E277" s="165"/>
+      <c r="C277" s="162"/>
+      <c r="D277" s="163"/>
+      <c r="E277" s="163"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A278" s="52">
@@ -7265,9 +7301,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="166"/>
-      <c r="D294" s="167"/>
-      <c r="E294" s="167"/>
+      <c r="C294" s="164"/>
+      <c r="D294" s="165"/>
+      <c r="E294" s="165"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A295" s="52">
@@ -7418,9 +7454,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="164"/>
-      <c r="D311" s="165"/>
-      <c r="E311" s="165"/>
+      <c r="C311" s="162"/>
+      <c r="D311" s="163"/>
+      <c r="E311" s="163"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A312" s="52">
@@ -7571,9 +7607,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="164"/>
-      <c r="D328" s="165"/>
-      <c r="E328" s="165"/>
+      <c r="C328" s="162"/>
+      <c r="D328" s="163"/>
+      <c r="E328" s="163"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A329" s="52">
@@ -7724,9 +7760,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="164"/>
-      <c r="D345" s="165"/>
-      <c r="E345" s="165"/>
+      <c r="C345" s="162"/>
+      <c r="D345" s="163"/>
+      <c r="E345" s="163"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A346" s="52">
@@ -7877,9 +7913,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="164"/>
-      <c r="D362" s="165"/>
-      <c r="E362" s="165"/>
+      <c r="C362" s="162"/>
+      <c r="D362" s="163"/>
+      <c r="E362" s="163"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A363" s="52">
@@ -8030,9 +8066,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="164"/>
-      <c r="D379" s="165"/>
-      <c r="E379" s="165"/>
+      <c r="C379" s="162"/>
+      <c r="D379" s="163"/>
+      <c r="E379" s="163"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A380" s="52">
@@ -8183,9 +8219,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="164"/>
-      <c r="D396" s="165"/>
-      <c r="E396" s="165"/>
+      <c r="C396" s="162"/>
+      <c r="D396" s="163"/>
+      <c r="E396" s="163"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="52">
@@ -8336,9 +8372,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="164"/>
-      <c r="D413" s="165"/>
-      <c r="E413" s="165"/>
+      <c r="C413" s="162"/>
+      <c r="D413" s="163"/>
+      <c r="E413" s="163"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A414" s="52">
@@ -8489,9 +8525,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="164"/>
-      <c r="D430" s="165"/>
-      <c r="E430" s="165"/>
+      <c r="C430" s="162"/>
+      <c r="D430" s="163"/>
+      <c r="E430" s="163"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A431" s="52">
@@ -8642,9 +8678,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="164"/>
-      <c r="D447" s="165"/>
-      <c r="E447" s="165"/>
+      <c r="C447" s="162"/>
+      <c r="D447" s="163"/>
+      <c r="E447" s="163"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A448" s="52">
@@ -8795,9 +8831,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="164"/>
-      <c r="D464" s="165"/>
-      <c r="E464" s="165"/>
+      <c r="C464" s="162"/>
+      <c r="D464" s="163"/>
+      <c r="E464" s="163"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="52">
@@ -8948,9 +8984,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="164"/>
-      <c r="D481" s="165"/>
-      <c r="E481" s="165"/>
+      <c r="C481" s="162"/>
+      <c r="D481" s="163"/>
+      <c r="E481" s="163"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="52">
@@ -9101,9 +9137,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="164"/>
-      <c r="D498" s="165"/>
-      <c r="E498" s="165"/>
+      <c r="C498" s="162"/>
+      <c r="D498" s="163"/>
+      <c r="E498" s="163"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A499" s="52">
@@ -9254,9 +9290,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="164"/>
-      <c r="D515" s="165"/>
-      <c r="E515" s="165"/>
+      <c r="C515" s="162"/>
+      <c r="D515" s="163"/>
+      <c r="E515" s="163"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A516" s="52">
@@ -9407,9 +9443,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="164"/>
-      <c r="D532" s="165"/>
-      <c r="E532" s="165"/>
+      <c r="C532" s="162"/>
+      <c r="D532" s="163"/>
+      <c r="E532" s="163"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A533" s="55">
@@ -9560,18 +9596,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="170"/>
-      <c r="D549" s="171"/>
-      <c r="E549" s="171"/>
+      <c r="C549" s="176"/>
+      <c r="D549" s="177"/>
+      <c r="E549" s="177"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="164"/>
-      <c r="D550" s="165"/>
-      <c r="E550" s="165"/>
+      <c r="C550" s="162"/>
+      <c r="D550" s="163"/>
+      <c r="E550" s="163"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A551" s="59">
@@ -9722,9 +9758,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="166"/>
-      <c r="D567" s="167"/>
-      <c r="E567" s="167"/>
+      <c r="C567" s="164"/>
+      <c r="D567" s="165"/>
+      <c r="E567" s="165"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A568" s="59">
@@ -9875,9 +9911,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="164"/>
-      <c r="D584" s="165"/>
-      <c r="E584" s="165"/>
+      <c r="C584" s="162"/>
+      <c r="D584" s="163"/>
+      <c r="E584" s="163"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A585" s="59">
@@ -10028,9 +10064,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="164"/>
-      <c r="D601" s="165"/>
-      <c r="E601" s="165"/>
+      <c r="C601" s="162"/>
+      <c r="D601" s="163"/>
+      <c r="E601" s="163"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A602" s="59">
@@ -10181,9 +10217,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="164"/>
-      <c r="D618" s="165"/>
-      <c r="E618" s="165"/>
+      <c r="C618" s="162"/>
+      <c r="D618" s="163"/>
+      <c r="E618" s="163"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A619" s="59">
@@ -10334,9 +10370,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="164"/>
-      <c r="D635" s="165"/>
-      <c r="E635" s="165"/>
+      <c r="C635" s="162"/>
+      <c r="D635" s="163"/>
+      <c r="E635" s="163"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A636" s="59">
@@ -10487,9 +10523,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="164"/>
-      <c r="D652" s="165"/>
-      <c r="E652" s="165"/>
+      <c r="C652" s="162"/>
+      <c r="D652" s="163"/>
+      <c r="E652" s="163"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A653" s="59">
@@ -10640,9 +10676,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="164"/>
-      <c r="D669" s="165"/>
-      <c r="E669" s="165"/>
+      <c r="C669" s="162"/>
+      <c r="D669" s="163"/>
+      <c r="E669" s="163"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A670" s="59">
@@ -10793,9 +10829,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="164"/>
-      <c r="D686" s="165"/>
-      <c r="E686" s="165"/>
+      <c r="C686" s="162"/>
+      <c r="D686" s="163"/>
+      <c r="E686" s="163"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A687" s="59">
@@ -10946,9 +10982,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="164"/>
-      <c r="D703" s="165"/>
-      <c r="E703" s="165"/>
+      <c r="C703" s="162"/>
+      <c r="D703" s="163"/>
+      <c r="E703" s="163"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A704" s="59">
@@ -11099,9 +11135,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="164"/>
-      <c r="D720" s="165"/>
-      <c r="E720" s="165"/>
+      <c r="C720" s="162"/>
+      <c r="D720" s="163"/>
+      <c r="E720" s="163"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A721" s="59">
@@ -11252,9 +11288,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="164"/>
-      <c r="D737" s="165"/>
-      <c r="E737" s="165"/>
+      <c r="C737" s="162"/>
+      <c r="D737" s="163"/>
+      <c r="E737" s="163"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A738" s="59">
@@ -11405,9 +11441,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="164"/>
-      <c r="D754" s="165"/>
-      <c r="E754" s="165"/>
+      <c r="C754" s="162"/>
+      <c r="D754" s="163"/>
+      <c r="E754" s="163"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A755" s="59">
@@ -11558,9 +11594,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="164"/>
-      <c r="D771" s="165"/>
-      <c r="E771" s="165"/>
+      <c r="C771" s="162"/>
+      <c r="D771" s="163"/>
+      <c r="E771" s="163"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A772" s="59">
@@ -11711,9 +11747,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="164"/>
-      <c r="D788" s="165"/>
-      <c r="E788" s="165"/>
+      <c r="C788" s="162"/>
+      <c r="D788" s="163"/>
+      <c r="E788" s="163"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A789" s="59">
@@ -11864,9 +11900,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="164"/>
-      <c r="D805" s="165"/>
-      <c r="E805" s="165"/>
+      <c r="C805" s="162"/>
+      <c r="D805" s="163"/>
+      <c r="E805" s="163"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A806" s="59">
@@ -12017,18 +12053,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="172"/>
-      <c r="D822" s="173"/>
-      <c r="E822" s="173"/>
+      <c r="C822" s="174"/>
+      <c r="D822" s="175"/>
+      <c r="E822" s="175"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="164"/>
-      <c r="D823" s="165"/>
-      <c r="E823" s="165"/>
+      <c r="C823" s="162"/>
+      <c r="D823" s="163"/>
+      <c r="E823" s="163"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A824" s="64">
@@ -12179,9 +12215,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="166"/>
-      <c r="D840" s="167"/>
-      <c r="E840" s="167"/>
+      <c r="C840" s="164"/>
+      <c r="D840" s="165"/>
+      <c r="E840" s="165"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A841" s="64">
@@ -12332,9 +12368,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="164"/>
-      <c r="D857" s="165"/>
-      <c r="E857" s="165"/>
+      <c r="C857" s="162"/>
+      <c r="D857" s="163"/>
+      <c r="E857" s="163"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A858" s="64">
@@ -12485,9 +12521,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="164"/>
-      <c r="D874" s="165"/>
-      <c r="E874" s="165"/>
+      <c r="C874" s="162"/>
+      <c r="D874" s="163"/>
+      <c r="E874" s="163"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A875" s="64">
@@ -12638,9 +12674,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="164"/>
-      <c r="D891" s="165"/>
-      <c r="E891" s="165"/>
+      <c r="C891" s="162"/>
+      <c r="D891" s="163"/>
+      <c r="E891" s="163"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A892" s="64">
@@ -12791,9 +12827,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="164"/>
-      <c r="D908" s="165"/>
-      <c r="E908" s="165"/>
+      <c r="C908" s="162"/>
+      <c r="D908" s="163"/>
+      <c r="E908" s="163"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A909" s="64">
@@ -12944,9 +12980,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="164"/>
-      <c r="D925" s="165"/>
-      <c r="E925" s="165"/>
+      <c r="C925" s="162"/>
+      <c r="D925" s="163"/>
+      <c r="E925" s="163"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A926" s="64">
@@ -13097,9 +13133,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="164"/>
-      <c r="D942" s="165"/>
-      <c r="E942" s="165"/>
+      <c r="C942" s="162"/>
+      <c r="D942" s="163"/>
+      <c r="E942" s="163"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A943" s="64">
@@ -13250,9 +13286,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="164"/>
-      <c r="D959" s="165"/>
-      <c r="E959" s="165"/>
+      <c r="C959" s="162"/>
+      <c r="D959" s="163"/>
+      <c r="E959" s="163"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A960" s="64">
@@ -13403,9 +13439,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="164"/>
-      <c r="D976" s="165"/>
-      <c r="E976" s="165"/>
+      <c r="C976" s="162"/>
+      <c r="D976" s="163"/>
+      <c r="E976" s="163"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A977" s="64">
@@ -13556,9 +13592,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="164"/>
-      <c r="D993" s="165"/>
-      <c r="E993" s="165"/>
+      <c r="C993" s="162"/>
+      <c r="D993" s="163"/>
+      <c r="E993" s="163"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A994" s="64">
@@ -13709,9 +13745,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="164"/>
-      <c r="D1010" s="165"/>
-      <c r="E1010" s="165"/>
+      <c r="C1010" s="162"/>
+      <c r="D1010" s="163"/>
+      <c r="E1010" s="163"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1011" s="64">
@@ -13862,9 +13898,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="164"/>
-      <c r="D1027" s="165"/>
-      <c r="E1027" s="165"/>
+      <c r="C1027" s="162"/>
+      <c r="D1027" s="163"/>
+      <c r="E1027" s="163"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1028" s="64">
@@ -14015,9 +14051,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="164"/>
-      <c r="D1044" s="165"/>
-      <c r="E1044" s="165"/>
+      <c r="C1044" s="162"/>
+      <c r="D1044" s="163"/>
+      <c r="E1044" s="163"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1045" s="64">
@@ -14168,9 +14204,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="164"/>
-      <c r="D1061" s="165"/>
-      <c r="E1061" s="165"/>
+      <c r="C1061" s="162"/>
+      <c r="D1061" s="163"/>
+      <c r="E1061" s="163"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1062" s="64">
@@ -14321,9 +14357,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="164"/>
-      <c r="D1078" s="165"/>
-      <c r="E1078" s="165"/>
+      <c r="C1078" s="162"/>
+      <c r="D1078" s="163"/>
+      <c r="E1078" s="163"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1079" s="64">
@@ -14474,18 +14510,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="174"/>
-      <c r="D1095" s="175"/>
-      <c r="E1095" s="175"/>
+      <c r="C1095" s="172"/>
+      <c r="D1095" s="173"/>
+      <c r="E1095" s="173"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="164"/>
-      <c r="D1096" s="165"/>
-      <c r="E1096" s="165"/>
+      <c r="C1096" s="162"/>
+      <c r="D1096" s="163"/>
+      <c r="E1096" s="163"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1097" s="69">
@@ -14636,9 +14672,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="166"/>
-      <c r="D1113" s="167"/>
-      <c r="E1113" s="167"/>
+      <c r="C1113" s="164"/>
+      <c r="D1113" s="165"/>
+      <c r="E1113" s="165"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1114" s="69">
@@ -14789,9 +14825,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="164"/>
-      <c r="D1130" s="165"/>
-      <c r="E1130" s="165"/>
+      <c r="C1130" s="162"/>
+      <c r="D1130" s="163"/>
+      <c r="E1130" s="163"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1131" s="69">
@@ -14942,9 +14978,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="164"/>
-      <c r="D1147" s="165"/>
-      <c r="E1147" s="165"/>
+      <c r="C1147" s="162"/>
+      <c r="D1147" s="163"/>
+      <c r="E1147" s="163"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1148" s="69">
@@ -15095,9 +15131,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="164"/>
-      <c r="D1164" s="165"/>
-      <c r="E1164" s="165"/>
+      <c r="C1164" s="162"/>
+      <c r="D1164" s="163"/>
+      <c r="E1164" s="163"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1165" s="69">
@@ -15248,9 +15284,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="164"/>
-      <c r="D1181" s="165"/>
-      <c r="E1181" s="165"/>
+      <c r="C1181" s="162"/>
+      <c r="D1181" s="163"/>
+      <c r="E1181" s="163"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3" x14ac:dyDescent="0.2">
       <c r="A1182" s="69">
@@ -15401,9 +15437,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="164"/>
-      <c r="D1198" s="165"/>
-      <c r="E1198" s="165"/>
+      <c r="C1198" s="162"/>
+      <c r="D1198" s="163"/>
+      <c r="E1198" s="163"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1199" s="69">
@@ -15554,9 +15590,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="164"/>
-      <c r="D1215" s="165"/>
-      <c r="E1215" s="165"/>
+      <c r="C1215" s="162"/>
+      <c r="D1215" s="163"/>
+      <c r="E1215" s="163"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1216" s="69">
@@ -15707,9 +15743,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="164"/>
-      <c r="D1232" s="165"/>
-      <c r="E1232" s="165"/>
+      <c r="C1232" s="162"/>
+      <c r="D1232" s="163"/>
+      <c r="E1232" s="163"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1233" s="69">
@@ -15860,9 +15896,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="164"/>
-      <c r="D1249" s="165"/>
-      <c r="E1249" s="165"/>
+      <c r="C1249" s="162"/>
+      <c r="D1249" s="163"/>
+      <c r="E1249" s="163"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1250" s="69">
@@ -16013,9 +16049,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="164"/>
-      <c r="D1266" s="165"/>
-      <c r="E1266" s="165"/>
+      <c r="C1266" s="162"/>
+      <c r="D1266" s="163"/>
+      <c r="E1266" s="163"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1267" s="69">
@@ -16166,9 +16202,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="164"/>
-      <c r="D1283" s="165"/>
-      <c r="E1283" s="165"/>
+      <c r="C1283" s="162"/>
+      <c r="D1283" s="163"/>
+      <c r="E1283" s="163"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1284" s="69">
@@ -16319,9 +16355,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="164"/>
-      <c r="D1300" s="165"/>
-      <c r="E1300" s="165"/>
+      <c r="C1300" s="162"/>
+      <c r="D1300" s="163"/>
+      <c r="E1300" s="163"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1301" s="69">
@@ -16472,9 +16508,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="164"/>
-      <c r="D1317" s="165"/>
-      <c r="E1317" s="165"/>
+      <c r="C1317" s="162"/>
+      <c r="D1317" s="163"/>
+      <c r="E1317" s="163"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1318" s="69">
@@ -16625,9 +16661,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="164"/>
-      <c r="D1334" s="165"/>
-      <c r="E1334" s="165"/>
+      <c r="C1334" s="162"/>
+      <c r="D1334" s="163"/>
+      <c r="E1334" s="163"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1335" s="69">
@@ -16778,9 +16814,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="164"/>
-      <c r="D1351" s="165"/>
-      <c r="E1351" s="165"/>
+      <c r="C1351" s="162"/>
+      <c r="D1351" s="163"/>
+      <c r="E1351" s="163"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1352" s="69">
@@ -16931,18 +16967,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="176"/>
-      <c r="D1368" s="177"/>
-      <c r="E1368" s="177"/>
+      <c r="C1368" s="170"/>
+      <c r="D1368" s="171"/>
+      <c r="E1368" s="171"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="164"/>
-      <c r="D1369" s="165"/>
-      <c r="E1369" s="165"/>
+      <c r="C1369" s="162"/>
+      <c r="D1369" s="163"/>
+      <c r="E1369" s="163"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1370" s="74">
@@ -17093,9 +17129,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
-      <c r="D1386" s="167"/>
-      <c r="E1386" s="167"/>
+      <c r="C1386" s="164"/>
+      <c r="D1386" s="165"/>
+      <c r="E1386" s="165"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1387" s="74">
@@ -17246,9 +17282,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="164"/>
-      <c r="D1403" s="165"/>
-      <c r="E1403" s="165"/>
+      <c r="C1403" s="162"/>
+      <c r="D1403" s="163"/>
+      <c r="E1403" s="163"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1404" s="74">
@@ -17399,9 +17435,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="164"/>
-      <c r="D1420" s="165"/>
-      <c r="E1420" s="165"/>
+      <c r="C1420" s="162"/>
+      <c r="D1420" s="163"/>
+      <c r="E1420" s="163"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1421" s="74">
@@ -17552,9 +17588,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="164"/>
-      <c r="D1437" s="165"/>
-      <c r="E1437" s="165"/>
+      <c r="C1437" s="162"/>
+      <c r="D1437" s="163"/>
+      <c r="E1437" s="163"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1438" s="74">
@@ -17705,9 +17741,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="164"/>
-      <c r="D1454" s="165"/>
-      <c r="E1454" s="165"/>
+      <c r="C1454" s="162"/>
+      <c r="D1454" s="163"/>
+      <c r="E1454" s="163"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1455" s="74">
@@ -17858,9 +17894,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="164"/>
-      <c r="D1471" s="165"/>
-      <c r="E1471" s="165"/>
+      <c r="C1471" s="162"/>
+      <c r="D1471" s="163"/>
+      <c r="E1471" s="163"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1472" s="74">
@@ -18011,9 +18047,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="164"/>
-      <c r="D1488" s="165"/>
-      <c r="E1488" s="165"/>
+      <c r="C1488" s="162"/>
+      <c r="D1488" s="163"/>
+      <c r="E1488" s="163"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1489" s="74">
@@ -18164,9 +18200,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="164"/>
-      <c r="D1505" s="165"/>
-      <c r="E1505" s="165"/>
+      <c r="C1505" s="162"/>
+      <c r="D1505" s="163"/>
+      <c r="E1505" s="163"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1506" s="74">
@@ -18317,9 +18353,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="164"/>
-      <c r="D1522" s="165"/>
-      <c r="E1522" s="165"/>
+      <c r="C1522" s="162"/>
+      <c r="D1522" s="163"/>
+      <c r="E1522" s="163"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1523" s="74">
@@ -18470,9 +18506,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="164"/>
-      <c r="D1539" s="165"/>
-      <c r="E1539" s="165"/>
+      <c r="C1539" s="162"/>
+      <c r="D1539" s="163"/>
+      <c r="E1539" s="163"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1540" s="74">
@@ -18623,9 +18659,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="164"/>
-      <c r="D1556" s="165"/>
-      <c r="E1556" s="165"/>
+      <c r="C1556" s="162"/>
+      <c r="D1556" s="163"/>
+      <c r="E1556" s="163"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1557" s="74">
@@ -18776,9 +18812,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="164"/>
-      <c r="D1573" s="165"/>
-      <c r="E1573" s="165"/>
+      <c r="C1573" s="162"/>
+      <c r="D1573" s="163"/>
+      <c r="E1573" s="163"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1574" s="74">
@@ -18929,9 +18965,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="164"/>
-      <c r="D1590" s="165"/>
-      <c r="E1590" s="165"/>
+      <c r="C1590" s="162"/>
+      <c r="D1590" s="163"/>
+      <c r="E1590" s="163"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1591" s="74">
@@ -19082,9 +19118,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="164"/>
-      <c r="D1607" s="165"/>
-      <c r="E1607" s="165"/>
+      <c r="C1607" s="162"/>
+      <c r="D1607" s="163"/>
+      <c r="E1607" s="163"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1608" s="74">
@@ -19235,9 +19271,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="164"/>
-      <c r="D1624" s="165"/>
-      <c r="E1624" s="165"/>
+      <c r="C1624" s="162"/>
+      <c r="D1624" s="163"/>
+      <c r="E1624" s="163"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1625" s="74">
@@ -19388,18 +19424,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="178"/>
-      <c r="D1641" s="179"/>
-      <c r="E1641" s="179"/>
+      <c r="C1641" s="168"/>
+      <c r="D1641" s="169"/>
+      <c r="E1641" s="169"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="164"/>
-      <c r="D1642" s="165"/>
-      <c r="E1642" s="165"/>
+      <c r="C1642" s="162"/>
+      <c r="D1642" s="163"/>
+      <c r="E1642" s="163"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1643" s="79">
@@ -19550,9 +19586,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="166"/>
-      <c r="D1659" s="167"/>
-      <c r="E1659" s="167"/>
+      <c r="C1659" s="164"/>
+      <c r="D1659" s="165"/>
+      <c r="E1659" s="165"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1660" s="79">
@@ -19703,9 +19739,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="164"/>
-      <c r="D1676" s="165"/>
-      <c r="E1676" s="165"/>
+      <c r="C1676" s="162"/>
+      <c r="D1676" s="163"/>
+      <c r="E1676" s="163"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1677" s="79">
@@ -19856,9 +19892,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="164"/>
-      <c r="D1693" s="165"/>
-      <c r="E1693" s="165"/>
+      <c r="C1693" s="162"/>
+      <c r="D1693" s="163"/>
+      <c r="E1693" s="163"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1694" s="79">
@@ -20009,9 +20045,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="164"/>
-      <c r="D1710" s="165"/>
-      <c r="E1710" s="165"/>
+      <c r="C1710" s="162"/>
+      <c r="D1710" s="163"/>
+      <c r="E1710" s="163"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1711" s="79">
@@ -20162,9 +20198,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="164"/>
-      <c r="D1727" s="165"/>
-      <c r="E1727" s="165"/>
+      <c r="C1727" s="162"/>
+      <c r="D1727" s="163"/>
+      <c r="E1727" s="163"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1728" s="79">
@@ -20315,9 +20351,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="164"/>
-      <c r="D1744" s="165"/>
-      <c r="E1744" s="165"/>
+      <c r="C1744" s="162"/>
+      <c r="D1744" s="163"/>
+      <c r="E1744" s="163"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1745" s="79">
@@ -20468,9 +20504,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="164"/>
-      <c r="D1761" s="165"/>
-      <c r="E1761" s="165"/>
+      <c r="C1761" s="162"/>
+      <c r="D1761" s="163"/>
+      <c r="E1761" s="163"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1762" s="79">
@@ -20621,9 +20657,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="164"/>
-      <c r="D1778" s="165"/>
-      <c r="E1778" s="165"/>
+      <c r="C1778" s="162"/>
+      <c r="D1778" s="163"/>
+      <c r="E1778" s="163"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1779" s="79">
@@ -20774,9 +20810,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="164"/>
-      <c r="D1795" s="165"/>
-      <c r="E1795" s="165"/>
+      <c r="C1795" s="162"/>
+      <c r="D1795" s="163"/>
+      <c r="E1795" s="163"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1796" s="79">
@@ -20927,9 +20963,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="164"/>
-      <c r="D1812" s="165"/>
-      <c r="E1812" s="165"/>
+      <c r="C1812" s="162"/>
+      <c r="D1812" s="163"/>
+      <c r="E1812" s="163"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1813" s="79">
@@ -21080,9 +21116,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="164"/>
-      <c r="D1829" s="165"/>
-      <c r="E1829" s="165"/>
+      <c r="C1829" s="162"/>
+      <c r="D1829" s="163"/>
+      <c r="E1829" s="163"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1830" s="79">
@@ -21233,9 +21269,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="164"/>
-      <c r="D1846" s="165"/>
-      <c r="E1846" s="165"/>
+      <c r="C1846" s="162"/>
+      <c r="D1846" s="163"/>
+      <c r="E1846" s="163"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1847" s="79">
@@ -21386,9 +21422,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="164"/>
-      <c r="D1863" s="165"/>
-      <c r="E1863" s="165"/>
+      <c r="C1863" s="162"/>
+      <c r="D1863" s="163"/>
+      <c r="E1863" s="163"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1864" s="79">
@@ -21539,9 +21575,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="164"/>
-      <c r="D1880" s="165"/>
-      <c r="E1880" s="165"/>
+      <c r="C1880" s="162"/>
+      <c r="D1880" s="163"/>
+      <c r="E1880" s="163"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1881" s="79">
@@ -21692,9 +21728,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="164"/>
-      <c r="D1897" s="165"/>
-      <c r="E1897" s="165"/>
+      <c r="C1897" s="162"/>
+      <c r="D1897" s="163"/>
+      <c r="E1897" s="163"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1898" s="79">
@@ -21845,18 +21881,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="180"/>
-      <c r="D1914" s="181"/>
-      <c r="E1914" s="181"/>
+      <c r="C1914" s="166"/>
+      <c r="D1914" s="167"/>
+      <c r="E1914" s="167"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="164"/>
-      <c r="D1915" s="165"/>
-      <c r="E1915" s="165"/>
+      <c r="C1915" s="162"/>
+      <c r="D1915" s="163"/>
+      <c r="E1915" s="163"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1916" s="84">
@@ -22007,9 +22043,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="166"/>
-      <c r="D1932" s="167"/>
-      <c r="E1932" s="167"/>
+      <c r="C1932" s="164"/>
+      <c r="D1932" s="165"/>
+      <c r="E1932" s="165"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1933" s="84">
@@ -22160,9 +22196,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="164"/>
-      <c r="D1949" s="165"/>
-      <c r="E1949" s="165"/>
+      <c r="C1949" s="162"/>
+      <c r="D1949" s="163"/>
+      <c r="E1949" s="163"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1950" s="84">
@@ -22313,9 +22349,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="164"/>
-      <c r="D1966" s="165"/>
-      <c r="E1966" s="165"/>
+      <c r="C1966" s="162"/>
+      <c r="D1966" s="163"/>
+      <c r="E1966" s="163"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1967" s="84">
@@ -22466,9 +22502,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="164"/>
-      <c r="D1983" s="165"/>
-      <c r="E1983" s="165"/>
+      <c r="C1983" s="162"/>
+      <c r="D1983" s="163"/>
+      <c r="E1983" s="163"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A1984" s="84">
@@ -22619,9 +22655,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="164"/>
-      <c r="D2000" s="165"/>
-      <c r="E2000" s="165"/>
+      <c r="C2000" s="162"/>
+      <c r="D2000" s="163"/>
+      <c r="E2000" s="163"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2001" s="84">
@@ -22772,9 +22808,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="164"/>
-      <c r="D2017" s="165"/>
-      <c r="E2017" s="165"/>
+      <c r="C2017" s="162"/>
+      <c r="D2017" s="163"/>
+      <c r="E2017" s="163"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2018" s="84">
@@ -22925,9 +22961,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="164"/>
-      <c r="D2034" s="165"/>
-      <c r="E2034" s="165"/>
+      <c r="C2034" s="162"/>
+      <c r="D2034" s="163"/>
+      <c r="E2034" s="163"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2035" s="84">
@@ -23078,9 +23114,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="164"/>
-      <c r="D2051" s="165"/>
-      <c r="E2051" s="165"/>
+      <c r="C2051" s="162"/>
+      <c r="D2051" s="163"/>
+      <c r="E2051" s="163"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2052" s="84">
@@ -23231,9 +23267,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="164"/>
-      <c r="D2068" s="165"/>
-      <c r="E2068" s="165"/>
+      <c r="C2068" s="162"/>
+      <c r="D2068" s="163"/>
+      <c r="E2068" s="163"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2069" s="84">
@@ -23384,9 +23420,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="164"/>
-      <c r="D2085" s="165"/>
-      <c r="E2085" s="165"/>
+      <c r="C2085" s="162"/>
+      <c r="D2085" s="163"/>
+      <c r="E2085" s="163"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2086" s="84">
@@ -23537,9 +23573,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="164"/>
-      <c r="D2102" s="165"/>
-      <c r="E2102" s="165"/>
+      <c r="C2102" s="162"/>
+      <c r="D2102" s="163"/>
+      <c r="E2102" s="163"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2103" s="84">
@@ -23690,9 +23726,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="164"/>
-      <c r="D2119" s="165"/>
-      <c r="E2119" s="165"/>
+      <c r="C2119" s="162"/>
+      <c r="D2119" s="163"/>
+      <c r="E2119" s="163"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2120" s="84">
@@ -23843,9 +23879,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="164"/>
-      <c r="D2136" s="165"/>
-      <c r="E2136" s="165"/>
+      <c r="C2136" s="162"/>
+      <c r="D2136" s="163"/>
+      <c r="E2136" s="163"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2137" s="84">
@@ -23996,9 +24032,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="164"/>
-      <c r="D2153" s="165"/>
-      <c r="E2153" s="165"/>
+      <c r="C2153" s="162"/>
+      <c r="D2153" s="163"/>
+      <c r="E2153" s="163"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2154" s="84">
@@ -24149,9 +24185,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="164"/>
-      <c r="D2170" s="165"/>
-      <c r="E2170" s="165"/>
+      <c r="C2170" s="162"/>
+      <c r="D2170" s="163"/>
+      <c r="E2170" s="163"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2171" s="84">
@@ -24299,15 +24335,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24320,124 +24463,17 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24462,51 +24498,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="189" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
-      <c r="J1" s="188"/>
-      <c r="K1" s="188"/>
-      <c r="L1" s="188"/>
+      <c r="B1" s="189"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
+      <c r="E1" s="189"/>
+      <c r="F1" s="189"/>
+      <c r="G1" s="189"/>
+      <c r="H1" s="189"/>
+      <c r="I1" s="189"/>
+      <c r="J1" s="189"/>
+      <c r="K1" s="189"/>
+      <c r="L1" s="189"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="186" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="186"/>
-      <c r="I2" s="186"/>
-      <c r="J2" s="186"/>
-      <c r="K2" s="186"/>
-      <c r="L2" s="187"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="188"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="182" t="s">
+      <c r="A3" s="183" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
-      <c r="G3" s="183"/>
-      <c r="H3" s="183"/>
-      <c r="I3" s="183"/>
-      <c r="J3" s="183"/>
-      <c r="K3" s="184"/>
+      <c r="B3" s="184"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="185"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
@@ -24723,19 +24759,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="182" t="s">
+      <c r="A20" s="183" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="183"/>
-      <c r="C20" s="183"/>
-      <c r="D20" s="183"/>
-      <c r="E20" s="183"/>
-      <c r="F20" s="183"/>
-      <c r="G20" s="183"/>
-      <c r="H20" s="183"/>
-      <c r="I20" s="183"/>
-      <c r="J20" s="183"/>
-      <c r="K20" s="184"/>
+      <c r="B20" s="184"/>
+      <c r="C20" s="184"/>
+      <c r="D20" s="184"/>
+      <c r="E20" s="184"/>
+      <c r="F20" s="184"/>
+      <c r="G20" s="184"/>
+      <c r="H20" s="184"/>
+      <c r="I20" s="184"/>
+      <c r="J20" s="184"/>
+      <c r="K20" s="185"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
@@ -24952,19 +24988,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="182" t="s">
+      <c r="A37" s="183" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="183"/>
-      <c r="C37" s="183"/>
-      <c r="D37" s="183"/>
-      <c r="E37" s="183"/>
-      <c r="F37" s="183"/>
-      <c r="G37" s="183"/>
-      <c r="H37" s="183"/>
-      <c r="I37" s="183"/>
-      <c r="J37" s="183"/>
-      <c r="K37" s="184"/>
+      <c r="B37" s="184"/>
+      <c r="C37" s="184"/>
+      <c r="D37" s="184"/>
+      <c r="E37" s="184"/>
+      <c r="F37" s="184"/>
+      <c r="G37" s="184"/>
+      <c r="H37" s="184"/>
+      <c r="I37" s="184"/>
+      <c r="J37" s="184"/>
+      <c r="K37" s="185"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
@@ -25188,7 +25224,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25222,28 +25258,28 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="189"/>
+      <c r="A3" s="190"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="190"/>
+      <c r="A4" s="191"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="190"/>
+      <c r="A5" s="191"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="190"/>
+      <c r="A6" s="191"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="190"/>
+      <c r="A7" s="191"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="190"/>
+      <c r="A8" s="191"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="190"/>
+      <c r="A9" s="191"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="191"/>
+      <c r="A10" s="192"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -25399,7 +25435,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25426,10 +25462,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="192" t="s">
+      <c r="B1" s="193" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="193"/>
+      <c r="C1" s="194"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25440,7 +25476,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="195" t="s">
         <v>213</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25454,7 +25490,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="195"/>
+      <c r="A4" s="196"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25466,7 +25502,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="195"/>
+      <c r="A5" s="196"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25475,7 +25511,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="195"/>
+      <c r="A6" s="196"/>
       <c r="B6" s="139" t="s">
         <v>215</v>
       </c>
@@ -25487,7 +25523,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="195"/>
+      <c r="A7" s="196"/>
       <c r="B7" s="128" t="s">
         <v>178</v>
       </c>
@@ -25499,7 +25535,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="195"/>
+      <c r="A8" s="196"/>
       <c r="B8" s="128" t="s">
         <v>179</v>
       </c>
@@ -25508,7 +25544,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="196"/>
+      <c r="A9" s="197"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25523,7 +25559,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="194" t="s">
+      <c r="A11" s="195" t="s">
         <v>214</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25537,7 +25573,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="195"/>
+      <c r="A12" s="196"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25549,7 +25585,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="195"/>
+      <c r="A13" s="196"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25558,7 +25594,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="195"/>
+      <c r="A14" s="196"/>
       <c r="B14" s="139" t="s">
         <v>215</v>
       </c>
@@ -25570,7 +25606,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="195"/>
+      <c r="A15" s="196"/>
       <c r="B15" s="128" t="s">
         <v>178</v>
       </c>
@@ -25582,7 +25618,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="195"/>
+      <c r="A16" s="196"/>
       <c r="B16" s="128" t="s">
         <v>179</v>
       </c>
@@ -25591,7 +25627,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="196"/>
+      <c r="A17" s="197"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25606,7 +25642,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="194" t="s">
+      <c r="A19" s="195" t="s">
         <v>214</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25615,7 +25651,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="195"/>
+      <c r="A20" s="196"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25625,14 +25661,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="195"/>
+      <c r="A21" s="196"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="195"/>
+      <c r="A22" s="196"/>
       <c r="B22" s="139" t="s">
         <v>215</v>
       </c>
@@ -25642,7 +25678,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="195"/>
+      <c r="A23" s="196"/>
       <c r="B23" s="128" t="s">
         <v>178</v>
       </c>
@@ -25652,14 +25688,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="195"/>
+      <c r="A24" s="196"/>
       <c r="B24" s="128" t="s">
         <v>179</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="196"/>
+      <c r="A25" s="197"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25672,7 +25708,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25703,17 +25739,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="204" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="214"/>
+      <c r="B2" s="205"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="215" t="s">
+      <c r="A3" s="206" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="214"/>
+      <c r="B3" s="205"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -25729,115 +25765,128 @@
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="201" t="s">
+      <c r="A7" s="215" t="s">
         <v>197</v>
       </c>
-      <c r="B7" s="202"/>
+      <c r="B7" s="216"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="203" t="s">
+      <c r="A9" s="213" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="204"/>
+      <c r="B9" s="214"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="205"/>
-      <c r="B10" s="206"/>
+      <c r="A10" s="200"/>
+      <c r="B10" s="201"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="202" t="s">
         <v>199</v>
       </c>
-      <c r="B11" s="198"/>
+      <c r="B11" s="203"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="197" t="s">
+      <c r="A12" s="202" t="s">
         <v>200</v>
       </c>
-      <c r="B12" s="198"/>
+      <c r="B12" s="203"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="197" t="s">
+      <c r="A13" s="202" t="s">
         <v>201</v>
       </c>
-      <c r="B13" s="198"/>
+      <c r="B13" s="203"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="197" t="s">
+      <c r="A14" s="202" t="s">
         <v>202</v>
       </c>
-      <c r="B14" s="198"/>
+      <c r="B14" s="203"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="197" t="s">
+      <c r="A15" s="202" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="198"/>
+      <c r="B15" s="203"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="197" t="s">
+      <c r="A16" s="202" t="s">
         <v>204</v>
       </c>
-      <c r="B16" s="198"/>
+      <c r="B16" s="203"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="199" t="s">
+      <c r="A17" s="198" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="200"/>
+      <c r="B17" s="199"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="201" t="s">
+      <c r="A19" s="215" t="s">
         <v>208</v>
       </c>
-      <c r="B19" s="202"/>
+      <c r="B19" s="216"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="203" t="s">
+      <c r="A21" s="213" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="204"/>
+      <c r="B21" s="214"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="205"/>
-      <c r="B22" s="206"/>
+      <c r="A22" s="200"/>
+      <c r="B22" s="201"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="197" t="s">
+      <c r="A23" s="202" t="s">
         <v>210</v>
       </c>
-      <c r="B23" s="198"/>
+      <c r="B23" s="203"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="197"/>
-      <c r="B24" s="198"/>
+      <c r="A24" s="202"/>
+      <c r="B24" s="203"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="197" t="s">
+      <c r="A25" s="202" t="s">
         <v>211</v>
       </c>
-      <c r="B25" s="198"/>
+      <c r="B25" s="203"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="197" t="s">
+      <c r="A26" s="202" t="s">
         <v>212</v>
       </c>
-      <c r="B26" s="198"/>
+      <c r="B26" s="203"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="199"/>
-      <c r="B27" s="200"/>
+      <c r="A27" s="198"/>
+      <c r="B27" s="199"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25848,19 +25897,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Flintstones - level 5 done, 1211 ahead
</commit_message>
<xml_diff>
--- a/Flintstones/Compare/Flintstones.xlsx
+++ b/Flintstones/Compare/Flintstones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="242">
   <si>
     <t>Notes</t>
   </si>
@@ -782,6 +782,9 @@
   </si>
   <si>
     <t>X = 151</t>
+  </si>
+  <si>
+    <t>Timer ticks to 59</t>
   </si>
 </sst>
 </file>
@@ -2483,8 +2486,8 @@
   <dimension ref="A1:K172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D109" sqref="D109"/>
+      <pane ySplit="6" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -4135,23 +4138,35 @@
     </row>
     <row r="109" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="155"/>
-      <c r="B109" s="100"/>
-      <c r="C109" s="101"/>
-      <c r="D109" s="101"/>
+      <c r="B109" s="218" t="s">
+        <v>241</v>
+      </c>
+      <c r="C109" s="101">
+        <v>24667</v>
+      </c>
+      <c r="D109" s="101">
+        <v>25856</v>
+      </c>
       <c r="E109" s="123">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1189</v>
       </c>
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="155"/>
-      <c r="B110" s="100"/>
-      <c r="C110" s="101"/>
-      <c r="D110" s="101"/>
+      <c r="B110" s="218" t="s">
+        <v>169</v>
+      </c>
+      <c r="C110" s="101">
+        <v>28611</v>
+      </c>
+      <c r="D110" s="101">
+        <v>29821</v>
+      </c>
       <c r="E110" s="123">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1210</v>
       </c>
       <c r="F110" s="105"/>
     </row>
@@ -4260,7 +4275,9 @@
         <v>188</v>
       </c>
       <c r="C120" s="99"/>
-      <c r="D120" s="99"/>
+      <c r="D120" s="99">
+        <v>30015</v>
+      </c>
       <c r="E120" s="125">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4280,7 +4297,7 @@
       </c>
       <c r="D121" s="103">
         <f>D120-D107</f>
-        <v>-25749</v>
+        <v>4266</v>
       </c>
       <c r="E121" s="126">
         <f>E120-E107</f>
@@ -4292,7 +4309,8 @@
         <v>-1189</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:7" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A123" s="154" t="s">
         <v>174</v>
       </c>
@@ -4312,42 +4330,56 @@
         <v>184</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="155"/>
       <c r="B124" s="98" t="s">
         <v>185</v>
       </c>
       <c r="C124" s="99"/>
-      <c r="D124" s="99"/>
+      <c r="D124" s="99">
+        <v>30015</v>
+      </c>
       <c r="E124" s="123">
         <f t="shared" ref="E124:E137" si="6">IF(AND(C124&gt;0,D124&gt;0), D124-C124, 0)</f>
         <v>0</v>
       </c>
       <c r="F124" s="104"/>
     </row>
-    <row r="125" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A125" s="155"/>
-      <c r="B125" s="100"/>
-      <c r="C125" s="101"/>
-      <c r="D125" s="101"/>
+      <c r="B125" s="218" t="s">
+        <v>229</v>
+      </c>
+      <c r="C125" s="101">
+        <v>28805</v>
+      </c>
+      <c r="D125" s="101">
+        <v>30015</v>
+      </c>
       <c r="E125" s="124">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1210</v>
       </c>
       <c r="F125" s="105"/>
     </row>
-    <row r="126" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A126" s="155"/>
-      <c r="B126" s="100"/>
-      <c r="C126" s="101"/>
-      <c r="D126" s="101"/>
+      <c r="B126" s="218" t="s">
+        <v>217</v>
+      </c>
+      <c r="C126" s="101">
+        <v>29293</v>
+      </c>
+      <c r="D126" s="101">
+        <v>30504</v>
+      </c>
       <c r="E126" s="123">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1211</v>
       </c>
       <c r="F126" s="105"/>
     </row>
-    <row r="127" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A127" s="155"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
@@ -4358,7 +4390,7 @@
       </c>
       <c r="F127" s="105"/>
     </row>
-    <row r="128" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A128" s="155"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
@@ -4369,7 +4401,7 @@
       </c>
       <c r="F128" s="105"/>
     </row>
-    <row r="129" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A129" s="155"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
@@ -4380,7 +4412,7 @@
       </c>
       <c r="F129" s="105"/>
     </row>
-    <row r="130" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A130" s="155"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
@@ -4391,7 +4423,7 @@
       </c>
       <c r="F130" s="105"/>
     </row>
-    <row r="131" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A131" s="155"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
@@ -4402,7 +4434,7 @@
       </c>
       <c r="F131" s="105"/>
     </row>
-    <row r="132" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A132" s="155"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
@@ -4413,7 +4445,7 @@
       </c>
       <c r="F132" s="105"/>
     </row>
-    <row r="133" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A133" s="155"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
@@ -4424,7 +4456,7 @@
       </c>
       <c r="F133" s="105"/>
     </row>
-    <row r="134" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A134" s="155"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
@@ -4435,7 +4467,7 @@
       </c>
       <c r="F134" s="105"/>
     </row>
-    <row r="135" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" s="155"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
@@ -4446,7 +4478,7 @@
       </c>
       <c r="F135" s="105"/>
     </row>
-    <row r="136" spans="1:7" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A136" s="155"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
@@ -4457,7 +4489,7 @@
       </c>
       <c r="F136" s="105"/>
     </row>
-    <row r="137" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="155"/>
       <c r="B137" s="98" t="s">
         <v>188</v>
@@ -4470,7 +4502,7 @@
       </c>
       <c r="F137" s="104"/>
     </row>
-    <row r="138" spans="1:7" ht="16.5" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="116">
         <v>6</v>
       </c>
@@ -4483,7 +4515,7 @@
       </c>
       <c r="D138" s="103">
         <f>D137-D124</f>
-        <v>0</v>
+        <v>-30015</v>
       </c>
       <c r="E138" s="103">
         <f>E137-E124</f>

</xml_diff>

<commit_message>
Flintstones - a bit of progress
</commit_message>
<xml_diff>
--- a/Flintstones/Compare/Flintstones.xlsx
+++ b/Flintstones/Compare/Flintstones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="252">
   <si>
     <t>Notes</t>
   </si>
@@ -812,6 +812,9 @@
   </si>
   <si>
     <t>Level end</t>
+  </si>
+  <si>
+    <t>X = 5</t>
   </si>
 </sst>
 </file>
@@ -2525,7 +2528,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B157" sqref="B157"/>
+      <selection pane="bottomLeft" activeCell="D160" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -4918,34 +4921,50 @@
     </row>
     <row r="157" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A157" s="156"/>
-      <c r="B157" s="100"/>
-      <c r="C157" s="101"/>
-      <c r="D157" s="101"/>
+      <c r="B157" s="219" t="s">
+        <v>217</v>
+      </c>
+      <c r="C157" s="101">
+        <v>36656</v>
+      </c>
+      <c r="D157" s="101">
+        <v>37917</v>
+      </c>
       <c r="E157" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1261</v>
       </c>
       <c r="F157" s="105"/>
     </row>
     <row r="158" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A158" s="156"/>
-      <c r="B158" s="100"/>
-      <c r="C158" s="101"/>
-      <c r="D158" s="101"/>
+      <c r="B158" s="219" t="s">
+        <v>251</v>
+      </c>
+      <c r="C158" s="101">
+        <v>36903</v>
+      </c>
+      <c r="D158" s="101">
+        <v>38160</v>
+      </c>
       <c r="E158" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1257</v>
       </c>
       <c r="F158" s="105"/>
     </row>
     <row r="159" spans="1:7" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A159" s="156"/>
       <c r="B159" s="100"/>
-      <c r="C159" s="101"/>
-      <c r="D159" s="101"/>
+      <c r="C159" s="101">
+        <v>36692</v>
+      </c>
+      <c r="D159" s="101">
+        <v>37950</v>
+      </c>
       <c r="E159" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1258</v>
       </c>
       <c r="F159" s="105"/>
     </row>

</xml_diff>

<commit_message>
Flintstones - a chunk of level 8 done
</commit_message>
<xml_diff>
--- a/Flintstones/Compare/Flintstones.xlsx
+++ b/Flintstones/Compare/Flintstones.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="262">
   <si>
     <t>Notes</t>
   </si>
@@ -827,6 +827,24 @@
   </si>
   <si>
     <t>X = 1</t>
+  </si>
+  <si>
+    <t>X = 163</t>
+  </si>
+  <si>
+    <t>X = 102</t>
+  </si>
+  <si>
+    <t>X = 18</t>
+  </si>
+  <si>
+    <t>X = 193</t>
+  </si>
+  <si>
+    <t>X = 24</t>
+  </si>
+  <si>
+    <t>X = 40</t>
   </si>
 </sst>
 </file>
@@ -1815,7 +1833,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2232,6 +2250,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2546,11 +2565,11 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K191"/>
+  <dimension ref="A1:K196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C179" sqref="C179"/>
+      <pane ySplit="6" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2578,7 +2597,7 @@
       <c r="F1" s="164"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
-        <f>SUM(G1:G65573)</f>
+        <f>SUM(G1:G65578)</f>
         <v>-1228</v>
       </c>
       <c r="I1" s="141" t="s">
@@ -5252,7 +5271,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="158"/>
       <c r="B177" s="98" t="s">
         <v>185</v>
@@ -5264,12 +5283,12 @@
         <v>41441</v>
       </c>
       <c r="E177" s="123">
-        <f t="shared" ref="E177:E190" si="8">IF(AND(C177&gt;0,D177&gt;0), D177-C177, 0)</f>
+        <f t="shared" ref="E177:E195" si="8">IF(AND(C177&gt;0,D177&gt;0), D177-C177, 0)</f>
         <v>1295</v>
       </c>
       <c r="F177" s="104"/>
     </row>
-    <row r="178" spans="1:7" ht="15.75" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="15.75" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A178" s="158"/>
       <c r="B178" s="221" t="s">
         <v>216</v>
@@ -5286,168 +5305,299 @@
       </c>
       <c r="F178" s="105"/>
     </row>
-    <row r="179" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A179" s="158"/>
-      <c r="B179" s="100"/>
-      <c r="C179" s="101"/>
-      <c r="D179" s="101"/>
+      <c r="B179" s="221" t="s">
+        <v>217</v>
+      </c>
+      <c r="C179" s="101">
+        <v>40161</v>
+      </c>
+      <c r="D179" s="101">
+        <v>41456</v>
+      </c>
       <c r="E179" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1295</v>
       </c>
       <c r="F179" s="105"/>
     </row>
-    <row r="180" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A180" s="158"/>
-      <c r="B180" s="100"/>
-      <c r="C180" s="101"/>
-      <c r="D180" s="101"/>
+      <c r="B180" s="221" t="s">
+        <v>256</v>
+      </c>
+      <c r="C180" s="101">
+        <v>40370</v>
+      </c>
+      <c r="D180" s="101">
+        <v>41664</v>
+      </c>
       <c r="E180" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1294</v>
       </c>
       <c r="F180" s="105"/>
     </row>
-    <row r="181" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A181" s="158"/>
-      <c r="B181" s="100"/>
-      <c r="C181" s="101"/>
-      <c r="D181" s="101"/>
+      <c r="B181" s="221" t="s">
+        <v>257</v>
+      </c>
+      <c r="C181" s="222"/>
+      <c r="D181" s="101">
+        <v>41820</v>
+      </c>
       <c r="E181" s="123">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F181" s="105"/>
     </row>
-    <row r="182" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A182" s="158"/>
-      <c r="B182" s="100"/>
-      <c r="C182" s="101"/>
-      <c r="D182" s="101"/>
+      <c r="B182" s="221" t="s">
+        <v>217</v>
+      </c>
+      <c r="C182" s="101">
+        <v>40843</v>
+      </c>
+      <c r="D182" s="101">
+        <v>42138</v>
+      </c>
       <c r="E182" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1295</v>
       </c>
       <c r="F182" s="105"/>
     </row>
-    <row r="183" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A183" s="158"/>
-      <c r="B183" s="100"/>
-      <c r="C183" s="101"/>
-      <c r="D183" s="101"/>
+      <c r="B183" s="221" t="s">
+        <v>258</v>
+      </c>
+      <c r="C183" s="101">
+        <v>40947</v>
+      </c>
+      <c r="D183" s="101">
+        <v>42241</v>
+      </c>
       <c r="E183" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1294</v>
       </c>
       <c r="F183" s="105"/>
     </row>
-    <row r="184" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A184" s="158"/>
-      <c r="B184" s="100"/>
-      <c r="C184" s="101"/>
-      <c r="D184" s="101"/>
+      <c r="B184" s="221" t="s">
+        <v>259</v>
+      </c>
+      <c r="C184" s="101">
+        <v>41666</v>
+      </c>
+      <c r="D184" s="101">
+        <v>42959</v>
+      </c>
       <c r="E184" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1293</v>
       </c>
       <c r="F184" s="105"/>
     </row>
-    <row r="185" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A185" s="158"/>
-      <c r="B185" s="100"/>
-      <c r="C185" s="101"/>
-      <c r="D185" s="101"/>
+      <c r="B185" s="221" t="s">
+        <v>249</v>
+      </c>
+      <c r="C185" s="101">
+        <v>42004</v>
+      </c>
+      <c r="D185" s="101">
+        <v>43297</v>
+      </c>
       <c r="E185" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1293</v>
       </c>
       <c r="F185" s="105"/>
     </row>
-    <row r="186" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A186" s="158"/>
-      <c r="B186" s="100"/>
-      <c r="C186" s="101"/>
-      <c r="D186" s="101"/>
+      <c r="B186" s="221" t="s">
+        <v>217</v>
+      </c>
+      <c r="C186" s="101">
+        <v>42108</v>
+      </c>
+      <c r="D186" s="101">
+        <v>43402</v>
+      </c>
       <c r="E186" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1294</v>
       </c>
       <c r="F186" s="105"/>
     </row>
-    <row r="187" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A187" s="158"/>
-      <c r="B187" s="100"/>
-      <c r="C187" s="101"/>
-      <c r="D187" s="101"/>
+      <c r="B187" s="221" t="s">
+        <v>260</v>
+      </c>
+      <c r="C187" s="101">
+        <v>42204</v>
+      </c>
+      <c r="D187" s="101">
+        <v>43497</v>
+      </c>
       <c r="E187" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1293</v>
       </c>
       <c r="F187" s="105"/>
     </row>
-    <row r="188" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A188" s="158"/>
-      <c r="B188" s="100"/>
-      <c r="C188" s="101"/>
-      <c r="D188" s="101"/>
+      <c r="B188" s="221" t="s">
+        <v>217</v>
+      </c>
+      <c r="C188" s="101">
+        <v>42452</v>
+      </c>
+      <c r="D188" s="101">
+        <v>43746</v>
+      </c>
       <c r="E188" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1294</v>
       </c>
       <c r="F188" s="105"/>
     </row>
-    <row r="189" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A189" s="158"/>
-      <c r="B189" s="100"/>
-      <c r="C189" s="101"/>
-      <c r="D189" s="101"/>
+      <c r="B189" s="221" t="s">
+        <v>221</v>
+      </c>
+      <c r="C189" s="101">
+        <v>42545</v>
+      </c>
+      <c r="D189" s="101">
+        <v>43838</v>
+      </c>
       <c r="E189" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1293</v>
       </c>
       <c r="F189" s="105"/>
     </row>
-    <row r="190" spans="1:7" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A190" s="158"/>
-      <c r="B190" s="98" t="s">
-        <v>188</v>
-      </c>
-      <c r="C190" s="99"/>
-      <c r="D190" s="99"/>
-      <c r="E190" s="125">
+      <c r="B190" s="221" t="s">
+        <v>227</v>
+      </c>
+      <c r="C190" s="101">
+        <v>42984</v>
+      </c>
+      <c r="D190" s="101">
+        <v>44278</v>
+      </c>
+      <c r="E190" s="123">
+        <f t="shared" si="8"/>
+        <v>1294</v>
+      </c>
+      <c r="F190" s="105"/>
+    </row>
+    <row r="191" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A191" s="158"/>
+      <c r="B191" s="221" t="s">
+        <v>261</v>
+      </c>
+      <c r="C191" s="101">
+        <v>43604</v>
+      </c>
+      <c r="D191" s="101">
+        <v>44897</v>
+      </c>
+      <c r="E191" s="123">
+        <f t="shared" si="8"/>
+        <v>1293</v>
+      </c>
+      <c r="F191" s="105"/>
+    </row>
+    <row r="192" spans="1:6" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A192" s="158"/>
+      <c r="B192" s="221"/>
+      <c r="C192" s="101"/>
+      <c r="D192" s="101"/>
+      <c r="E192" s="123">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F190" s="104"/>
-    </row>
-    <row r="191" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="116">
+      <c r="F192" s="105"/>
+    </row>
+    <row r="193" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A193" s="158"/>
+      <c r="B193" s="100"/>
+      <c r="C193" s="101"/>
+      <c r="D193" s="101"/>
+      <c r="E193" s="123">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F193" s="105"/>
+    </row>
+    <row r="194" spans="1:7" ht="15" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A194" s="158"/>
+      <c r="B194" s="100"/>
+      <c r="C194" s="101"/>
+      <c r="D194" s="101"/>
+      <c r="E194" s="123">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F194" s="105"/>
+    </row>
+    <row r="195" spans="1:7" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="158"/>
+      <c r="B195" s="98" t="s">
+        <v>188</v>
+      </c>
+      <c r="C195" s="99"/>
+      <c r="D195" s="99"/>
+      <c r="E195" s="125">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F195" s="104"/>
+    </row>
+    <row r="196" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="116">
         <v>8</v>
       </c>
-      <c r="B191" s="102" t="s">
+      <c r="B196" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="C191" s="103">
-        <f>C190-C177</f>
+      <c r="C196" s="103">
+        <f>C195-C177</f>
         <v>-40146</v>
       </c>
-      <c r="D191" s="103">
-        <f>D190-D177</f>
+      <c r="D196" s="103">
+        <f>D195-D177</f>
         <v>-41441</v>
       </c>
-      <c r="E191" s="103">
-        <f>E190-E177</f>
+      <c r="E196" s="103">
+        <f>E195-E177</f>
         <v>-1295</v>
       </c>
-      <c r="F191" s="107"/>
-      <c r="G191" s="112">
-        <f>E191</f>
+      <c r="F196" s="107"/>
+      <c r="G196" s="112">
+        <f>E196</f>
         <v>-1295</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A176:A190"/>
+    <mergeCell ref="A176:A195"/>
     <mergeCell ref="A123:A151"/>
     <mergeCell ref="A76:A103"/>
     <mergeCell ref="A154:A173"/>

</xml_diff>